<commit_message>
adjustments to pulse ox
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-VA.MHV.bloodOxygenSat.xlsx
+++ b/docs/StructureDefinition-VA.MHV.bloodOxygenSat.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3132" uniqueCount="573">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3132" uniqueCount="572">
   <si>
     <t>Path</t>
   </si>
@@ -625,9 +625,6 @@
   </si>
   <si>
     <t>Need to track the status of individual results. Some results are finalized before the whole report is finalized.</t>
-  </si>
-  <si>
-    <t>final</t>
   </si>
   <si>
     <t>required</t>
@@ -4517,26 +4514,26 @@
         <v>45</v>
       </c>
       <c r="R22" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="S22" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="T22" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="U22" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="V22" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="W22" t="s" s="2">
         <v>194</v>
-      </c>
-      <c r="S22" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="T22" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="U22" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="V22" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="W22" t="s" s="2">
-        <v>195</v>
       </c>
       <c r="X22" s="2"/>
       <c r="Y22" t="s" s="2">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="Z22" t="s" s="2">
         <v>45</v>
@@ -4569,19 +4566,19 @@
         <v>67</v>
       </c>
       <c r="AJ22" t="s" s="2">
+        <v>196</v>
+      </c>
+      <c r="AK22" t="s" s="2">
         <v>197</v>
       </c>
-      <c r="AK22" t="s" s="2">
+      <c r="AL22" t="s" s="2">
         <v>198</v>
       </c>
-      <c r="AL22" t="s" s="2">
+      <c r="AM22" t="s" s="2">
         <v>199</v>
       </c>
-      <c r="AM22" t="s" s="2">
+      <c r="AN22" t="s" s="2">
         <v>200</v>
-      </c>
-      <c r="AN22" t="s" s="2">
-        <v>201</v>
       </c>
       <c r="AO22" t="s" s="2">
         <v>45</v>
@@ -4589,7 +4586,7 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
@@ -4612,19 +4609,19 @@
         <v>45</v>
       </c>
       <c r="J23" t="s" s="2">
+        <v>202</v>
+      </c>
+      <c r="K23" t="s" s="2">
         <v>203</v>
       </c>
-      <c r="K23" t="s" s="2">
+      <c r="L23" t="s" s="2">
         <v>204</v>
       </c>
-      <c r="L23" t="s" s="2">
+      <c r="M23" t="s" s="2">
         <v>205</v>
       </c>
-      <c r="M23" t="s" s="2">
+      <c r="N23" t="s" s="2">
         <v>206</v>
-      </c>
-      <c r="N23" t="s" s="2">
-        <v>207</v>
       </c>
       <c r="O23" t="s" s="2">
         <v>45</v>
@@ -4634,7 +4631,7 @@
         <v>45</v>
       </c>
       <c r="R23" t="s" s="2">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="S23" t="s" s="2">
         <v>45</v>
@@ -4652,16 +4649,16 @@
         <v>136</v>
       </c>
       <c r="X23" t="s" s="2">
+        <v>208</v>
+      </c>
+      <c r="Y23" t="s" s="2">
         <v>209</v>
       </c>
-      <c r="Y23" t="s" s="2">
+      <c r="Z23" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA23" t="s" s="2">
         <v>210</v>
-      </c>
-      <c r="Z23" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AA23" t="s" s="2">
-        <v>211</v>
       </c>
       <c r="AB23" s="2"/>
       <c r="AC23" t="s" s="2">
@@ -4671,7 +4668,7 @@
         <v>81</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>43</v>
@@ -4695,10 +4692,10 @@
         <v>45</v>
       </c>
       <c r="AM23" t="s" s="2">
+        <v>211</v>
+      </c>
+      <c r="AN23" t="s" s="2">
         <v>212</v>
-      </c>
-      <c r="AN23" t="s" s="2">
-        <v>213</v>
       </c>
       <c r="AO23" t="s" s="2">
         <v>45</v>
@@ -4706,10 +4703,10 @@
     </row>
     <row r="24">
       <c r="A24" t="s" s="2">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B24" t="s" s="2">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C24" t="s" s="2">
         <v>45</v>
@@ -4731,19 +4728,19 @@
         <v>45</v>
       </c>
       <c r="J24" t="s" s="2">
+        <v>202</v>
+      </c>
+      <c r="K24" t="s" s="2">
         <v>203</v>
       </c>
-      <c r="K24" t="s" s="2">
+      <c r="L24" t="s" s="2">
         <v>204</v>
       </c>
-      <c r="L24" t="s" s="2">
+      <c r="M24" t="s" s="2">
         <v>205</v>
       </c>
-      <c r="M24" t="s" s="2">
+      <c r="N24" t="s" s="2">
         <v>206</v>
-      </c>
-      <c r="N24" t="s" s="2">
-        <v>207</v>
       </c>
       <c r="O24" t="s" s="2">
         <v>45</v>
@@ -4771,11 +4768,11 @@
         <v>136</v>
       </c>
       <c r="X24" t="s" s="2">
+        <v>208</v>
+      </c>
+      <c r="Y24" t="s" s="2">
         <v>209</v>
       </c>
-      <c r="Y24" t="s" s="2">
-        <v>210</v>
-      </c>
       <c r="Z24" t="s" s="2">
         <v>45</v>
       </c>
@@ -4792,7 +4789,7 @@
         <v>45</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>43</v>
@@ -4816,10 +4813,10 @@
         <v>45</v>
       </c>
       <c r="AM24" t="s" s="2">
+        <v>211</v>
+      </c>
+      <c r="AN24" t="s" s="2">
         <v>212</v>
-      </c>
-      <c r="AN24" t="s" s="2">
-        <v>213</v>
       </c>
       <c r="AO24" t="s" s="2">
         <v>45</v>
@@ -4827,7 +4824,7 @@
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
@@ -4942,7 +4939,7 @@
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
@@ -5059,7 +5056,7 @@
     </row>
     <row r="27">
       <c r="A27" t="s" s="2">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -5085,16 +5082,16 @@
         <v>109</v>
       </c>
       <c r="K27" t="s" s="2">
+        <v>217</v>
+      </c>
+      <c r="L27" t="s" s="2">
         <v>218</v>
       </c>
-      <c r="L27" t="s" s="2">
+      <c r="M27" t="s" s="2">
         <v>219</v>
       </c>
-      <c r="M27" t="s" s="2">
+      <c r="N27" t="s" s="2">
         <v>220</v>
-      </c>
-      <c r="N27" t="s" s="2">
-        <v>221</v>
       </c>
       <c r="O27" t="s" s="2">
         <v>45</v>
@@ -5143,7 +5140,7 @@
         <v>45</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>43</v>
@@ -5164,10 +5161,10 @@
         <v>45</v>
       </c>
       <c r="AL27" t="s" s="2">
+        <v>222</v>
+      </c>
+      <c r="AM27" t="s" s="2">
         <v>223</v>
-      </c>
-      <c r="AM27" t="s" s="2">
-        <v>224</v>
       </c>
       <c r="AN27" t="s" s="2">
         <v>45</v>
@@ -5178,7 +5175,7 @@
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -5293,7 +5290,7 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -5410,7 +5407,7 @@
     </row>
     <row r="30">
       <c r="A30" t="s" s="2">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -5436,65 +5433,65 @@
         <v>97</v>
       </c>
       <c r="K30" t="s" s="2">
+        <v>227</v>
+      </c>
+      <c r="L30" t="s" s="2">
         <v>228</v>
       </c>
-      <c r="L30" t="s" s="2">
+      <c r="M30" t="s" s="2">
         <v>229</v>
       </c>
-      <c r="M30" t="s" s="2">
+      <c r="N30" t="s" s="2">
         <v>230</v>
-      </c>
-      <c r="N30" t="s" s="2">
-        <v>231</v>
       </c>
       <c r="O30" t="s" s="2">
         <v>45</v>
       </c>
       <c r="P30" s="2"/>
       <c r="Q30" t="s" s="2">
+        <v>231</v>
+      </c>
+      <c r="R30" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="S30" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="T30" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="U30" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="V30" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="W30" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="X30" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Y30" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Z30" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA30" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB30" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC30" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD30" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE30" t="s" s="2">
         <v>232</v>
-      </c>
-      <c r="R30" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="S30" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="T30" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="U30" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="V30" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="W30" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="X30" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="Y30" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="Z30" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AA30" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AB30" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AC30" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AD30" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AE30" t="s" s="2">
-        <v>233</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>43</v>
@@ -5515,10 +5512,10 @@
         <v>45</v>
       </c>
       <c r="AL30" t="s" s="2">
+        <v>233</v>
+      </c>
+      <c r="AM30" t="s" s="2">
         <v>234</v>
-      </c>
-      <c r="AM30" t="s" s="2">
-        <v>235</v>
       </c>
       <c r="AN30" t="s" s="2">
         <v>45</v>
@@ -5529,7 +5526,7 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -5555,13 +5552,13 @@
         <v>57</v>
       </c>
       <c r="K31" t="s" s="2">
+        <v>236</v>
+      </c>
+      <c r="L31" t="s" s="2">
         <v>237</v>
       </c>
-      <c r="L31" t="s" s="2">
+      <c r="M31" t="s" s="2">
         <v>238</v>
-      </c>
-      <c r="M31" t="s" s="2">
-        <v>239</v>
       </c>
       <c r="N31" s="2"/>
       <c r="O31" t="s" s="2">
@@ -5611,7 +5608,7 @@
         <v>45</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>43</v>
@@ -5632,10 +5629,10 @@
         <v>45</v>
       </c>
       <c r="AL31" t="s" s="2">
+        <v>240</v>
+      </c>
+      <c r="AM31" t="s" s="2">
         <v>241</v>
-      </c>
-      <c r="AM31" t="s" s="2">
-        <v>242</v>
       </c>
       <c r="AN31" t="s" s="2">
         <v>45</v>
@@ -5646,7 +5643,7 @@
     </row>
     <row r="32">
       <c r="A32" t="s" s="2">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -5672,63 +5669,63 @@
         <v>132</v>
       </c>
       <c r="K32" t="s" s="2">
+        <v>243</v>
+      </c>
+      <c r="L32" t="s" s="2">
         <v>244</v>
-      </c>
-      <c r="L32" t="s" s="2">
-        <v>245</v>
       </c>
       <c r="M32" s="2"/>
       <c r="N32" t="s" s="2">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="O32" t="s" s="2">
         <v>45</v>
       </c>
       <c r="P32" s="2"/>
       <c r="Q32" t="s" s="2">
+        <v>246</v>
+      </c>
+      <c r="R32" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="S32" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="T32" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="U32" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="V32" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="W32" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="X32" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Y32" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Z32" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA32" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB32" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC32" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD32" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE32" t="s" s="2">
         <v>247</v>
-      </c>
-      <c r="R32" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="S32" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="T32" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="U32" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="V32" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="W32" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="X32" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="Y32" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="Z32" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AA32" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AB32" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AC32" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AD32" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AE32" t="s" s="2">
-        <v>248</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>43</v>
@@ -5749,10 +5746,10 @@
         <v>45</v>
       </c>
       <c r="AL32" t="s" s="2">
+        <v>248</v>
+      </c>
+      <c r="AM32" t="s" s="2">
         <v>249</v>
-      </c>
-      <c r="AM32" t="s" s="2">
-        <v>250</v>
       </c>
       <c r="AN32" t="s" s="2">
         <v>45</v>
@@ -5763,7 +5760,7 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -5789,14 +5786,14 @@
         <v>57</v>
       </c>
       <c r="K33" t="s" s="2">
+        <v>251</v>
+      </c>
+      <c r="L33" t="s" s="2">
         <v>252</v>
-      </c>
-      <c r="L33" t="s" s="2">
-        <v>253</v>
       </c>
       <c r="M33" s="2"/>
       <c r="N33" t="s" s="2">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="O33" t="s" s="2">
         <v>45</v>
@@ -5845,7 +5842,7 @@
         <v>45</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>43</v>
@@ -5866,10 +5863,10 @@
         <v>45</v>
       </c>
       <c r="AL33" t="s" s="2">
+        <v>255</v>
+      </c>
+      <c r="AM33" t="s" s="2">
         <v>256</v>
-      </c>
-      <c r="AM33" t="s" s="2">
-        <v>257</v>
       </c>
       <c r="AN33" t="s" s="2">
         <v>45</v>
@@ -5880,7 +5877,7 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
@@ -5903,19 +5900,19 @@
         <v>56</v>
       </c>
       <c r="J34" t="s" s="2">
+        <v>258</v>
+      </c>
+      <c r="K34" t="s" s="2">
         <v>259</v>
       </c>
-      <c r="K34" t="s" s="2">
+      <c r="L34" t="s" s="2">
         <v>260</v>
       </c>
-      <c r="L34" t="s" s="2">
+      <c r="M34" t="s" s="2">
         <v>261</v>
       </c>
-      <c r="M34" t="s" s="2">
+      <c r="N34" t="s" s="2">
         <v>262</v>
-      </c>
-      <c r="N34" t="s" s="2">
-        <v>263</v>
       </c>
       <c r="O34" t="s" s="2">
         <v>45</v>
@@ -5964,7 +5961,7 @@
         <v>45</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>43</v>
@@ -5985,10 +5982,10 @@
         <v>45</v>
       </c>
       <c r="AL34" t="s" s="2">
+        <v>264</v>
+      </c>
+      <c r="AM34" t="s" s="2">
         <v>265</v>
-      </c>
-      <c r="AM34" t="s" s="2">
-        <v>266</v>
       </c>
       <c r="AN34" t="s" s="2">
         <v>45</v>
@@ -5999,7 +5996,7 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -6025,16 +6022,16 @@
         <v>57</v>
       </c>
       <c r="K35" t="s" s="2">
+        <v>267</v>
+      </c>
+      <c r="L35" t="s" s="2">
         <v>268</v>
       </c>
-      <c r="L35" t="s" s="2">
+      <c r="M35" t="s" s="2">
         <v>269</v>
       </c>
-      <c r="M35" t="s" s="2">
+      <c r="N35" t="s" s="2">
         <v>270</v>
-      </c>
-      <c r="N35" t="s" s="2">
-        <v>271</v>
       </c>
       <c r="O35" t="s" s="2">
         <v>45</v>
@@ -6083,7 +6080,7 @@
         <v>45</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>43</v>
@@ -6104,10 +6101,10 @@
         <v>45</v>
       </c>
       <c r="AL35" t="s" s="2">
+        <v>272</v>
+      </c>
+      <c r="AM35" t="s" s="2">
         <v>273</v>
-      </c>
-      <c r="AM35" t="s" s="2">
-        <v>274</v>
       </c>
       <c r="AN35" t="s" s="2">
         <v>45</v>
@@ -6118,11 +6115,11 @@
     </row>
     <row r="36">
       <c r="A36" t="s" s="2">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" t="s" s="2">
@@ -6141,19 +6138,19 @@
         <v>56</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="K36" t="s" s="2">
+        <v>276</v>
+      </c>
+      <c r="L36" t="s" s="2">
         <v>277</v>
       </c>
-      <c r="L36" t="s" s="2">
+      <c r="M36" t="s" s="2">
         <v>278</v>
       </c>
-      <c r="M36" t="s" s="2">
+      <c r="N36" t="s" s="2">
         <v>279</v>
-      </c>
-      <c r="N36" t="s" s="2">
-        <v>280</v>
       </c>
       <c r="O36" t="s" s="2">
         <v>45</v>
@@ -6181,11 +6178,11 @@
         <v>113</v>
       </c>
       <c r="X36" t="s" s="2">
+        <v>280</v>
+      </c>
+      <c r="Y36" t="s" s="2">
         <v>281</v>
       </c>
-      <c r="Y36" t="s" s="2">
-        <v>282</v>
-      </c>
       <c r="Z36" t="s" s="2">
         <v>45</v>
       </c>
@@ -6202,7 +6199,7 @@
         <v>45</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>55</v>
@@ -6217,27 +6214,27 @@
         <v>67</v>
       </c>
       <c r="AJ36" t="s" s="2">
+        <v>282</v>
+      </c>
+      <c r="AK36" t="s" s="2">
         <v>283</v>
       </c>
-      <c r="AK36" t="s" s="2">
+      <c r="AL36" t="s" s="2">
         <v>284</v>
       </c>
-      <c r="AL36" t="s" s="2">
+      <c r="AM36" t="s" s="2">
         <v>285</v>
       </c>
-      <c r="AM36" t="s" s="2">
+      <c r="AN36" t="s" s="2">
         <v>286</v>
       </c>
-      <c r="AN36" t="s" s="2">
+      <c r="AO36" t="s" s="2">
         <v>287</v>
-      </c>
-      <c r="AO36" t="s" s="2">
-        <v>288</v>
       </c>
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -6352,7 +6349,7 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -6469,7 +6466,7 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -6495,16 +6492,16 @@
         <v>109</v>
       </c>
       <c r="K39" t="s" s="2">
+        <v>217</v>
+      </c>
+      <c r="L39" t="s" s="2">
         <v>218</v>
       </c>
-      <c r="L39" t="s" s="2">
+      <c r="M39" t="s" s="2">
         <v>219</v>
       </c>
-      <c r="M39" t="s" s="2">
+      <c r="N39" t="s" s="2">
         <v>220</v>
-      </c>
-      <c r="N39" t="s" s="2">
-        <v>221</v>
       </c>
       <c r="O39" t="s" s="2">
         <v>45</v>
@@ -6553,7 +6550,7 @@
         <v>45</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>43</v>
@@ -6574,10 +6571,10 @@
         <v>45</v>
       </c>
       <c r="AL39" t="s" s="2">
+        <v>222</v>
+      </c>
+      <c r="AM39" t="s" s="2">
         <v>223</v>
-      </c>
-      <c r="AM39" t="s" s="2">
-        <v>224</v>
       </c>
       <c r="AN39" t="s" s="2">
         <v>45</v>
@@ -6588,7 +6585,7 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -6614,16 +6611,16 @@
         <v>57</v>
       </c>
       <c r="K40" t="s" s="2">
+        <v>267</v>
+      </c>
+      <c r="L40" t="s" s="2">
         <v>268</v>
       </c>
-      <c r="L40" t="s" s="2">
+      <c r="M40" t="s" s="2">
         <v>269</v>
       </c>
-      <c r="M40" t="s" s="2">
+      <c r="N40" t="s" s="2">
         <v>270</v>
-      </c>
-      <c r="N40" t="s" s="2">
-        <v>271</v>
       </c>
       <c r="O40" t="s" s="2">
         <v>45</v>
@@ -6672,7 +6669,7 @@
         <v>45</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>43</v>
@@ -6693,10 +6690,10 @@
         <v>45</v>
       </c>
       <c r="AL40" t="s" s="2">
+        <v>272</v>
+      </c>
+      <c r="AM40" t="s" s="2">
         <v>273</v>
-      </c>
-      <c r="AM40" t="s" s="2">
-        <v>274</v>
       </c>
       <c r="AN40" t="s" s="2">
         <v>45</v>
@@ -6707,7 +6704,7 @@
     </row>
     <row r="41">
       <c r="A41" t="s" s="2">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -6730,19 +6727,19 @@
         <v>56</v>
       </c>
       <c r="J41" t="s" s="2">
+        <v>293</v>
+      </c>
+      <c r="K41" t="s" s="2">
         <v>294</v>
       </c>
-      <c r="K41" t="s" s="2">
+      <c r="L41" t="s" s="2">
         <v>295</v>
       </c>
-      <c r="L41" t="s" s="2">
+      <c r="M41" t="s" s="2">
         <v>296</v>
       </c>
-      <c r="M41" t="s" s="2">
+      <c r="N41" t="s" s="2">
         <v>297</v>
-      </c>
-      <c r="N41" t="s" s="2">
-        <v>298</v>
       </c>
       <c r="O41" t="s" s="2">
         <v>45</v>
@@ -6791,7 +6788,7 @@
         <v>45</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>43</v>
@@ -6806,19 +6803,19 @@
         <v>67</v>
       </c>
       <c r="AJ41" t="s" s="2">
+        <v>298</v>
+      </c>
+      <c r="AK41" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL41" t="s" s="2">
         <v>299</v>
       </c>
-      <c r="AK41" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL41" t="s" s="2">
+      <c r="AM41" t="s" s="2">
         <v>300</v>
       </c>
-      <c r="AM41" t="s" s="2">
+      <c r="AN41" t="s" s="2">
         <v>301</v>
-      </c>
-      <c r="AN41" t="s" s="2">
-        <v>302</v>
       </c>
       <c r="AO41" t="s" s="2">
         <v>45</v>
@@ -6826,7 +6823,7 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -6849,16 +6846,16 @@
         <v>56</v>
       </c>
       <c r="J42" t="s" s="2">
+        <v>303</v>
+      </c>
+      <c r="K42" t="s" s="2">
         <v>304</v>
       </c>
-      <c r="K42" t="s" s="2">
+      <c r="L42" t="s" s="2">
         <v>305</v>
       </c>
-      <c r="L42" t="s" s="2">
+      <c r="M42" t="s" s="2">
         <v>306</v>
-      </c>
-      <c r="M42" t="s" s="2">
-        <v>307</v>
       </c>
       <c r="N42" s="2"/>
       <c r="O42" t="s" s="2">
@@ -6908,7 +6905,7 @@
         <v>45</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>43</v>
@@ -6929,13 +6926,13 @@
         <v>45</v>
       </c>
       <c r="AL42" t="s" s="2">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AN42" t="s" s="2">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="AO42" t="s" s="2">
         <v>45</v>
@@ -6943,11 +6940,11 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" t="s" s="2">
@@ -6966,19 +6963,19 @@
         <v>56</v>
       </c>
       <c r="J43" t="s" s="2">
+        <v>310</v>
+      </c>
+      <c r="K43" t="s" s="2">
         <v>311</v>
       </c>
-      <c r="K43" t="s" s="2">
+      <c r="L43" t="s" s="2">
         <v>312</v>
       </c>
-      <c r="L43" t="s" s="2">
+      <c r="M43" t="s" s="2">
         <v>313</v>
       </c>
-      <c r="M43" t="s" s="2">
+      <c r="N43" t="s" s="2">
         <v>314</v>
-      </c>
-      <c r="N43" t="s" s="2">
-        <v>315</v>
       </c>
       <c r="O43" t="s" s="2">
         <v>45</v>
@@ -7027,7 +7024,7 @@
         <v>45</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>43</v>
@@ -7042,19 +7039,19 @@
         <v>67</v>
       </c>
       <c r="AJ43" t="s" s="2">
+        <v>315</v>
+      </c>
+      <c r="AK43" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL43" t="s" s="2">
         <v>316</v>
       </c>
-      <c r="AK43" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL43" t="s" s="2">
+      <c r="AM43" t="s" s="2">
         <v>317</v>
       </c>
-      <c r="AM43" t="s" s="2">
+      <c r="AN43" t="s" s="2">
         <v>318</v>
-      </c>
-      <c r="AN43" t="s" s="2">
-        <v>319</v>
       </c>
       <c r="AO43" t="s" s="2">
         <v>45</v>
@@ -7062,11 +7059,11 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" t="s" s="2">
@@ -7085,19 +7082,19 @@
         <v>56</v>
       </c>
       <c r="J44" t="s" s="2">
+        <v>321</v>
+      </c>
+      <c r="K44" t="s" s="2">
         <v>322</v>
       </c>
-      <c r="K44" t="s" s="2">
+      <c r="L44" t="s" s="2">
         <v>323</v>
       </c>
-      <c r="L44" t="s" s="2">
+      <c r="M44" t="s" s="2">
         <v>324</v>
       </c>
-      <c r="M44" t="s" s="2">
+      <c r="N44" t="s" s="2">
         <v>325</v>
-      </c>
-      <c r="N44" t="s" s="2">
-        <v>326</v>
       </c>
       <c r="O44" t="s" s="2">
         <v>45</v>
@@ -7134,17 +7131,17 @@
         <v>45</v>
       </c>
       <c r="AA44" t="s" s="2">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="AB44" s="2"/>
       <c r="AC44" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AD44" t="s" s="2">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>43</v>
@@ -7153,25 +7150,25 @@
         <v>55</v>
       </c>
       <c r="AH44" t="s" s="2">
+        <v>328</v>
+      </c>
+      <c r="AI44" t="s" s="2">
         <v>329</v>
       </c>
-      <c r="AI44" t="s" s="2">
+      <c r="AJ44" t="s" s="2">
         <v>330</v>
       </c>
-      <c r="AJ44" t="s" s="2">
+      <c r="AK44" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL44" t="s" s="2">
         <v>331</v>
       </c>
-      <c r="AK44" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL44" t="s" s="2">
+      <c r="AM44" t="s" s="2">
         <v>332</v>
       </c>
-      <c r="AM44" t="s" s="2">
+      <c r="AN44" t="s" s="2">
         <v>333</v>
-      </c>
-      <c r="AN44" t="s" s="2">
-        <v>334</v>
       </c>
       <c r="AO44" t="s" s="2">
         <v>45</v>
@@ -7179,13 +7176,13 @@
     </row>
     <row r="45">
       <c r="A45" t="s" s="2">
+        <v>319</v>
+      </c>
+      <c r="B45" t="s" s="2">
+        <v>334</v>
+      </c>
+      <c r="C45" t="s" s="2">
         <v>320</v>
-      </c>
-      <c r="B45" t="s" s="2">
-        <v>335</v>
-      </c>
-      <c r="C45" t="s" s="2">
-        <v>321</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" t="s" s="2">
@@ -7204,19 +7201,19 @@
         <v>56</v>
       </c>
       <c r="J45" t="s" s="2">
+        <v>321</v>
+      </c>
+      <c r="K45" t="s" s="2">
         <v>322</v>
       </c>
-      <c r="K45" t="s" s="2">
+      <c r="L45" t="s" s="2">
         <v>323</v>
       </c>
-      <c r="L45" t="s" s="2">
+      <c r="M45" t="s" s="2">
         <v>324</v>
       </c>
-      <c r="M45" t="s" s="2">
+      <c r="N45" t="s" s="2">
         <v>325</v>
-      </c>
-      <c r="N45" t="s" s="2">
-        <v>326</v>
       </c>
       <c r="O45" t="s" s="2">
         <v>45</v>
@@ -7265,7 +7262,7 @@
         <v>45</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>43</v>
@@ -7274,25 +7271,25 @@
         <v>55</v>
       </c>
       <c r="AH45" t="s" s="2">
+        <v>328</v>
+      </c>
+      <c r="AI45" t="s" s="2">
         <v>329</v>
       </c>
-      <c r="AI45" t="s" s="2">
+      <c r="AJ45" t="s" s="2">
         <v>330</v>
       </c>
-      <c r="AJ45" t="s" s="2">
+      <c r="AK45" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL45" t="s" s="2">
         <v>331</v>
       </c>
-      <c r="AK45" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL45" t="s" s="2">
+      <c r="AM45" t="s" s="2">
         <v>332</v>
       </c>
-      <c r="AM45" t="s" s="2">
+      <c r="AN45" t="s" s="2">
         <v>333</v>
-      </c>
-      <c r="AN45" t="s" s="2">
-        <v>334</v>
       </c>
       <c r="AO45" t="s" s="2">
         <v>45</v>
@@ -7300,7 +7297,7 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -7326,13 +7323,13 @@
         <v>91</v>
       </c>
       <c r="K46" t="s" s="2">
+        <v>336</v>
+      </c>
+      <c r="L46" t="s" s="2">
         <v>337</v>
       </c>
-      <c r="L46" t="s" s="2">
+      <c r="M46" t="s" s="2">
         <v>338</v>
-      </c>
-      <c r="M46" t="s" s="2">
-        <v>339</v>
       </c>
       <c r="N46" s="2"/>
       <c r="O46" t="s" s="2">
@@ -7382,7 +7379,7 @@
         <v>45</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>43</v>
@@ -7403,13 +7400,13 @@
         <v>45</v>
       </c>
       <c r="AL46" t="s" s="2">
+        <v>339</v>
+      </c>
+      <c r="AM46" t="s" s="2">
         <v>340</v>
       </c>
-      <c r="AM46" t="s" s="2">
+      <c r="AN46" t="s" s="2">
         <v>341</v>
-      </c>
-      <c r="AN46" t="s" s="2">
-        <v>342</v>
       </c>
       <c r="AO46" t="s" s="2">
         <v>45</v>
@@ -7417,7 +7414,7 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -7440,17 +7437,17 @@
         <v>56</v>
       </c>
       <c r="J47" t="s" s="2">
+        <v>343</v>
+      </c>
+      <c r="K47" t="s" s="2">
         <v>344</v>
       </c>
-      <c r="K47" t="s" s="2">
+      <c r="L47" t="s" s="2">
         <v>345</v>
-      </c>
-      <c r="L47" t="s" s="2">
-        <v>346</v>
       </c>
       <c r="M47" s="2"/>
       <c r="N47" t="s" s="2">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="O47" t="s" s="2">
         <v>45</v>
@@ -7499,7 +7496,7 @@
         <v>45</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>43</v>
@@ -7514,19 +7511,19 @@
         <v>67</v>
       </c>
       <c r="AJ47" t="s" s="2">
+        <v>347</v>
+      </c>
+      <c r="AK47" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL47" t="s" s="2">
         <v>348</v>
       </c>
-      <c r="AK47" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL47" t="s" s="2">
+      <c r="AM47" t="s" s="2">
         <v>349</v>
       </c>
-      <c r="AM47" t="s" s="2">
+      <c r="AN47" t="s" s="2">
         <v>350</v>
-      </c>
-      <c r="AN47" t="s" s="2">
-        <v>351</v>
       </c>
       <c r="AO47" t="s" s="2">
         <v>45</v>
@@ -7534,7 +7531,7 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
@@ -7557,19 +7554,19 @@
         <v>56</v>
       </c>
       <c r="J48" t="s" s="2">
+        <v>352</v>
+      </c>
+      <c r="K48" t="s" s="2">
         <v>353</v>
       </c>
-      <c r="K48" t="s" s="2">
+      <c r="L48" t="s" s="2">
+        <v>353</v>
+      </c>
+      <c r="M48" t="s" s="2">
         <v>354</v>
       </c>
-      <c r="L48" t="s" s="2">
-        <v>354</v>
-      </c>
-      <c r="M48" t="s" s="2">
+      <c r="N48" t="s" s="2">
         <v>355</v>
-      </c>
-      <c r="N48" t="s" s="2">
-        <v>356</v>
       </c>
       <c r="O48" t="s" s="2">
         <v>45</v>
@@ -7606,17 +7603,17 @@
         <v>45</v>
       </c>
       <c r="AA48" t="s" s="2">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="AB48" s="2"/>
       <c r="AC48" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AD48" t="s" s="2">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>43</v>
@@ -7625,7 +7622,7 @@
         <v>55</v>
       </c>
       <c r="AH48" t="s" s="2">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="AI48" t="s" s="2">
         <v>67</v>
@@ -7634,27 +7631,27 @@
         <v>45</v>
       </c>
       <c r="AK48" t="s" s="2">
+        <v>357</v>
+      </c>
+      <c r="AL48" t="s" s="2">
         <v>358</v>
       </c>
-      <c r="AL48" t="s" s="2">
+      <c r="AM48" t="s" s="2">
         <v>359</v>
       </c>
-      <c r="AM48" t="s" s="2">
+      <c r="AN48" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO48" t="s" s="2">
         <v>360</v>
-      </c>
-      <c r="AN48" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO48" t="s" s="2">
-        <v>361</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="2">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B49" t="s" s="2">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C49" t="s" s="2">
         <v>45</v>
@@ -7676,19 +7673,19 @@
         <v>56</v>
       </c>
       <c r="J49" t="s" s="2">
+        <v>352</v>
+      </c>
+      <c r="K49" t="s" s="2">
         <v>353</v>
       </c>
-      <c r="K49" t="s" s="2">
+      <c r="L49" t="s" s="2">
+        <v>353</v>
+      </c>
+      <c r="M49" t="s" s="2">
         <v>354</v>
       </c>
-      <c r="L49" t="s" s="2">
-        <v>354</v>
-      </c>
-      <c r="M49" t="s" s="2">
+      <c r="N49" t="s" s="2">
         <v>355</v>
-      </c>
-      <c r="N49" t="s" s="2">
-        <v>356</v>
       </c>
       <c r="O49" t="s" s="2">
         <v>45</v>
@@ -7737,7 +7734,7 @@
         <v>45</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>43</v>
@@ -7746,7 +7743,7 @@
         <v>55</v>
       </c>
       <c r="AH49" t="s" s="2">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="AI49" t="s" s="2">
         <v>67</v>
@@ -7755,24 +7752,24 @@
         <v>45</v>
       </c>
       <c r="AK49" t="s" s="2">
+        <v>357</v>
+      </c>
+      <c r="AL49" t="s" s="2">
         <v>358</v>
       </c>
-      <c r="AL49" t="s" s="2">
+      <c r="AM49" t="s" s="2">
         <v>359</v>
       </c>
-      <c r="AM49" t="s" s="2">
+      <c r="AN49" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO49" t="s" s="2">
         <v>360</v>
-      </c>
-      <c r="AN49" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO49" t="s" s="2">
-        <v>361</v>
       </c>
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
@@ -7887,7 +7884,7 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -8004,7 +8001,7 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
@@ -8027,19 +8024,19 @@
         <v>56</v>
       </c>
       <c r="J52" t="s" s="2">
+        <v>365</v>
+      </c>
+      <c r="K52" t="s" s="2">
         <v>366</v>
       </c>
-      <c r="K52" t="s" s="2">
+      <c r="L52" t="s" s="2">
         <v>367</v>
       </c>
-      <c r="L52" t="s" s="2">
+      <c r="M52" t="s" s="2">
         <v>368</v>
       </c>
-      <c r="M52" t="s" s="2">
+      <c r="N52" t="s" s="2">
         <v>369</v>
-      </c>
-      <c r="N52" t="s" s="2">
-        <v>370</v>
       </c>
       <c r="O52" t="s" s="2">
         <v>45</v>
@@ -8088,7 +8085,7 @@
         <v>45</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>43</v>
@@ -8109,10 +8106,10 @@
         <v>45</v>
       </c>
       <c r="AL52" t="s" s="2">
+        <v>371</v>
+      </c>
+      <c r="AM52" t="s" s="2">
         <v>372</v>
-      </c>
-      <c r="AM52" t="s" s="2">
-        <v>373</v>
       </c>
       <c r="AN52" t="s" s="2">
         <v>45</v>
@@ -8123,7 +8120,7 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
@@ -8149,65 +8146,65 @@
         <v>132</v>
       </c>
       <c r="K53" t="s" s="2">
+        <v>374</v>
+      </c>
+      <c r="L53" t="s" s="2">
         <v>375</v>
-      </c>
-      <c r="L53" t="s" s="2">
-        <v>376</v>
       </c>
       <c r="M53" s="2"/>
       <c r="N53" t="s" s="2">
+        <v>376</v>
+      </c>
+      <c r="O53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="P53" t="s" s="2">
         <v>377</v>
       </c>
-      <c r="O53" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="P53" t="s" s="2">
+      <c r="Q53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="R53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="S53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="T53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="U53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="V53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="W53" t="s" s="2">
+        <v>194</v>
+      </c>
+      <c r="X53" t="s" s="2">
         <v>378</v>
       </c>
-      <c r="Q53" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="R53" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="S53" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="T53" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="U53" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="V53" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="W53" t="s" s="2">
-        <v>195</v>
-      </c>
-      <c r="X53" t="s" s="2">
+      <c r="Y53" t="s" s="2">
         <v>379</v>
       </c>
-      <c r="Y53" t="s" s="2">
+      <c r="Z53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE53" t="s" s="2">
         <v>380</v>
-      </c>
-      <c r="Z53" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AA53" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AB53" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AC53" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AD53" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AE53" t="s" s="2">
-        <v>381</v>
       </c>
       <c r="AF53" t="s" s="2">
         <v>43</v>
@@ -8228,10 +8225,10 @@
         <v>45</v>
       </c>
       <c r="AL53" t="s" s="2">
+        <v>381</v>
+      </c>
+      <c r="AM53" t="s" s="2">
         <v>382</v>
-      </c>
-      <c r="AM53" t="s" s="2">
-        <v>383</v>
       </c>
       <c r="AN53" t="s" s="2">
         <v>45</v>
@@ -8242,7 +8239,7 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
@@ -8268,14 +8265,14 @@
         <v>57</v>
       </c>
       <c r="K54" t="s" s="2">
+        <v>384</v>
+      </c>
+      <c r="L54" t="s" s="2">
         <v>385</v>
-      </c>
-      <c r="L54" t="s" s="2">
-        <v>386</v>
       </c>
       <c r="M54" s="2"/>
       <c r="N54" t="s" s="2">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="O54" t="s" s="2">
         <v>45</v>
@@ -8285,46 +8282,46 @@
         <v>45</v>
       </c>
       <c r="R54" t="s" s="2">
+        <v>387</v>
+      </c>
+      <c r="S54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="T54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="U54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="V54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="W54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="X54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Y54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Z54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE54" t="s" s="2">
         <v>388</v>
-      </c>
-      <c r="S54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="T54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="U54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="V54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="W54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="X54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="Y54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="Z54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AA54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AB54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AC54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AD54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AE54" t="s" s="2">
-        <v>389</v>
       </c>
       <c r="AF54" t="s" s="2">
         <v>43</v>
@@ -8345,10 +8342,10 @@
         <v>45</v>
       </c>
       <c r="AL54" t="s" s="2">
+        <v>389</v>
+      </c>
+      <c r="AM54" t="s" s="2">
         <v>390</v>
-      </c>
-      <c r="AM54" t="s" s="2">
-        <v>391</v>
       </c>
       <c r="AN54" t="s" s="2">
         <v>45</v>
@@ -8359,7 +8356,7 @@
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" t="s" s="2">
@@ -8385,14 +8382,14 @@
         <v>97</v>
       </c>
       <c r="K55" t="s" s="2">
+        <v>392</v>
+      </c>
+      <c r="L55" t="s" s="2">
         <v>393</v>
-      </c>
-      <c r="L55" t="s" s="2">
-        <v>394</v>
       </c>
       <c r="M55" s="2"/>
       <c r="N55" t="s" s="2">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="O55" t="s" s="2">
         <v>45</v>
@@ -8441,7 +8438,7 @@
         <v>45</v>
       </c>
       <c r="AE55" t="s" s="2">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="AF55" t="s" s="2">
         <v>43</v>
@@ -8450,7 +8447,7 @@
         <v>55</v>
       </c>
       <c r="AH55" t="s" s="2">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="AI55" t="s" s="2">
         <v>67</v>
@@ -8462,10 +8459,10 @@
         <v>45</v>
       </c>
       <c r="AL55" t="s" s="2">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="AM55" t="s" s="2">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="AN55" t="s" s="2">
         <v>45</v>
@@ -8476,7 +8473,7 @@
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
@@ -8502,16 +8499,16 @@
         <v>132</v>
       </c>
       <c r="K56" t="s" s="2">
+        <v>399</v>
+      </c>
+      <c r="L56" t="s" s="2">
         <v>400</v>
       </c>
-      <c r="L56" t="s" s="2">
+      <c r="M56" t="s" s="2">
         <v>401</v>
       </c>
-      <c r="M56" t="s" s="2">
+      <c r="N56" t="s" s="2">
         <v>402</v>
-      </c>
-      <c r="N56" t="s" s="2">
-        <v>403</v>
       </c>
       <c r="O56" t="s" s="2">
         <v>45</v>
@@ -8560,7 +8557,7 @@
         <v>45</v>
       </c>
       <c r="AE56" t="s" s="2">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="AF56" t="s" s="2">
         <v>43</v>
@@ -8581,10 +8578,10 @@
         <v>45</v>
       </c>
       <c r="AL56" t="s" s="2">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="AM56" t="s" s="2">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="AN56" t="s" s="2">
         <v>45</v>
@@ -8595,7 +8592,7 @@
     </row>
     <row r="57">
       <c r="A57" t="s" s="2">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
@@ -8618,19 +8615,19 @@
         <v>45</v>
       </c>
       <c r="J57" t="s" s="2">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="K57" t="s" s="2">
+        <v>406</v>
+      </c>
+      <c r="L57" t="s" s="2">
         <v>407</v>
       </c>
-      <c r="L57" t="s" s="2">
+      <c r="M57" t="s" s="2">
         <v>408</v>
       </c>
-      <c r="M57" t="s" s="2">
+      <c r="N57" t="s" s="2">
         <v>409</v>
-      </c>
-      <c r="N57" t="s" s="2">
-        <v>410</v>
       </c>
       <c r="O57" t="s" s="2">
         <v>45</v>
@@ -8658,11 +8655,11 @@
         <v>113</v>
       </c>
       <c r="X57" t="s" s="2">
+        <v>410</v>
+      </c>
+      <c r="Y57" t="s" s="2">
         <v>411</v>
       </c>
-      <c r="Y57" t="s" s="2">
-        <v>412</v>
-      </c>
       <c r="Z57" t="s" s="2">
         <v>45</v>
       </c>
@@ -8679,7 +8676,7 @@
         <v>45</v>
       </c>
       <c r="AE57" t="s" s="2">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="AF57" t="s" s="2">
         <v>43</v>
@@ -8688,7 +8685,7 @@
         <v>55</v>
       </c>
       <c r="AH57" t="s" s="2">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="AI57" t="s" s="2">
         <v>67</v>
@@ -8703,7 +8700,7 @@
         <v>155</v>
       </c>
       <c r="AM57" t="s" s="2">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="AN57" t="s" s="2">
         <v>45</v>
@@ -8714,11 +8711,11 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D58" s="2"/>
       <c r="E58" t="s" s="2">
@@ -8737,19 +8734,19 @@
         <v>45</v>
       </c>
       <c r="J58" t="s" s="2">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="K58" t="s" s="2">
+        <v>416</v>
+      </c>
+      <c r="L58" t="s" s="2">
         <v>417</v>
       </c>
-      <c r="L58" t="s" s="2">
+      <c r="M58" t="s" s="2">
         <v>418</v>
       </c>
-      <c r="M58" t="s" s="2">
+      <c r="N58" t="s" s="2">
         <v>419</v>
-      </c>
-      <c r="N58" t="s" s="2">
-        <v>420</v>
       </c>
       <c r="O58" t="s" s="2">
         <v>45</v>
@@ -8777,11 +8774,11 @@
         <v>113</v>
       </c>
       <c r="X58" t="s" s="2">
+        <v>420</v>
+      </c>
+      <c r="Y58" t="s" s="2">
         <v>421</v>
       </c>
-      <c r="Y58" t="s" s="2">
-        <v>422</v>
-      </c>
       <c r="Z58" t="s" s="2">
         <v>45</v>
       </c>
@@ -8798,7 +8795,7 @@
         <v>45</v>
       </c>
       <c r="AE58" t="s" s="2">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="AF58" t="s" s="2">
         <v>43</v>
@@ -8816,24 +8813,24 @@
         <v>45</v>
       </c>
       <c r="AK58" t="s" s="2">
+        <v>422</v>
+      </c>
+      <c r="AL58" t="s" s="2">
         <v>423</v>
       </c>
-      <c r="AL58" t="s" s="2">
+      <c r="AM58" t="s" s="2">
         <v>424</v>
       </c>
-      <c r="AM58" t="s" s="2">
+      <c r="AN58" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO58" t="s" s="2">
         <v>425</v>
-      </c>
-      <c r="AN58" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO58" t="s" s="2">
-        <v>426</v>
       </c>
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
@@ -8856,19 +8853,19 @@
         <v>45</v>
       </c>
       <c r="J59" t="s" s="2">
+        <v>427</v>
+      </c>
+      <c r="K59" t="s" s="2">
         <v>428</v>
       </c>
-      <c r="K59" t="s" s="2">
+      <c r="L59" t="s" s="2">
         <v>429</v>
       </c>
-      <c r="L59" t="s" s="2">
+      <c r="M59" t="s" s="2">
         <v>430</v>
       </c>
-      <c r="M59" t="s" s="2">
+      <c r="N59" t="s" s="2">
         <v>431</v>
-      </c>
-      <c r="N59" t="s" s="2">
-        <v>432</v>
       </c>
       <c r="O59" t="s" s="2">
         <v>45</v>
@@ -8917,7 +8914,7 @@
         <v>45</v>
       </c>
       <c r="AE59" t="s" s="2">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="AF59" t="s" s="2">
         <v>43</v>
@@ -8938,10 +8935,10 @@
         <v>45</v>
       </c>
       <c r="AL59" t="s" s="2">
+        <v>432</v>
+      </c>
+      <c r="AM59" t="s" s="2">
         <v>433</v>
-      </c>
-      <c r="AM59" t="s" s="2">
-        <v>434</v>
       </c>
       <c r="AN59" t="s" s="2">
         <v>45</v>
@@ -8952,7 +8949,7 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
@@ -8975,16 +8972,16 @@
         <v>45</v>
       </c>
       <c r="J60" t="s" s="2">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="K60" t="s" s="2">
+        <v>435</v>
+      </c>
+      <c r="L60" t="s" s="2">
         <v>436</v>
       </c>
-      <c r="L60" t="s" s="2">
+      <c r="M60" t="s" s="2">
         <v>437</v>
-      </c>
-      <c r="M60" t="s" s="2">
-        <v>438</v>
       </c>
       <c r="N60" s="2"/>
       <c r="O60" t="s" s="2">
@@ -9013,11 +9010,11 @@
         <v>122</v>
       </c>
       <c r="X60" t="s" s="2">
+        <v>438</v>
+      </c>
+      <c r="Y60" t="s" s="2">
         <v>439</v>
       </c>
-      <c r="Y60" t="s" s="2">
-        <v>440</v>
-      </c>
       <c r="Z60" t="s" s="2">
         <v>45</v>
       </c>
@@ -9034,7 +9031,7 @@
         <v>45</v>
       </c>
       <c r="AE60" t="s" s="2">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="AF60" t="s" s="2">
         <v>43</v>
@@ -9052,24 +9049,24 @@
         <v>45</v>
       </c>
       <c r="AK60" t="s" s="2">
+        <v>440</v>
+      </c>
+      <c r="AL60" t="s" s="2">
         <v>441</v>
       </c>
-      <c r="AL60" t="s" s="2">
+      <c r="AM60" t="s" s="2">
         <v>442</v>
       </c>
-      <c r="AM60" t="s" s="2">
+      <c r="AN60" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO60" t="s" s="2">
         <v>443</v>
-      </c>
-      <c r="AN60" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO60" t="s" s="2">
-        <v>444</v>
       </c>
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
@@ -9092,19 +9089,19 @@
         <v>45</v>
       </c>
       <c r="J61" t="s" s="2">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="K61" t="s" s="2">
+        <v>445</v>
+      </c>
+      <c r="L61" t="s" s="2">
         <v>446</v>
       </c>
-      <c r="L61" t="s" s="2">
+      <c r="M61" t="s" s="2">
         <v>447</v>
       </c>
-      <c r="M61" t="s" s="2">
+      <c r="N61" t="s" s="2">
         <v>448</v>
-      </c>
-      <c r="N61" t="s" s="2">
-        <v>449</v>
       </c>
       <c r="O61" t="s" s="2">
         <v>45</v>
@@ -9132,11 +9129,11 @@
         <v>122</v>
       </c>
       <c r="X61" t="s" s="2">
+        <v>449</v>
+      </c>
+      <c r="Y61" t="s" s="2">
         <v>450</v>
       </c>
-      <c r="Y61" t="s" s="2">
-        <v>451</v>
-      </c>
       <c r="Z61" t="s" s="2">
         <v>45</v>
       </c>
@@ -9153,7 +9150,7 @@
         <v>45</v>
       </c>
       <c r="AE61" t="s" s="2">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="AF61" t="s" s="2">
         <v>43</v>
@@ -9174,10 +9171,10 @@
         <v>45</v>
       </c>
       <c r="AL61" t="s" s="2">
+        <v>451</v>
+      </c>
+      <c r="AM61" t="s" s="2">
         <v>452</v>
-      </c>
-      <c r="AM61" t="s" s="2">
-        <v>453</v>
       </c>
       <c r="AN61" t="s" s="2">
         <v>45</v>
@@ -9188,7 +9185,7 @@
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
@@ -9211,16 +9208,16 @@
         <v>45</v>
       </c>
       <c r="J62" t="s" s="2">
+        <v>454</v>
+      </c>
+      <c r="K62" t="s" s="2">
         <v>455</v>
       </c>
-      <c r="K62" t="s" s="2">
+      <c r="L62" t="s" s="2">
         <v>456</v>
       </c>
-      <c r="L62" t="s" s="2">
+      <c r="M62" t="s" s="2">
         <v>457</v>
-      </c>
-      <c r="M62" t="s" s="2">
-        <v>458</v>
       </c>
       <c r="N62" s="2"/>
       <c r="O62" t="s" s="2">
@@ -9270,7 +9267,7 @@
         <v>45</v>
       </c>
       <c r="AE62" t="s" s="2">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="AF62" t="s" s="2">
         <v>43</v>
@@ -9288,24 +9285,24 @@
         <v>45</v>
       </c>
       <c r="AK62" t="s" s="2">
+        <v>458</v>
+      </c>
+      <c r="AL62" t="s" s="2">
         <v>459</v>
       </c>
-      <c r="AL62" t="s" s="2">
+      <c r="AM62" t="s" s="2">
         <v>460</v>
       </c>
-      <c r="AM62" t="s" s="2">
+      <c r="AN62" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO62" t="s" s="2">
         <v>461</v>
-      </c>
-      <c r="AN62" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO62" t="s" s="2">
-        <v>462</v>
       </c>
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" t="s" s="2">
@@ -9328,16 +9325,16 @@
         <v>45</v>
       </c>
       <c r="J63" t="s" s="2">
+        <v>463</v>
+      </c>
+      <c r="K63" t="s" s="2">
         <v>464</v>
       </c>
-      <c r="K63" t="s" s="2">
+      <c r="L63" t="s" s="2">
         <v>465</v>
       </c>
-      <c r="L63" t="s" s="2">
+      <c r="M63" t="s" s="2">
         <v>466</v>
-      </c>
-      <c r="M63" t="s" s="2">
-        <v>467</v>
       </c>
       <c r="N63" s="2"/>
       <c r="O63" t="s" s="2">
@@ -9387,7 +9384,7 @@
         <v>45</v>
       </c>
       <c r="AE63" t="s" s="2">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="AF63" t="s" s="2">
         <v>43</v>
@@ -9405,24 +9402,24 @@
         <v>45</v>
       </c>
       <c r="AK63" t="s" s="2">
+        <v>467</v>
+      </c>
+      <c r="AL63" t="s" s="2">
         <v>468</v>
       </c>
-      <c r="AL63" t="s" s="2">
+      <c r="AM63" t="s" s="2">
         <v>469</v>
       </c>
-      <c r="AM63" t="s" s="2">
+      <c r="AN63" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO63" t="s" s="2">
         <v>470</v>
-      </c>
-      <c r="AN63" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO63" t="s" s="2">
-        <v>471</v>
       </c>
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" t="s" s="2">
@@ -9445,19 +9442,19 @@
         <v>45</v>
       </c>
       <c r="J64" t="s" s="2">
+        <v>472</v>
+      </c>
+      <c r="K64" t="s" s="2">
         <v>473</v>
       </c>
-      <c r="K64" t="s" s="2">
+      <c r="L64" t="s" s="2">
         <v>474</v>
       </c>
-      <c r="L64" t="s" s="2">
+      <c r="M64" t="s" s="2">
         <v>475</v>
       </c>
-      <c r="M64" t="s" s="2">
+      <c r="N64" t="s" s="2">
         <v>476</v>
-      </c>
-      <c r="N64" t="s" s="2">
-        <v>477</v>
       </c>
       <c r="O64" t="s" s="2">
         <v>45</v>
@@ -9506,7 +9503,7 @@
         <v>45</v>
       </c>
       <c r="AE64" t="s" s="2">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="AF64" t="s" s="2">
         <v>43</v>
@@ -9518,19 +9515,19 @@
         <v>45</v>
       </c>
       <c r="AI64" t="s" s="2">
+        <v>477</v>
+      </c>
+      <c r="AJ64" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK64" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL64" t="s" s="2">
         <v>478</v>
       </c>
-      <c r="AJ64" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK64" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL64" t="s" s="2">
+      <c r="AM64" t="s" s="2">
         <v>479</v>
-      </c>
-      <c r="AM64" t="s" s="2">
-        <v>480</v>
       </c>
       <c r="AN64" t="s" s="2">
         <v>45</v>
@@ -9541,7 +9538,7 @@
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" t="s" s="2">
@@ -9656,7 +9653,7 @@
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" t="s" s="2">
@@ -9773,11 +9770,11 @@
     </row>
     <row r="67" hidden="true">
       <c r="A67" t="s" s="2">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" t="s" s="2">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D67" s="2"/>
       <c r="E67" t="s" s="2">
@@ -9799,16 +9796,16 @@
         <v>75</v>
       </c>
       <c r="K67" t="s" s="2">
+        <v>484</v>
+      </c>
+      <c r="L67" t="s" s="2">
         <v>485</v>
-      </c>
-      <c r="L67" t="s" s="2">
-        <v>486</v>
       </c>
       <c r="M67" t="s" s="2">
         <v>78</v>
       </c>
       <c r="N67" t="s" s="2">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="O67" t="s" s="2">
         <v>45</v>
@@ -9857,7 +9854,7 @@
         <v>45</v>
       </c>
       <c r="AE67" t="s" s="2">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="AF67" t="s" s="2">
         <v>43</v>
@@ -9892,7 +9889,7 @@
     </row>
     <row r="68" hidden="true">
       <c r="A68" t="s" s="2">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B68" s="2"/>
       <c r="C68" t="s" s="2">
@@ -9915,13 +9912,13 @@
         <v>45</v>
       </c>
       <c r="J68" t="s" s="2">
+        <v>489</v>
+      </c>
+      <c r="K68" t="s" s="2">
         <v>490</v>
       </c>
-      <c r="K68" t="s" s="2">
+      <c r="L68" t="s" s="2">
         <v>491</v>
-      </c>
-      <c r="L68" t="s" s="2">
-        <v>492</v>
       </c>
       <c r="M68" s="2"/>
       <c r="N68" s="2"/>
@@ -9972,7 +9969,7 @@
         <v>45</v>
       </c>
       <c r="AE68" t="s" s="2">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="AF68" t="s" s="2">
         <v>43</v>
@@ -9981,7 +9978,7 @@
         <v>55</v>
       </c>
       <c r="AH68" t="s" s="2">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="AI68" t="s" s="2">
         <v>67</v>
@@ -9993,10 +9990,10 @@
         <v>45</v>
       </c>
       <c r="AL68" t="s" s="2">
+        <v>493</v>
+      </c>
+      <c r="AM68" t="s" s="2">
         <v>494</v>
-      </c>
-      <c r="AM68" t="s" s="2">
-        <v>495</v>
       </c>
       <c r="AN68" t="s" s="2">
         <v>45</v>
@@ -10007,7 +10004,7 @@
     </row>
     <row r="69" hidden="true">
       <c r="A69" t="s" s="2">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" t="s" s="2">
@@ -10030,13 +10027,13 @@
         <v>45</v>
       </c>
       <c r="J69" t="s" s="2">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="K69" t="s" s="2">
+        <v>496</v>
+      </c>
+      <c r="L69" t="s" s="2">
         <v>497</v>
-      </c>
-      <c r="L69" t="s" s="2">
-        <v>498</v>
       </c>
       <c r="M69" s="2"/>
       <c r="N69" s="2"/>
@@ -10087,7 +10084,7 @@
         <v>45</v>
       </c>
       <c r="AE69" t="s" s="2">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="AF69" t="s" s="2">
         <v>43</v>
@@ -10096,7 +10093,7 @@
         <v>55</v>
       </c>
       <c r="AH69" t="s" s="2">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="AI69" t="s" s="2">
         <v>67</v>
@@ -10108,10 +10105,10 @@
         <v>45</v>
       </c>
       <c r="AL69" t="s" s="2">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="AM69" t="s" s="2">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="AN69" t="s" s="2">
         <v>45</v>
@@ -10122,7 +10119,7 @@
     </row>
     <row r="70" hidden="true">
       <c r="A70" t="s" s="2">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" t="s" s="2">
@@ -10145,19 +10142,19 @@
         <v>45</v>
       </c>
       <c r="J70" t="s" s="2">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="K70" t="s" s="2">
+        <v>500</v>
+      </c>
+      <c r="L70" t="s" s="2">
         <v>501</v>
       </c>
-      <c r="L70" t="s" s="2">
+      <c r="M70" t="s" s="2">
         <v>502</v>
       </c>
-      <c r="M70" t="s" s="2">
+      <c r="N70" t="s" s="2">
         <v>503</v>
-      </c>
-      <c r="N70" t="s" s="2">
-        <v>504</v>
       </c>
       <c r="O70" t="s" s="2">
         <v>45</v>
@@ -10185,11 +10182,11 @@
         <v>136</v>
       </c>
       <c r="X70" t="s" s="2">
+        <v>504</v>
+      </c>
+      <c r="Y70" t="s" s="2">
         <v>505</v>
       </c>
-      <c r="Y70" t="s" s="2">
-        <v>506</v>
-      </c>
       <c r="Z70" t="s" s="2">
         <v>45</v>
       </c>
@@ -10206,7 +10203,7 @@
         <v>45</v>
       </c>
       <c r="AE70" t="s" s="2">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="AF70" t="s" s="2">
         <v>43</v>
@@ -10224,13 +10221,13 @@
         <v>45</v>
       </c>
       <c r="AK70" t="s" s="2">
+        <v>506</v>
+      </c>
+      <c r="AL70" t="s" s="2">
         <v>507</v>
       </c>
-      <c r="AL70" t="s" s="2">
-        <v>508</v>
-      </c>
       <c r="AM70" t="s" s="2">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="AN70" t="s" s="2">
         <v>45</v>
@@ -10241,7 +10238,7 @@
     </row>
     <row r="71" hidden="true">
       <c r="A71" t="s" s="2">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B71" s="2"/>
       <c r="C71" t="s" s="2">
@@ -10264,19 +10261,19 @@
         <v>45</v>
       </c>
       <c r="J71" t="s" s="2">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="K71" t="s" s="2">
+        <v>509</v>
+      </c>
+      <c r="L71" t="s" s="2">
         <v>510</v>
       </c>
-      <c r="L71" t="s" s="2">
+      <c r="M71" t="s" s="2">
         <v>511</v>
       </c>
-      <c r="M71" t="s" s="2">
+      <c r="N71" t="s" s="2">
         <v>512</v>
-      </c>
-      <c r="N71" t="s" s="2">
-        <v>513</v>
       </c>
       <c r="O71" t="s" s="2">
         <v>45</v>
@@ -10304,11 +10301,11 @@
         <v>122</v>
       </c>
       <c r="X71" t="s" s="2">
+        <v>513</v>
+      </c>
+      <c r="Y71" t="s" s="2">
         <v>514</v>
       </c>
-      <c r="Y71" t="s" s="2">
-        <v>515</v>
-      </c>
       <c r="Z71" t="s" s="2">
         <v>45</v>
       </c>
@@ -10325,7 +10322,7 @@
         <v>45</v>
       </c>
       <c r="AE71" t="s" s="2">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="AF71" t="s" s="2">
         <v>43</v>
@@ -10343,13 +10340,13 @@
         <v>45</v>
       </c>
       <c r="AK71" t="s" s="2">
+        <v>506</v>
+      </c>
+      <c r="AL71" t="s" s="2">
         <v>507</v>
       </c>
-      <c r="AL71" t="s" s="2">
-        <v>508</v>
-      </c>
       <c r="AM71" t="s" s="2">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="AN71" t="s" s="2">
         <v>45</v>
@@ -10360,7 +10357,7 @@
     </row>
     <row r="72" hidden="true">
       <c r="A72" t="s" s="2">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" t="s" s="2">
@@ -10383,17 +10380,17 @@
         <v>45</v>
       </c>
       <c r="J72" t="s" s="2">
+        <v>516</v>
+      </c>
+      <c r="K72" t="s" s="2">
         <v>517</v>
       </c>
-      <c r="K72" t="s" s="2">
+      <c r="L72" t="s" s="2">
         <v>518</v>
-      </c>
-      <c r="L72" t="s" s="2">
-        <v>519</v>
       </c>
       <c r="M72" s="2"/>
       <c r="N72" t="s" s="2">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="O72" t="s" s="2">
         <v>45</v>
@@ -10442,7 +10439,7 @@
         <v>45</v>
       </c>
       <c r="AE72" t="s" s="2">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="AF72" t="s" s="2">
         <v>43</v>
@@ -10466,7 +10463,7 @@
         <v>45</v>
       </c>
       <c r="AM72" t="s" s="2">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="AN72" t="s" s="2">
         <v>45</v>
@@ -10477,7 +10474,7 @@
     </row>
     <row r="73" hidden="true">
       <c r="A73" t="s" s="2">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" t="s" s="2">
@@ -10503,10 +10500,10 @@
         <v>57</v>
       </c>
       <c r="K73" t="s" s="2">
+        <v>522</v>
+      </c>
+      <c r="L73" t="s" s="2">
         <v>523</v>
-      </c>
-      <c r="L73" t="s" s="2">
-        <v>524</v>
       </c>
       <c r="M73" s="2"/>
       <c r="N73" s="2"/>
@@ -10557,7 +10554,7 @@
         <v>45</v>
       </c>
       <c r="AE73" t="s" s="2">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="AF73" t="s" s="2">
         <v>43</v>
@@ -10578,10 +10575,10 @@
         <v>45</v>
       </c>
       <c r="AL73" t="s" s="2">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="AM73" t="s" s="2">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="AN73" t="s" s="2">
         <v>45</v>
@@ -10592,7 +10589,7 @@
     </row>
     <row r="74" hidden="true">
       <c r="A74" t="s" s="2">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B74" s="2"/>
       <c r="C74" t="s" s="2">
@@ -10615,16 +10612,16 @@
         <v>56</v>
       </c>
       <c r="J74" t="s" s="2">
+        <v>526</v>
+      </c>
+      <c r="K74" t="s" s="2">
         <v>527</v>
       </c>
-      <c r="K74" t="s" s="2">
+      <c r="L74" t="s" s="2">
         <v>528</v>
       </c>
-      <c r="L74" t="s" s="2">
+      <c r="M74" t="s" s="2">
         <v>529</v>
-      </c>
-      <c r="M74" t="s" s="2">
-        <v>530</v>
       </c>
       <c r="N74" s="2"/>
       <c r="O74" t="s" s="2">
@@ -10674,7 +10671,7 @@
         <v>45</v>
       </c>
       <c r="AE74" t="s" s="2">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="AF74" t="s" s="2">
         <v>43</v>
@@ -10695,10 +10692,10 @@
         <v>45</v>
       </c>
       <c r="AL74" t="s" s="2">
+        <v>530</v>
+      </c>
+      <c r="AM74" t="s" s="2">
         <v>531</v>
-      </c>
-      <c r="AM74" t="s" s="2">
-        <v>532</v>
       </c>
       <c r="AN74" t="s" s="2">
         <v>45</v>
@@ -10709,7 +10706,7 @@
     </row>
     <row r="75" hidden="true">
       <c r="A75" t="s" s="2">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B75" s="2"/>
       <c r="C75" t="s" s="2">
@@ -10732,16 +10729,16 @@
         <v>56</v>
       </c>
       <c r="J75" t="s" s="2">
+        <v>533</v>
+      </c>
+      <c r="K75" t="s" s="2">
         <v>534</v>
       </c>
-      <c r="K75" t="s" s="2">
+      <c r="L75" t="s" s="2">
         <v>535</v>
       </c>
-      <c r="L75" t="s" s="2">
+      <c r="M75" t="s" s="2">
         <v>536</v>
-      </c>
-      <c r="M75" t="s" s="2">
-        <v>537</v>
       </c>
       <c r="N75" s="2"/>
       <c r="O75" t="s" s="2">
@@ -10791,7 +10788,7 @@
         <v>45</v>
       </c>
       <c r="AE75" t="s" s="2">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="AF75" t="s" s="2">
         <v>43</v>
@@ -10812,10 +10809,10 @@
         <v>45</v>
       </c>
       <c r="AL75" t="s" s="2">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="AM75" t="s" s="2">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="AN75" t="s" s="2">
         <v>45</v>
@@ -10826,7 +10823,7 @@
     </row>
     <row r="76">
       <c r="A76" t="s" s="2">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B76" s="2"/>
       <c r="C76" t="s" s="2">
@@ -10849,19 +10846,19 @@
         <v>56</v>
       </c>
       <c r="J76" t="s" s="2">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="K76" t="s" s="2">
+        <v>539</v>
+      </c>
+      <c r="L76" t="s" s="2">
+        <v>539</v>
+      </c>
+      <c r="M76" t="s" s="2">
         <v>540</v>
       </c>
-      <c r="L76" t="s" s="2">
-        <v>540</v>
-      </c>
-      <c r="M76" t="s" s="2">
+      <c r="N76" t="s" s="2">
         <v>541</v>
-      </c>
-      <c r="N76" t="s" s="2">
-        <v>542</v>
       </c>
       <c r="O76" t="s" s="2">
         <v>45</v>
@@ -10910,7 +10907,7 @@
         <v>45</v>
       </c>
       <c r="AE76" t="s" s="2">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="AF76" t="s" s="2">
         <v>43</v>
@@ -10922,19 +10919,19 @@
         <v>45</v>
       </c>
       <c r="AI76" t="s" s="2">
+        <v>542</v>
+      </c>
+      <c r="AJ76" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK76" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL76" t="s" s="2">
         <v>543</v>
       </c>
-      <c r="AJ76" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK76" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL76" t="s" s="2">
+      <c r="AM76" t="s" s="2">
         <v>544</v>
-      </c>
-      <c r="AM76" t="s" s="2">
-        <v>545</v>
       </c>
       <c r="AN76" t="s" s="2">
         <v>45</v>
@@ -10945,7 +10942,7 @@
     </row>
     <row r="77" hidden="true">
       <c r="A77" t="s" s="2">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B77" s="2"/>
       <c r="C77" t="s" s="2">
@@ -11060,7 +11057,7 @@
     </row>
     <row r="78" hidden="true">
       <c r="A78" t="s" s="2">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B78" s="2"/>
       <c r="C78" t="s" s="2">
@@ -11177,11 +11174,11 @@
     </row>
     <row r="79" hidden="true">
       <c r="A79" t="s" s="2">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B79" s="2"/>
       <c r="C79" t="s" s="2">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D79" s="2"/>
       <c r="E79" t="s" s="2">
@@ -11203,16 +11200,16 @@
         <v>75</v>
       </c>
       <c r="K79" t="s" s="2">
+        <v>484</v>
+      </c>
+      <c r="L79" t="s" s="2">
         <v>485</v>
-      </c>
-      <c r="L79" t="s" s="2">
-        <v>486</v>
       </c>
       <c r="M79" t="s" s="2">
         <v>78</v>
       </c>
       <c r="N79" t="s" s="2">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="O79" t="s" s="2">
         <v>45</v>
@@ -11261,7 +11258,7 @@
         <v>45</v>
       </c>
       <c r="AE79" t="s" s="2">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="AF79" t="s" s="2">
         <v>43</v>
@@ -11296,7 +11293,7 @@
     </row>
     <row r="80">
       <c r="A80" t="s" s="2">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" t="s" s="2">
@@ -11319,19 +11316,19 @@
         <v>56</v>
       </c>
       <c r="J80" t="s" s="2">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="K80" t="s" s="2">
+        <v>549</v>
+      </c>
+      <c r="L80" t="s" s="2">
         <v>550</v>
       </c>
-      <c r="L80" t="s" s="2">
+      <c r="M80" t="s" s="2">
         <v>551</v>
       </c>
-      <c r="M80" t="s" s="2">
+      <c r="N80" t="s" s="2">
         <v>552</v>
-      </c>
-      <c r="N80" t="s" s="2">
-        <v>553</v>
       </c>
       <c r="O80" t="s" s="2">
         <v>45</v>
@@ -11359,11 +11356,11 @@
         <v>113</v>
       </c>
       <c r="X80" t="s" s="2">
+        <v>280</v>
+      </c>
+      <c r="Y80" t="s" s="2">
         <v>281</v>
       </c>
-      <c r="Y80" t="s" s="2">
-        <v>282</v>
-      </c>
       <c r="Z80" t="s" s="2">
         <v>45</v>
       </c>
@@ -11380,7 +11377,7 @@
         <v>45</v>
       </c>
       <c r="AE80" t="s" s="2">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="AF80" t="s" s="2">
         <v>55</v>
@@ -11398,16 +11395,16 @@
         <v>45</v>
       </c>
       <c r="AK80" t="s" s="2">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="AL80" t="s" s="2">
+        <v>284</v>
+      </c>
+      <c r="AM80" t="s" s="2">
         <v>285</v>
       </c>
-      <c r="AM80" t="s" s="2">
+      <c r="AN80" t="s" s="2">
         <v>286</v>
-      </c>
-      <c r="AN80" t="s" s="2">
-        <v>287</v>
       </c>
       <c r="AO80" t="s" s="2">
         <v>45</v>
@@ -11415,7 +11412,7 @@
     </row>
     <row r="81">
       <c r="A81" t="s" s="2">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B81" s="2"/>
       <c r="C81" t="s" s="2">
@@ -11438,19 +11435,19 @@
         <v>56</v>
       </c>
       <c r="J81" t="s" s="2">
+        <v>555</v>
+      </c>
+      <c r="K81" t="s" s="2">
         <v>556</v>
       </c>
-      <c r="K81" t="s" s="2">
+      <c r="L81" t="s" s="2">
         <v>557</v>
       </c>
-      <c r="L81" t="s" s="2">
+      <c r="M81" t="s" s="2">
         <v>558</v>
       </c>
-      <c r="M81" t="s" s="2">
-        <v>559</v>
-      </c>
       <c r="N81" t="s" s="2">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="O81" t="s" s="2">
         <v>45</v>
@@ -11475,14 +11472,14 @@
         <v>45</v>
       </c>
       <c r="W81" t="s" s="2">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="X81" t="s" s="2">
+        <v>559</v>
+      </c>
+      <c r="Y81" t="s" s="2">
         <v>560</v>
       </c>
-      <c r="Y81" t="s" s="2">
-        <v>561</v>
-      </c>
       <c r="Z81" t="s" s="2">
         <v>45</v>
       </c>
@@ -11499,7 +11496,7 @@
         <v>45</v>
       </c>
       <c r="AE81" t="s" s="2">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="AF81" t="s" s="2">
         <v>43</v>
@@ -11508,7 +11505,7 @@
         <v>55</v>
       </c>
       <c r="AH81" t="s" s="2">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="AI81" t="s" s="2">
         <v>67</v>
@@ -11517,24 +11514,24 @@
         <v>45</v>
       </c>
       <c r="AK81" t="s" s="2">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AL81" t="s" s="2">
+        <v>358</v>
+      </c>
+      <c r="AM81" t="s" s="2">
         <v>359</v>
       </c>
-      <c r="AM81" t="s" s="2">
+      <c r="AN81" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO81" t="s" s="2">
         <v>360</v>
-      </c>
-      <c r="AN81" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO81" t="s" s="2">
-        <v>361</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s" s="2">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B82" s="2"/>
       <c r="C82" t="s" s="2">
@@ -11557,19 +11554,19 @@
         <v>45</v>
       </c>
       <c r="J82" t="s" s="2">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="K82" t="s" s="2">
+        <v>564</v>
+      </c>
+      <c r="L82" t="s" s="2">
         <v>565</v>
       </c>
-      <c r="L82" t="s" s="2">
+      <c r="M82" t="s" s="2">
         <v>566</v>
       </c>
-      <c r="M82" t="s" s="2">
-        <v>567</v>
-      </c>
       <c r="N82" t="s" s="2">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="O82" t="s" s="2">
         <v>45</v>
@@ -11597,11 +11594,11 @@
         <v>113</v>
       </c>
       <c r="X82" t="s" s="2">
+        <v>410</v>
+      </c>
+      <c r="Y82" t="s" s="2">
         <v>411</v>
       </c>
-      <c r="Y82" t="s" s="2">
-        <v>412</v>
-      </c>
       <c r="Z82" t="s" s="2">
         <v>45</v>
       </c>
@@ -11618,7 +11615,7 @@
         <v>45</v>
       </c>
       <c r="AE82" t="s" s="2">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="AF82" t="s" s="2">
         <v>43</v>
@@ -11627,7 +11624,7 @@
         <v>55</v>
       </c>
       <c r="AH82" t="s" s="2">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="AI82" t="s" s="2">
         <v>67</v>
@@ -11642,7 +11639,7 @@
         <v>155</v>
       </c>
       <c r="AM82" t="s" s="2">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="AN82" t="s" s="2">
         <v>45</v>
@@ -11653,11 +11650,11 @@
     </row>
     <row r="83" hidden="true">
       <c r="A83" t="s" s="2">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B83" s="2"/>
       <c r="C83" t="s" s="2">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D83" s="2"/>
       <c r="E83" t="s" s="2">
@@ -11676,19 +11673,19 @@
         <v>45</v>
       </c>
       <c r="J83" t="s" s="2">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="K83" t="s" s="2">
+        <v>416</v>
+      </c>
+      <c r="L83" t="s" s="2">
         <v>417</v>
       </c>
-      <c r="L83" t="s" s="2">
+      <c r="M83" t="s" s="2">
         <v>418</v>
       </c>
-      <c r="M83" t="s" s="2">
+      <c r="N83" t="s" s="2">
         <v>419</v>
-      </c>
-      <c r="N83" t="s" s="2">
-        <v>420</v>
       </c>
       <c r="O83" t="s" s="2">
         <v>45</v>
@@ -11716,11 +11713,11 @@
         <v>113</v>
       </c>
       <c r="X83" t="s" s="2">
+        <v>420</v>
+      </c>
+      <c r="Y83" t="s" s="2">
         <v>421</v>
       </c>
-      <c r="Y83" t="s" s="2">
-        <v>422</v>
-      </c>
       <c r="Z83" t="s" s="2">
         <v>45</v>
       </c>
@@ -11737,7 +11734,7 @@
         <v>45</v>
       </c>
       <c r="AE83" t="s" s="2">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="AF83" t="s" s="2">
         <v>43</v>
@@ -11755,24 +11752,24 @@
         <v>45</v>
       </c>
       <c r="AK83" t="s" s="2">
+        <v>422</v>
+      </c>
+      <c r="AL83" t="s" s="2">
         <v>423</v>
       </c>
-      <c r="AL83" t="s" s="2">
+      <c r="AM83" t="s" s="2">
         <v>424</v>
       </c>
-      <c r="AM83" t="s" s="2">
+      <c r="AN83" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO83" t="s" s="2">
         <v>425</v>
-      </c>
-      <c r="AN83" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO83" t="s" s="2">
-        <v>426</v>
       </c>
     </row>
     <row r="84" hidden="true">
       <c r="A84" t="s" s="2">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B84" s="2"/>
       <c r="C84" t="s" s="2">
@@ -11798,16 +11795,16 @@
         <v>45</v>
       </c>
       <c r="K84" t="s" s="2">
+        <v>570</v>
+      </c>
+      <c r="L84" t="s" s="2">
         <v>571</v>
       </c>
-      <c r="L84" t="s" s="2">
-        <v>572</v>
-      </c>
       <c r="M84" t="s" s="2">
+        <v>475</v>
+      </c>
+      <c r="N84" t="s" s="2">
         <v>476</v>
-      </c>
-      <c r="N84" t="s" s="2">
-        <v>477</v>
       </c>
       <c r="O84" t="s" s="2">
         <v>45</v>
@@ -11856,7 +11853,7 @@
         <v>45</v>
       </c>
       <c r="AE84" t="s" s="2">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="AF84" t="s" s="2">
         <v>43</v>
@@ -11877,10 +11874,10 @@
         <v>45</v>
       </c>
       <c r="AL84" t="s" s="2">
+        <v>478</v>
+      </c>
+      <c r="AM84" t="s" s="2">
         <v>479</v>
-      </c>
-      <c r="AM84" t="s" s="2">
-        <v>480</v>
       </c>
       <c r="AN84" t="s" s="2">
         <v>45</v>

</xml_diff>

<commit_message>
fix double coding in pulseOx examples
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-VA.MHV.bloodOxygenSat.xlsx
+++ b/docs/StructureDefinition-VA.MHV.bloodOxygenSat.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3132" uniqueCount="572">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3132" uniqueCount="571">
   <si>
     <t>Path</t>
   </si>
@@ -665,14 +665,6 @@
   </si>
   <si>
     <t>Used for filtering what observations are retrieved and displayed.</t>
-  </si>
-  <si>
-    <t>&lt;valueCodeableConcept xmlns="http://hl7.org/fhir"&gt;
-  &lt;coding&gt;
-    &lt;system value="http://terminology.hl7.org/CodeSystem/observation-category"/&gt;
-    &lt;code value="vital-signs"/&gt;
-  &lt;/coding&gt;
-&lt;/valueCodeableConcept&gt;</t>
   </si>
   <si>
     <t>Codes for high level observation categories.</t>
@@ -4631,7 +4623,7 @@
         <v>45</v>
       </c>
       <c r="R23" t="s" s="2">
-        <v>207</v>
+        <v>45</v>
       </c>
       <c r="S23" t="s" s="2">
         <v>45</v>
@@ -4649,16 +4641,16 @@
         <v>136</v>
       </c>
       <c r="X23" t="s" s="2">
+        <v>207</v>
+      </c>
+      <c r="Y23" t="s" s="2">
         <v>208</v>
       </c>
-      <c r="Y23" t="s" s="2">
+      <c r="Z23" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA23" t="s" s="2">
         <v>209</v>
-      </c>
-      <c r="Z23" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AA23" t="s" s="2">
-        <v>210</v>
       </c>
       <c r="AB23" s="2"/>
       <c r="AC23" t="s" s="2">
@@ -4692,10 +4684,10 @@
         <v>45</v>
       </c>
       <c r="AM23" t="s" s="2">
+        <v>210</v>
+      </c>
+      <c r="AN23" t="s" s="2">
         <v>211</v>
-      </c>
-      <c r="AN23" t="s" s="2">
-        <v>212</v>
       </c>
       <c r="AO23" t="s" s="2">
         <v>45</v>
@@ -4706,7 +4698,7 @@
         <v>201</v>
       </c>
       <c r="B24" t="s" s="2">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C24" t="s" s="2">
         <v>45</v>
@@ -4768,10 +4760,10 @@
         <v>136</v>
       </c>
       <c r="X24" t="s" s="2">
+        <v>207</v>
+      </c>
+      <c r="Y24" t="s" s="2">
         <v>208</v>
-      </c>
-      <c r="Y24" t="s" s="2">
-        <v>209</v>
       </c>
       <c r="Z24" t="s" s="2">
         <v>45</v>
@@ -4813,10 +4805,10 @@
         <v>45</v>
       </c>
       <c r="AM24" t="s" s="2">
+        <v>210</v>
+      </c>
+      <c r="AN24" t="s" s="2">
         <v>211</v>
-      </c>
-      <c r="AN24" t="s" s="2">
-        <v>212</v>
       </c>
       <c r="AO24" t="s" s="2">
         <v>45</v>
@@ -4824,7 +4816,7 @@
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
@@ -4939,7 +4931,7 @@
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
@@ -5056,7 +5048,7 @@
     </row>
     <row r="27">
       <c r="A27" t="s" s="2">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -5082,16 +5074,16 @@
         <v>109</v>
       </c>
       <c r="K27" t="s" s="2">
+        <v>216</v>
+      </c>
+      <c r="L27" t="s" s="2">
         <v>217</v>
       </c>
-      <c r="L27" t="s" s="2">
+      <c r="M27" t="s" s="2">
         <v>218</v>
       </c>
-      <c r="M27" t="s" s="2">
+      <c r="N27" t="s" s="2">
         <v>219</v>
-      </c>
-      <c r="N27" t="s" s="2">
-        <v>220</v>
       </c>
       <c r="O27" t="s" s="2">
         <v>45</v>
@@ -5140,7 +5132,7 @@
         <v>45</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>43</v>
@@ -5161,10 +5153,10 @@
         <v>45</v>
       </c>
       <c r="AL27" t="s" s="2">
+        <v>221</v>
+      </c>
+      <c r="AM27" t="s" s="2">
         <v>222</v>
-      </c>
-      <c r="AM27" t="s" s="2">
-        <v>223</v>
       </c>
       <c r="AN27" t="s" s="2">
         <v>45</v>
@@ -5175,7 +5167,7 @@
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -5290,7 +5282,7 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -5407,7 +5399,7 @@
     </row>
     <row r="30">
       <c r="A30" t="s" s="2">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -5433,65 +5425,65 @@
         <v>97</v>
       </c>
       <c r="K30" t="s" s="2">
+        <v>226</v>
+      </c>
+      <c r="L30" t="s" s="2">
         <v>227</v>
       </c>
-      <c r="L30" t="s" s="2">
+      <c r="M30" t="s" s="2">
         <v>228</v>
       </c>
-      <c r="M30" t="s" s="2">
+      <c r="N30" t="s" s="2">
         <v>229</v>
-      </c>
-      <c r="N30" t="s" s="2">
-        <v>230</v>
       </c>
       <c r="O30" t="s" s="2">
         <v>45</v>
       </c>
       <c r="P30" s="2"/>
       <c r="Q30" t="s" s="2">
+        <v>230</v>
+      </c>
+      <c r="R30" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="S30" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="T30" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="U30" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="V30" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="W30" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="X30" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Y30" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Z30" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA30" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB30" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC30" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD30" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE30" t="s" s="2">
         <v>231</v>
-      </c>
-      <c r="R30" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="S30" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="T30" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="U30" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="V30" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="W30" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="X30" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="Y30" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="Z30" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AA30" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AB30" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AC30" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AD30" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AE30" t="s" s="2">
-        <v>232</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>43</v>
@@ -5512,10 +5504,10 @@
         <v>45</v>
       </c>
       <c r="AL30" t="s" s="2">
+        <v>232</v>
+      </c>
+      <c r="AM30" t="s" s="2">
         <v>233</v>
-      </c>
-      <c r="AM30" t="s" s="2">
-        <v>234</v>
       </c>
       <c r="AN30" t="s" s="2">
         <v>45</v>
@@ -5526,7 +5518,7 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -5552,13 +5544,13 @@
         <v>57</v>
       </c>
       <c r="K31" t="s" s="2">
+        <v>235</v>
+      </c>
+      <c r="L31" t="s" s="2">
         <v>236</v>
       </c>
-      <c r="L31" t="s" s="2">
+      <c r="M31" t="s" s="2">
         <v>237</v>
-      </c>
-      <c r="M31" t="s" s="2">
-        <v>238</v>
       </c>
       <c r="N31" s="2"/>
       <c r="O31" t="s" s="2">
@@ -5608,7 +5600,7 @@
         <v>45</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>43</v>
@@ -5629,10 +5621,10 @@
         <v>45</v>
       </c>
       <c r="AL31" t="s" s="2">
+        <v>239</v>
+      </c>
+      <c r="AM31" t="s" s="2">
         <v>240</v>
-      </c>
-      <c r="AM31" t="s" s="2">
-        <v>241</v>
       </c>
       <c r="AN31" t="s" s="2">
         <v>45</v>
@@ -5643,7 +5635,7 @@
     </row>
     <row r="32">
       <c r="A32" t="s" s="2">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -5669,63 +5661,63 @@
         <v>132</v>
       </c>
       <c r="K32" t="s" s="2">
+        <v>242</v>
+      </c>
+      <c r="L32" t="s" s="2">
         <v>243</v>
-      </c>
-      <c r="L32" t="s" s="2">
-        <v>244</v>
       </c>
       <c r="M32" s="2"/>
       <c r="N32" t="s" s="2">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="O32" t="s" s="2">
         <v>45</v>
       </c>
       <c r="P32" s="2"/>
       <c r="Q32" t="s" s="2">
+        <v>245</v>
+      </c>
+      <c r="R32" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="S32" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="T32" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="U32" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="V32" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="W32" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="X32" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Y32" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Z32" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA32" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB32" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC32" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD32" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE32" t="s" s="2">
         <v>246</v>
-      </c>
-      <c r="R32" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="S32" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="T32" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="U32" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="V32" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="W32" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="X32" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="Y32" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="Z32" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AA32" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AB32" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AC32" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AD32" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AE32" t="s" s="2">
-        <v>247</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>43</v>
@@ -5746,10 +5738,10 @@
         <v>45</v>
       </c>
       <c r="AL32" t="s" s="2">
+        <v>247</v>
+      </c>
+      <c r="AM32" t="s" s="2">
         <v>248</v>
-      </c>
-      <c r="AM32" t="s" s="2">
-        <v>249</v>
       </c>
       <c r="AN32" t="s" s="2">
         <v>45</v>
@@ -5760,7 +5752,7 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -5786,14 +5778,14 @@
         <v>57</v>
       </c>
       <c r="K33" t="s" s="2">
+        <v>250</v>
+      </c>
+      <c r="L33" t="s" s="2">
         <v>251</v>
-      </c>
-      <c r="L33" t="s" s="2">
-        <v>252</v>
       </c>
       <c r="M33" s="2"/>
       <c r="N33" t="s" s="2">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O33" t="s" s="2">
         <v>45</v>
@@ -5842,7 +5834,7 @@
         <v>45</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>43</v>
@@ -5863,10 +5855,10 @@
         <v>45</v>
       </c>
       <c r="AL33" t="s" s="2">
+        <v>254</v>
+      </c>
+      <c r="AM33" t="s" s="2">
         <v>255</v>
-      </c>
-      <c r="AM33" t="s" s="2">
-        <v>256</v>
       </c>
       <c r="AN33" t="s" s="2">
         <v>45</v>
@@ -5877,7 +5869,7 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
@@ -5900,19 +5892,19 @@
         <v>56</v>
       </c>
       <c r="J34" t="s" s="2">
+        <v>257</v>
+      </c>
+      <c r="K34" t="s" s="2">
         <v>258</v>
       </c>
-      <c r="K34" t="s" s="2">
+      <c r="L34" t="s" s="2">
         <v>259</v>
       </c>
-      <c r="L34" t="s" s="2">
+      <c r="M34" t="s" s="2">
         <v>260</v>
       </c>
-      <c r="M34" t="s" s="2">
+      <c r="N34" t="s" s="2">
         <v>261</v>
-      </c>
-      <c r="N34" t="s" s="2">
-        <v>262</v>
       </c>
       <c r="O34" t="s" s="2">
         <v>45</v>
@@ -5961,7 +5953,7 @@
         <v>45</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>43</v>
@@ -5982,10 +5974,10 @@
         <v>45</v>
       </c>
       <c r="AL34" t="s" s="2">
+        <v>263</v>
+      </c>
+      <c r="AM34" t="s" s="2">
         <v>264</v>
-      </c>
-      <c r="AM34" t="s" s="2">
-        <v>265</v>
       </c>
       <c r="AN34" t="s" s="2">
         <v>45</v>
@@ -5996,7 +5988,7 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -6022,16 +6014,16 @@
         <v>57</v>
       </c>
       <c r="K35" t="s" s="2">
+        <v>266</v>
+      </c>
+      <c r="L35" t="s" s="2">
         <v>267</v>
       </c>
-      <c r="L35" t="s" s="2">
+      <c r="M35" t="s" s="2">
         <v>268</v>
       </c>
-      <c r="M35" t="s" s="2">
+      <c r="N35" t="s" s="2">
         <v>269</v>
-      </c>
-      <c r="N35" t="s" s="2">
-        <v>270</v>
       </c>
       <c r="O35" t="s" s="2">
         <v>45</v>
@@ -6080,7 +6072,7 @@
         <v>45</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>43</v>
@@ -6101,10 +6093,10 @@
         <v>45</v>
       </c>
       <c r="AL35" t="s" s="2">
+        <v>271</v>
+      </c>
+      <c r="AM35" t="s" s="2">
         <v>272</v>
-      </c>
-      <c r="AM35" t="s" s="2">
-        <v>273</v>
       </c>
       <c r="AN35" t="s" s="2">
         <v>45</v>
@@ -6115,11 +6107,11 @@
     </row>
     <row r="36">
       <c r="A36" t="s" s="2">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" t="s" s="2">
@@ -6141,16 +6133,16 @@
         <v>202</v>
       </c>
       <c r="K36" t="s" s="2">
+        <v>275</v>
+      </c>
+      <c r="L36" t="s" s="2">
         <v>276</v>
       </c>
-      <c r="L36" t="s" s="2">
+      <c r="M36" t="s" s="2">
         <v>277</v>
       </c>
-      <c r="M36" t="s" s="2">
+      <c r="N36" t="s" s="2">
         <v>278</v>
-      </c>
-      <c r="N36" t="s" s="2">
-        <v>279</v>
       </c>
       <c r="O36" t="s" s="2">
         <v>45</v>
@@ -6178,11 +6170,11 @@
         <v>113</v>
       </c>
       <c r="X36" t="s" s="2">
+        <v>279</v>
+      </c>
+      <c r="Y36" t="s" s="2">
         <v>280</v>
       </c>
-      <c r="Y36" t="s" s="2">
-        <v>281</v>
-      </c>
       <c r="Z36" t="s" s="2">
         <v>45</v>
       </c>
@@ -6199,7 +6191,7 @@
         <v>45</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>55</v>
@@ -6214,27 +6206,27 @@
         <v>67</v>
       </c>
       <c r="AJ36" t="s" s="2">
+        <v>281</v>
+      </c>
+      <c r="AK36" t="s" s="2">
         <v>282</v>
       </c>
-      <c r="AK36" t="s" s="2">
+      <c r="AL36" t="s" s="2">
         <v>283</v>
       </c>
-      <c r="AL36" t="s" s="2">
+      <c r="AM36" t="s" s="2">
         <v>284</v>
       </c>
-      <c r="AM36" t="s" s="2">
+      <c r="AN36" t="s" s="2">
         <v>285</v>
       </c>
-      <c r="AN36" t="s" s="2">
+      <c r="AO36" t="s" s="2">
         <v>286</v>
-      </c>
-      <c r="AO36" t="s" s="2">
-        <v>287</v>
       </c>
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -6349,7 +6341,7 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -6466,7 +6458,7 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -6492,16 +6484,16 @@
         <v>109</v>
       </c>
       <c r="K39" t="s" s="2">
+        <v>216</v>
+      </c>
+      <c r="L39" t="s" s="2">
         <v>217</v>
       </c>
-      <c r="L39" t="s" s="2">
+      <c r="M39" t="s" s="2">
         <v>218</v>
       </c>
-      <c r="M39" t="s" s="2">
+      <c r="N39" t="s" s="2">
         <v>219</v>
-      </c>
-      <c r="N39" t="s" s="2">
-        <v>220</v>
       </c>
       <c r="O39" t="s" s="2">
         <v>45</v>
@@ -6550,7 +6542,7 @@
         <v>45</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>43</v>
@@ -6571,10 +6563,10 @@
         <v>45</v>
       </c>
       <c r="AL39" t="s" s="2">
+        <v>221</v>
+      </c>
+      <c r="AM39" t="s" s="2">
         <v>222</v>
-      </c>
-      <c r="AM39" t="s" s="2">
-        <v>223</v>
       </c>
       <c r="AN39" t="s" s="2">
         <v>45</v>
@@ -6585,7 +6577,7 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -6611,16 +6603,16 @@
         <v>57</v>
       </c>
       <c r="K40" t="s" s="2">
+        <v>266</v>
+      </c>
+      <c r="L40" t="s" s="2">
         <v>267</v>
       </c>
-      <c r="L40" t="s" s="2">
+      <c r="M40" t="s" s="2">
         <v>268</v>
       </c>
-      <c r="M40" t="s" s="2">
+      <c r="N40" t="s" s="2">
         <v>269</v>
-      </c>
-      <c r="N40" t="s" s="2">
-        <v>270</v>
       </c>
       <c r="O40" t="s" s="2">
         <v>45</v>
@@ -6669,7 +6661,7 @@
         <v>45</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>43</v>
@@ -6690,10 +6682,10 @@
         <v>45</v>
       </c>
       <c r="AL40" t="s" s="2">
+        <v>271</v>
+      </c>
+      <c r="AM40" t="s" s="2">
         <v>272</v>
-      </c>
-      <c r="AM40" t="s" s="2">
-        <v>273</v>
       </c>
       <c r="AN40" t="s" s="2">
         <v>45</v>
@@ -6704,7 +6696,7 @@
     </row>
     <row r="41">
       <c r="A41" t="s" s="2">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -6727,19 +6719,19 @@
         <v>56</v>
       </c>
       <c r="J41" t="s" s="2">
+        <v>292</v>
+      </c>
+      <c r="K41" t="s" s="2">
         <v>293</v>
       </c>
-      <c r="K41" t="s" s="2">
+      <c r="L41" t="s" s="2">
         <v>294</v>
       </c>
-      <c r="L41" t="s" s="2">
+      <c r="M41" t="s" s="2">
         <v>295</v>
       </c>
-      <c r="M41" t="s" s="2">
+      <c r="N41" t="s" s="2">
         <v>296</v>
-      </c>
-      <c r="N41" t="s" s="2">
-        <v>297</v>
       </c>
       <c r="O41" t="s" s="2">
         <v>45</v>
@@ -6788,7 +6780,7 @@
         <v>45</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>43</v>
@@ -6803,19 +6795,19 @@
         <v>67</v>
       </c>
       <c r="AJ41" t="s" s="2">
+        <v>297</v>
+      </c>
+      <c r="AK41" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL41" t="s" s="2">
         <v>298</v>
       </c>
-      <c r="AK41" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL41" t="s" s="2">
+      <c r="AM41" t="s" s="2">
         <v>299</v>
       </c>
-      <c r="AM41" t="s" s="2">
+      <c r="AN41" t="s" s="2">
         <v>300</v>
-      </c>
-      <c r="AN41" t="s" s="2">
-        <v>301</v>
       </c>
       <c r="AO41" t="s" s="2">
         <v>45</v>
@@ -6823,7 +6815,7 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -6846,16 +6838,16 @@
         <v>56</v>
       </c>
       <c r="J42" t="s" s="2">
+        <v>302</v>
+      </c>
+      <c r="K42" t="s" s="2">
         <v>303</v>
       </c>
-      <c r="K42" t="s" s="2">
+      <c r="L42" t="s" s="2">
         <v>304</v>
       </c>
-      <c r="L42" t="s" s="2">
+      <c r="M42" t="s" s="2">
         <v>305</v>
-      </c>
-      <c r="M42" t="s" s="2">
-        <v>306</v>
       </c>
       <c r="N42" s="2"/>
       <c r="O42" t="s" s="2">
@@ -6905,7 +6897,7 @@
         <v>45</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>43</v>
@@ -6926,13 +6918,13 @@
         <v>45</v>
       </c>
       <c r="AL42" t="s" s="2">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AN42" t="s" s="2">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="AO42" t="s" s="2">
         <v>45</v>
@@ -6940,11 +6932,11 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" t="s" s="2">
@@ -6963,19 +6955,19 @@
         <v>56</v>
       </c>
       <c r="J43" t="s" s="2">
+        <v>309</v>
+      </c>
+      <c r="K43" t="s" s="2">
         <v>310</v>
       </c>
-      <c r="K43" t="s" s="2">
+      <c r="L43" t="s" s="2">
         <v>311</v>
       </c>
-      <c r="L43" t="s" s="2">
+      <c r="M43" t="s" s="2">
         <v>312</v>
       </c>
-      <c r="M43" t="s" s="2">
+      <c r="N43" t="s" s="2">
         <v>313</v>
-      </c>
-      <c r="N43" t="s" s="2">
-        <v>314</v>
       </c>
       <c r="O43" t="s" s="2">
         <v>45</v>
@@ -7024,7 +7016,7 @@
         <v>45</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>43</v>
@@ -7039,19 +7031,19 @@
         <v>67</v>
       </c>
       <c r="AJ43" t="s" s="2">
+        <v>314</v>
+      </c>
+      <c r="AK43" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL43" t="s" s="2">
         <v>315</v>
       </c>
-      <c r="AK43" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL43" t="s" s="2">
+      <c r="AM43" t="s" s="2">
         <v>316</v>
       </c>
-      <c r="AM43" t="s" s="2">
+      <c r="AN43" t="s" s="2">
         <v>317</v>
-      </c>
-      <c r="AN43" t="s" s="2">
-        <v>318</v>
       </c>
       <c r="AO43" t="s" s="2">
         <v>45</v>
@@ -7059,11 +7051,11 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" t="s" s="2">
@@ -7082,19 +7074,19 @@
         <v>56</v>
       </c>
       <c r="J44" t="s" s="2">
+        <v>320</v>
+      </c>
+      <c r="K44" t="s" s="2">
         <v>321</v>
       </c>
-      <c r="K44" t="s" s="2">
+      <c r="L44" t="s" s="2">
         <v>322</v>
       </c>
-      <c r="L44" t="s" s="2">
+      <c r="M44" t="s" s="2">
         <v>323</v>
       </c>
-      <c r="M44" t="s" s="2">
+      <c r="N44" t="s" s="2">
         <v>324</v>
-      </c>
-      <c r="N44" t="s" s="2">
-        <v>325</v>
       </c>
       <c r="O44" t="s" s="2">
         <v>45</v>
@@ -7131,17 +7123,17 @@
         <v>45</v>
       </c>
       <c r="AA44" t="s" s="2">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AB44" s="2"/>
       <c r="AC44" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AD44" t="s" s="2">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>43</v>
@@ -7150,25 +7142,25 @@
         <v>55</v>
       </c>
       <c r="AH44" t="s" s="2">
+        <v>327</v>
+      </c>
+      <c r="AI44" t="s" s="2">
         <v>328</v>
       </c>
-      <c r="AI44" t="s" s="2">
+      <c r="AJ44" t="s" s="2">
         <v>329</v>
       </c>
-      <c r="AJ44" t="s" s="2">
+      <c r="AK44" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL44" t="s" s="2">
         <v>330</v>
       </c>
-      <c r="AK44" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL44" t="s" s="2">
+      <c r="AM44" t="s" s="2">
         <v>331</v>
       </c>
-      <c r="AM44" t="s" s="2">
+      <c r="AN44" t="s" s="2">
         <v>332</v>
-      </c>
-      <c r="AN44" t="s" s="2">
-        <v>333</v>
       </c>
       <c r="AO44" t="s" s="2">
         <v>45</v>
@@ -7176,13 +7168,13 @@
     </row>
     <row r="45">
       <c r="A45" t="s" s="2">
+        <v>318</v>
+      </c>
+      <c r="B45" t="s" s="2">
+        <v>333</v>
+      </c>
+      <c r="C45" t="s" s="2">
         <v>319</v>
-      </c>
-      <c r="B45" t="s" s="2">
-        <v>334</v>
-      </c>
-      <c r="C45" t="s" s="2">
-        <v>320</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" t="s" s="2">
@@ -7201,19 +7193,19 @@
         <v>56</v>
       </c>
       <c r="J45" t="s" s="2">
+        <v>320</v>
+      </c>
+      <c r="K45" t="s" s="2">
         <v>321</v>
       </c>
-      <c r="K45" t="s" s="2">
+      <c r="L45" t="s" s="2">
         <v>322</v>
       </c>
-      <c r="L45" t="s" s="2">
+      <c r="M45" t="s" s="2">
         <v>323</v>
       </c>
-      <c r="M45" t="s" s="2">
+      <c r="N45" t="s" s="2">
         <v>324</v>
-      </c>
-      <c r="N45" t="s" s="2">
-        <v>325</v>
       </c>
       <c r="O45" t="s" s="2">
         <v>45</v>
@@ -7262,7 +7254,7 @@
         <v>45</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>43</v>
@@ -7271,25 +7263,25 @@
         <v>55</v>
       </c>
       <c r="AH45" t="s" s="2">
+        <v>327</v>
+      </c>
+      <c r="AI45" t="s" s="2">
         <v>328</v>
       </c>
-      <c r="AI45" t="s" s="2">
+      <c r="AJ45" t="s" s="2">
         <v>329</v>
       </c>
-      <c r="AJ45" t="s" s="2">
+      <c r="AK45" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL45" t="s" s="2">
         <v>330</v>
       </c>
-      <c r="AK45" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL45" t="s" s="2">
+      <c r="AM45" t="s" s="2">
         <v>331</v>
       </c>
-      <c r="AM45" t="s" s="2">
+      <c r="AN45" t="s" s="2">
         <v>332</v>
-      </c>
-      <c r="AN45" t="s" s="2">
-        <v>333</v>
       </c>
       <c r="AO45" t="s" s="2">
         <v>45</v>
@@ -7297,7 +7289,7 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -7323,13 +7315,13 @@
         <v>91</v>
       </c>
       <c r="K46" t="s" s="2">
+        <v>335</v>
+      </c>
+      <c r="L46" t="s" s="2">
         <v>336</v>
       </c>
-      <c r="L46" t="s" s="2">
+      <c r="M46" t="s" s="2">
         <v>337</v>
-      </c>
-      <c r="M46" t="s" s="2">
-        <v>338</v>
       </c>
       <c r="N46" s="2"/>
       <c r="O46" t="s" s="2">
@@ -7379,7 +7371,7 @@
         <v>45</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>43</v>
@@ -7400,13 +7392,13 @@
         <v>45</v>
       </c>
       <c r="AL46" t="s" s="2">
+        <v>338</v>
+      </c>
+      <c r="AM46" t="s" s="2">
         <v>339</v>
       </c>
-      <c r="AM46" t="s" s="2">
+      <c r="AN46" t="s" s="2">
         <v>340</v>
-      </c>
-      <c r="AN46" t="s" s="2">
-        <v>341</v>
       </c>
       <c r="AO46" t="s" s="2">
         <v>45</v>
@@ -7414,7 +7406,7 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -7437,17 +7429,17 @@
         <v>56</v>
       </c>
       <c r="J47" t="s" s="2">
+        <v>342</v>
+      </c>
+      <c r="K47" t="s" s="2">
         <v>343</v>
       </c>
-      <c r="K47" t="s" s="2">
+      <c r="L47" t="s" s="2">
         <v>344</v>
-      </c>
-      <c r="L47" t="s" s="2">
-        <v>345</v>
       </c>
       <c r="M47" s="2"/>
       <c r="N47" t="s" s="2">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="O47" t="s" s="2">
         <v>45</v>
@@ -7496,7 +7488,7 @@
         <v>45</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>43</v>
@@ -7511,19 +7503,19 @@
         <v>67</v>
       </c>
       <c r="AJ47" t="s" s="2">
+        <v>346</v>
+      </c>
+      <c r="AK47" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL47" t="s" s="2">
         <v>347</v>
       </c>
-      <c r="AK47" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL47" t="s" s="2">
+      <c r="AM47" t="s" s="2">
         <v>348</v>
       </c>
-      <c r="AM47" t="s" s="2">
+      <c r="AN47" t="s" s="2">
         <v>349</v>
-      </c>
-      <c r="AN47" t="s" s="2">
-        <v>350</v>
       </c>
       <c r="AO47" t="s" s="2">
         <v>45</v>
@@ -7531,7 +7523,7 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
@@ -7554,19 +7546,19 @@
         <v>56</v>
       </c>
       <c r="J48" t="s" s="2">
+        <v>351</v>
+      </c>
+      <c r="K48" t="s" s="2">
         <v>352</v>
       </c>
-      <c r="K48" t="s" s="2">
+      <c r="L48" t="s" s="2">
+        <v>352</v>
+      </c>
+      <c r="M48" t="s" s="2">
         <v>353</v>
       </c>
-      <c r="L48" t="s" s="2">
-        <v>353</v>
-      </c>
-      <c r="M48" t="s" s="2">
+      <c r="N48" t="s" s="2">
         <v>354</v>
-      </c>
-      <c r="N48" t="s" s="2">
-        <v>355</v>
       </c>
       <c r="O48" t="s" s="2">
         <v>45</v>
@@ -7603,17 +7595,17 @@
         <v>45</v>
       </c>
       <c r="AA48" t="s" s="2">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AB48" s="2"/>
       <c r="AC48" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AD48" t="s" s="2">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>43</v>
@@ -7622,7 +7614,7 @@
         <v>55</v>
       </c>
       <c r="AH48" t="s" s="2">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="AI48" t="s" s="2">
         <v>67</v>
@@ -7631,27 +7623,27 @@
         <v>45</v>
       </c>
       <c r="AK48" t="s" s="2">
+        <v>356</v>
+      </c>
+      <c r="AL48" t="s" s="2">
         <v>357</v>
       </c>
-      <c r="AL48" t="s" s="2">
+      <c r="AM48" t="s" s="2">
         <v>358</v>
       </c>
-      <c r="AM48" t="s" s="2">
+      <c r="AN48" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO48" t="s" s="2">
         <v>359</v>
-      </c>
-      <c r="AN48" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO48" t="s" s="2">
-        <v>360</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="2">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B49" t="s" s="2">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C49" t="s" s="2">
         <v>45</v>
@@ -7673,19 +7665,19 @@
         <v>56</v>
       </c>
       <c r="J49" t="s" s="2">
+        <v>351</v>
+      </c>
+      <c r="K49" t="s" s="2">
         <v>352</v>
       </c>
-      <c r="K49" t="s" s="2">
+      <c r="L49" t="s" s="2">
+        <v>352</v>
+      </c>
+      <c r="M49" t="s" s="2">
         <v>353</v>
       </c>
-      <c r="L49" t="s" s="2">
-        <v>353</v>
-      </c>
-      <c r="M49" t="s" s="2">
+      <c r="N49" t="s" s="2">
         <v>354</v>
-      </c>
-      <c r="N49" t="s" s="2">
-        <v>355</v>
       </c>
       <c r="O49" t="s" s="2">
         <v>45</v>
@@ -7734,7 +7726,7 @@
         <v>45</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>43</v>
@@ -7743,7 +7735,7 @@
         <v>55</v>
       </c>
       <c r="AH49" t="s" s="2">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="AI49" t="s" s="2">
         <v>67</v>
@@ -7752,24 +7744,24 @@
         <v>45</v>
       </c>
       <c r="AK49" t="s" s="2">
+        <v>356</v>
+      </c>
+      <c r="AL49" t="s" s="2">
         <v>357</v>
       </c>
-      <c r="AL49" t="s" s="2">
+      <c r="AM49" t="s" s="2">
         <v>358</v>
       </c>
-      <c r="AM49" t="s" s="2">
+      <c r="AN49" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO49" t="s" s="2">
         <v>359</v>
-      </c>
-      <c r="AN49" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO49" t="s" s="2">
-        <v>360</v>
       </c>
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
@@ -7884,7 +7876,7 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -8001,7 +7993,7 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
@@ -8024,19 +8016,19 @@
         <v>56</v>
       </c>
       <c r="J52" t="s" s="2">
+        <v>364</v>
+      </c>
+      <c r="K52" t="s" s="2">
         <v>365</v>
       </c>
-      <c r="K52" t="s" s="2">
+      <c r="L52" t="s" s="2">
         <v>366</v>
       </c>
-      <c r="L52" t="s" s="2">
+      <c r="M52" t="s" s="2">
         <v>367</v>
       </c>
-      <c r="M52" t="s" s="2">
+      <c r="N52" t="s" s="2">
         <v>368</v>
-      </c>
-      <c r="N52" t="s" s="2">
-        <v>369</v>
       </c>
       <c r="O52" t="s" s="2">
         <v>45</v>
@@ -8085,7 +8077,7 @@
         <v>45</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>43</v>
@@ -8106,10 +8098,10 @@
         <v>45</v>
       </c>
       <c r="AL52" t="s" s="2">
+        <v>370</v>
+      </c>
+      <c r="AM52" t="s" s="2">
         <v>371</v>
-      </c>
-      <c r="AM52" t="s" s="2">
-        <v>372</v>
       </c>
       <c r="AN52" t="s" s="2">
         <v>45</v>
@@ -8120,7 +8112,7 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
@@ -8146,20 +8138,20 @@
         <v>132</v>
       </c>
       <c r="K53" t="s" s="2">
+        <v>373</v>
+      </c>
+      <c r="L53" t="s" s="2">
         <v>374</v>
-      </c>
-      <c r="L53" t="s" s="2">
-        <v>375</v>
       </c>
       <c r="M53" s="2"/>
       <c r="N53" t="s" s="2">
+        <v>375</v>
+      </c>
+      <c r="O53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="P53" t="s" s="2">
         <v>376</v>
-      </c>
-      <c r="O53" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="P53" t="s" s="2">
-        <v>377</v>
       </c>
       <c r="Q53" t="s" s="2">
         <v>45</v>
@@ -8183,28 +8175,28 @@
         <v>194</v>
       </c>
       <c r="X53" t="s" s="2">
+        <v>377</v>
+      </c>
+      <c r="Y53" t="s" s="2">
         <v>378</v>
       </c>
-      <c r="Y53" t="s" s="2">
+      <c r="Z53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE53" t="s" s="2">
         <v>379</v>
-      </c>
-      <c r="Z53" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AA53" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AB53" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AC53" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AD53" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AE53" t="s" s="2">
-        <v>380</v>
       </c>
       <c r="AF53" t="s" s="2">
         <v>43</v>
@@ -8225,10 +8217,10 @@
         <v>45</v>
       </c>
       <c r="AL53" t="s" s="2">
+        <v>380</v>
+      </c>
+      <c r="AM53" t="s" s="2">
         <v>381</v>
-      </c>
-      <c r="AM53" t="s" s="2">
-        <v>382</v>
       </c>
       <c r="AN53" t="s" s="2">
         <v>45</v>
@@ -8239,7 +8231,7 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
@@ -8265,14 +8257,14 @@
         <v>57</v>
       </c>
       <c r="K54" t="s" s="2">
+        <v>383</v>
+      </c>
+      <c r="L54" t="s" s="2">
         <v>384</v>
-      </c>
-      <c r="L54" t="s" s="2">
-        <v>385</v>
       </c>
       <c r="M54" s="2"/>
       <c r="N54" t="s" s="2">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="O54" t="s" s="2">
         <v>45</v>
@@ -8282,46 +8274,46 @@
         <v>45</v>
       </c>
       <c r="R54" t="s" s="2">
+        <v>386</v>
+      </c>
+      <c r="S54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="T54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="U54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="V54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="W54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="X54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Y54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Z54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE54" t="s" s="2">
         <v>387</v>
-      </c>
-      <c r="S54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="T54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="U54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="V54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="W54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="X54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="Y54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="Z54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AA54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AB54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AC54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AD54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AE54" t="s" s="2">
-        <v>388</v>
       </c>
       <c r="AF54" t="s" s="2">
         <v>43</v>
@@ -8342,10 +8334,10 @@
         <v>45</v>
       </c>
       <c r="AL54" t="s" s="2">
+        <v>388</v>
+      </c>
+      <c r="AM54" t="s" s="2">
         <v>389</v>
-      </c>
-      <c r="AM54" t="s" s="2">
-        <v>390</v>
       </c>
       <c r="AN54" t="s" s="2">
         <v>45</v>
@@ -8356,7 +8348,7 @@
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" t="s" s="2">
@@ -8382,14 +8374,14 @@
         <v>97</v>
       </c>
       <c r="K55" t="s" s="2">
+        <v>391</v>
+      </c>
+      <c r="L55" t="s" s="2">
         <v>392</v>
-      </c>
-      <c r="L55" t="s" s="2">
-        <v>393</v>
       </c>
       <c r="M55" s="2"/>
       <c r="N55" t="s" s="2">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="O55" t="s" s="2">
         <v>45</v>
@@ -8438,7 +8430,7 @@
         <v>45</v>
       </c>
       <c r="AE55" t="s" s="2">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="AF55" t="s" s="2">
         <v>43</v>
@@ -8447,7 +8439,7 @@
         <v>55</v>
       </c>
       <c r="AH55" t="s" s="2">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="AI55" t="s" s="2">
         <v>67</v>
@@ -8459,10 +8451,10 @@
         <v>45</v>
       </c>
       <c r="AL55" t="s" s="2">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="AM55" t="s" s="2">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="AN55" t="s" s="2">
         <v>45</v>
@@ -8473,7 +8465,7 @@
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
@@ -8499,16 +8491,16 @@
         <v>132</v>
       </c>
       <c r="K56" t="s" s="2">
+        <v>398</v>
+      </c>
+      <c r="L56" t="s" s="2">
         <v>399</v>
       </c>
-      <c r="L56" t="s" s="2">
+      <c r="M56" t="s" s="2">
         <v>400</v>
       </c>
-      <c r="M56" t="s" s="2">
+      <c r="N56" t="s" s="2">
         <v>401</v>
-      </c>
-      <c r="N56" t="s" s="2">
-        <v>402</v>
       </c>
       <c r="O56" t="s" s="2">
         <v>45</v>
@@ -8557,7 +8549,7 @@
         <v>45</v>
       </c>
       <c r="AE56" t="s" s="2">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="AF56" t="s" s="2">
         <v>43</v>
@@ -8578,10 +8570,10 @@
         <v>45</v>
       </c>
       <c r="AL56" t="s" s="2">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="AM56" t="s" s="2">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="AN56" t="s" s="2">
         <v>45</v>
@@ -8592,7 +8584,7 @@
     </row>
     <row r="57">
       <c r="A57" t="s" s="2">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
@@ -8618,16 +8610,16 @@
         <v>202</v>
       </c>
       <c r="K57" t="s" s="2">
+        <v>405</v>
+      </c>
+      <c r="L57" t="s" s="2">
         <v>406</v>
       </c>
-      <c r="L57" t="s" s="2">
+      <c r="M57" t="s" s="2">
         <v>407</v>
       </c>
-      <c r="M57" t="s" s="2">
+      <c r="N57" t="s" s="2">
         <v>408</v>
-      </c>
-      <c r="N57" t="s" s="2">
-        <v>409</v>
       </c>
       <c r="O57" t="s" s="2">
         <v>45</v>
@@ -8655,11 +8647,11 @@
         <v>113</v>
       </c>
       <c r="X57" t="s" s="2">
+        <v>409</v>
+      </c>
+      <c r="Y57" t="s" s="2">
         <v>410</v>
       </c>
-      <c r="Y57" t="s" s="2">
-        <v>411</v>
-      </c>
       <c r="Z57" t="s" s="2">
         <v>45</v>
       </c>
@@ -8676,7 +8668,7 @@
         <v>45</v>
       </c>
       <c r="AE57" t="s" s="2">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="AF57" t="s" s="2">
         <v>43</v>
@@ -8685,7 +8677,7 @@
         <v>55</v>
       </c>
       <c r="AH57" t="s" s="2">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="AI57" t="s" s="2">
         <v>67</v>
@@ -8700,7 +8692,7 @@
         <v>155</v>
       </c>
       <c r="AM57" t="s" s="2">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="AN57" t="s" s="2">
         <v>45</v>
@@ -8711,11 +8703,11 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D58" s="2"/>
       <c r="E58" t="s" s="2">
@@ -8737,16 +8729,16 @@
         <v>202</v>
       </c>
       <c r="K58" t="s" s="2">
+        <v>415</v>
+      </c>
+      <c r="L58" t="s" s="2">
         <v>416</v>
       </c>
-      <c r="L58" t="s" s="2">
+      <c r="M58" t="s" s="2">
         <v>417</v>
       </c>
-      <c r="M58" t="s" s="2">
+      <c r="N58" t="s" s="2">
         <v>418</v>
-      </c>
-      <c r="N58" t="s" s="2">
-        <v>419</v>
       </c>
       <c r="O58" t="s" s="2">
         <v>45</v>
@@ -8774,11 +8766,11 @@
         <v>113</v>
       </c>
       <c r="X58" t="s" s="2">
+        <v>419</v>
+      </c>
+      <c r="Y58" t="s" s="2">
         <v>420</v>
       </c>
-      <c r="Y58" t="s" s="2">
-        <v>421</v>
-      </c>
       <c r="Z58" t="s" s="2">
         <v>45</v>
       </c>
@@ -8795,7 +8787,7 @@
         <v>45</v>
       </c>
       <c r="AE58" t="s" s="2">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="AF58" t="s" s="2">
         <v>43</v>
@@ -8813,24 +8805,24 @@
         <v>45</v>
       </c>
       <c r="AK58" t="s" s="2">
+        <v>421</v>
+      </c>
+      <c r="AL58" t="s" s="2">
         <v>422</v>
       </c>
-      <c r="AL58" t="s" s="2">
+      <c r="AM58" t="s" s="2">
         <v>423</v>
       </c>
-      <c r="AM58" t="s" s="2">
+      <c r="AN58" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO58" t="s" s="2">
         <v>424</v>
-      </c>
-      <c r="AN58" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO58" t="s" s="2">
-        <v>425</v>
       </c>
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
@@ -8853,19 +8845,19 @@
         <v>45</v>
       </c>
       <c r="J59" t="s" s="2">
+        <v>426</v>
+      </c>
+      <c r="K59" t="s" s="2">
         <v>427</v>
       </c>
-      <c r="K59" t="s" s="2">
+      <c r="L59" t="s" s="2">
         <v>428</v>
       </c>
-      <c r="L59" t="s" s="2">
+      <c r="M59" t="s" s="2">
         <v>429</v>
       </c>
-      <c r="M59" t="s" s="2">
+      <c r="N59" t="s" s="2">
         <v>430</v>
-      </c>
-      <c r="N59" t="s" s="2">
-        <v>431</v>
       </c>
       <c r="O59" t="s" s="2">
         <v>45</v>
@@ -8914,7 +8906,7 @@
         <v>45</v>
       </c>
       <c r="AE59" t="s" s="2">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="AF59" t="s" s="2">
         <v>43</v>
@@ -8935,10 +8927,10 @@
         <v>45</v>
       </c>
       <c r="AL59" t="s" s="2">
+        <v>431</v>
+      </c>
+      <c r="AM59" t="s" s="2">
         <v>432</v>
-      </c>
-      <c r="AM59" t="s" s="2">
-        <v>433</v>
       </c>
       <c r="AN59" t="s" s="2">
         <v>45</v>
@@ -8949,7 +8941,7 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
@@ -8975,13 +8967,13 @@
         <v>202</v>
       </c>
       <c r="K60" t="s" s="2">
+        <v>434</v>
+      </c>
+      <c r="L60" t="s" s="2">
         <v>435</v>
       </c>
-      <c r="L60" t="s" s="2">
+      <c r="M60" t="s" s="2">
         <v>436</v>
-      </c>
-      <c r="M60" t="s" s="2">
-        <v>437</v>
       </c>
       <c r="N60" s="2"/>
       <c r="O60" t="s" s="2">
@@ -9010,11 +9002,11 @@
         <v>122</v>
       </c>
       <c r="X60" t="s" s="2">
+        <v>437</v>
+      </c>
+      <c r="Y60" t="s" s="2">
         <v>438</v>
       </c>
-      <c r="Y60" t="s" s="2">
-        <v>439</v>
-      </c>
       <c r="Z60" t="s" s="2">
         <v>45</v>
       </c>
@@ -9031,7 +9023,7 @@
         <v>45</v>
       </c>
       <c r="AE60" t="s" s="2">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="AF60" t="s" s="2">
         <v>43</v>
@@ -9049,24 +9041,24 @@
         <v>45</v>
       </c>
       <c r="AK60" t="s" s="2">
+        <v>439</v>
+      </c>
+      <c r="AL60" t="s" s="2">
         <v>440</v>
       </c>
-      <c r="AL60" t="s" s="2">
+      <c r="AM60" t="s" s="2">
         <v>441</v>
       </c>
-      <c r="AM60" t="s" s="2">
+      <c r="AN60" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO60" t="s" s="2">
         <v>442</v>
-      </c>
-      <c r="AN60" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO60" t="s" s="2">
-        <v>443</v>
       </c>
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
@@ -9092,16 +9084,16 @@
         <v>202</v>
       </c>
       <c r="K61" t="s" s="2">
+        <v>444</v>
+      </c>
+      <c r="L61" t="s" s="2">
         <v>445</v>
       </c>
-      <c r="L61" t="s" s="2">
+      <c r="M61" t="s" s="2">
         <v>446</v>
       </c>
-      <c r="M61" t="s" s="2">
+      <c r="N61" t="s" s="2">
         <v>447</v>
-      </c>
-      <c r="N61" t="s" s="2">
-        <v>448</v>
       </c>
       <c r="O61" t="s" s="2">
         <v>45</v>
@@ -9129,11 +9121,11 @@
         <v>122</v>
       </c>
       <c r="X61" t="s" s="2">
+        <v>448</v>
+      </c>
+      <c r="Y61" t="s" s="2">
         <v>449</v>
       </c>
-      <c r="Y61" t="s" s="2">
-        <v>450</v>
-      </c>
       <c r="Z61" t="s" s="2">
         <v>45</v>
       </c>
@@ -9150,7 +9142,7 @@
         <v>45</v>
       </c>
       <c r="AE61" t="s" s="2">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="AF61" t="s" s="2">
         <v>43</v>
@@ -9171,10 +9163,10 @@
         <v>45</v>
       </c>
       <c r="AL61" t="s" s="2">
+        <v>450</v>
+      </c>
+      <c r="AM61" t="s" s="2">
         <v>451</v>
-      </c>
-      <c r="AM61" t="s" s="2">
-        <v>452</v>
       </c>
       <c r="AN61" t="s" s="2">
         <v>45</v>
@@ -9185,7 +9177,7 @@
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
@@ -9208,16 +9200,16 @@
         <v>45</v>
       </c>
       <c r="J62" t="s" s="2">
+        <v>453</v>
+      </c>
+      <c r="K62" t="s" s="2">
         <v>454</v>
       </c>
-      <c r="K62" t="s" s="2">
+      <c r="L62" t="s" s="2">
         <v>455</v>
       </c>
-      <c r="L62" t="s" s="2">
+      <c r="M62" t="s" s="2">
         <v>456</v>
-      </c>
-      <c r="M62" t="s" s="2">
-        <v>457</v>
       </c>
       <c r="N62" s="2"/>
       <c r="O62" t="s" s="2">
@@ -9267,7 +9259,7 @@
         <v>45</v>
       </c>
       <c r="AE62" t="s" s="2">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="AF62" t="s" s="2">
         <v>43</v>
@@ -9285,24 +9277,24 @@
         <v>45</v>
       </c>
       <c r="AK62" t="s" s="2">
+        <v>457</v>
+      </c>
+      <c r="AL62" t="s" s="2">
         <v>458</v>
       </c>
-      <c r="AL62" t="s" s="2">
+      <c r="AM62" t="s" s="2">
         <v>459</v>
       </c>
-      <c r="AM62" t="s" s="2">
+      <c r="AN62" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO62" t="s" s="2">
         <v>460</v>
-      </c>
-      <c r="AN62" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO62" t="s" s="2">
-        <v>461</v>
       </c>
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" t="s" s="2">
@@ -9325,16 +9317,16 @@
         <v>45</v>
       </c>
       <c r="J63" t="s" s="2">
+        <v>462</v>
+      </c>
+      <c r="K63" t="s" s="2">
         <v>463</v>
       </c>
-      <c r="K63" t="s" s="2">
+      <c r="L63" t="s" s="2">
         <v>464</v>
       </c>
-      <c r="L63" t="s" s="2">
+      <c r="M63" t="s" s="2">
         <v>465</v>
-      </c>
-      <c r="M63" t="s" s="2">
-        <v>466</v>
       </c>
       <c r="N63" s="2"/>
       <c r="O63" t="s" s="2">
@@ -9384,7 +9376,7 @@
         <v>45</v>
       </c>
       <c r="AE63" t="s" s="2">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="AF63" t="s" s="2">
         <v>43</v>
@@ -9402,24 +9394,24 @@
         <v>45</v>
       </c>
       <c r="AK63" t="s" s="2">
+        <v>466</v>
+      </c>
+      <c r="AL63" t="s" s="2">
         <v>467</v>
       </c>
-      <c r="AL63" t="s" s="2">
+      <c r="AM63" t="s" s="2">
         <v>468</v>
       </c>
-      <c r="AM63" t="s" s="2">
+      <c r="AN63" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO63" t="s" s="2">
         <v>469</v>
-      </c>
-      <c r="AN63" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO63" t="s" s="2">
-        <v>470</v>
       </c>
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" t="s" s="2">
@@ -9442,19 +9434,19 @@
         <v>45</v>
       </c>
       <c r="J64" t="s" s="2">
+        <v>471</v>
+      </c>
+      <c r="K64" t="s" s="2">
         <v>472</v>
       </c>
-      <c r="K64" t="s" s="2">
+      <c r="L64" t="s" s="2">
         <v>473</v>
       </c>
-      <c r="L64" t="s" s="2">
+      <c r="M64" t="s" s="2">
         <v>474</v>
       </c>
-      <c r="M64" t="s" s="2">
+      <c r="N64" t="s" s="2">
         <v>475</v>
-      </c>
-      <c r="N64" t="s" s="2">
-        <v>476</v>
       </c>
       <c r="O64" t="s" s="2">
         <v>45</v>
@@ -9503,7 +9495,7 @@
         <v>45</v>
       </c>
       <c r="AE64" t="s" s="2">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="AF64" t="s" s="2">
         <v>43</v>
@@ -9515,19 +9507,19 @@
         <v>45</v>
       </c>
       <c r="AI64" t="s" s="2">
+        <v>476</v>
+      </c>
+      <c r="AJ64" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK64" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL64" t="s" s="2">
         <v>477</v>
       </c>
-      <c r="AJ64" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK64" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL64" t="s" s="2">
+      <c r="AM64" t="s" s="2">
         <v>478</v>
-      </c>
-      <c r="AM64" t="s" s="2">
-        <v>479</v>
       </c>
       <c r="AN64" t="s" s="2">
         <v>45</v>
@@ -9538,7 +9530,7 @@
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" t="s" s="2">
@@ -9653,7 +9645,7 @@
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" t="s" s="2">
@@ -9770,11 +9762,11 @@
     </row>
     <row r="67" hidden="true">
       <c r="A67" t="s" s="2">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" t="s" s="2">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="D67" s="2"/>
       <c r="E67" t="s" s="2">
@@ -9796,16 +9788,16 @@
         <v>75</v>
       </c>
       <c r="K67" t="s" s="2">
+        <v>483</v>
+      </c>
+      <c r="L67" t="s" s="2">
         <v>484</v>
-      </c>
-      <c r="L67" t="s" s="2">
-        <v>485</v>
       </c>
       <c r="M67" t="s" s="2">
         <v>78</v>
       </c>
       <c r="N67" t="s" s="2">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="O67" t="s" s="2">
         <v>45</v>
@@ -9854,7 +9846,7 @@
         <v>45</v>
       </c>
       <c r="AE67" t="s" s="2">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="AF67" t="s" s="2">
         <v>43</v>
@@ -9889,7 +9881,7 @@
     </row>
     <row r="68" hidden="true">
       <c r="A68" t="s" s="2">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B68" s="2"/>
       <c r="C68" t="s" s="2">
@@ -9912,13 +9904,13 @@
         <v>45</v>
       </c>
       <c r="J68" t="s" s="2">
+        <v>488</v>
+      </c>
+      <c r="K68" t="s" s="2">
         <v>489</v>
       </c>
-      <c r="K68" t="s" s="2">
+      <c r="L68" t="s" s="2">
         <v>490</v>
-      </c>
-      <c r="L68" t="s" s="2">
-        <v>491</v>
       </c>
       <c r="M68" s="2"/>
       <c r="N68" s="2"/>
@@ -9969,7 +9961,7 @@
         <v>45</v>
       </c>
       <c r="AE68" t="s" s="2">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="AF68" t="s" s="2">
         <v>43</v>
@@ -9978,7 +9970,7 @@
         <v>55</v>
       </c>
       <c r="AH68" t="s" s="2">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="AI68" t="s" s="2">
         <v>67</v>
@@ -9990,10 +9982,10 @@
         <v>45</v>
       </c>
       <c r="AL68" t="s" s="2">
+        <v>492</v>
+      </c>
+      <c r="AM68" t="s" s="2">
         <v>493</v>
-      </c>
-      <c r="AM68" t="s" s="2">
-        <v>494</v>
       </c>
       <c r="AN68" t="s" s="2">
         <v>45</v>
@@ -10004,7 +9996,7 @@
     </row>
     <row r="69" hidden="true">
       <c r="A69" t="s" s="2">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" t="s" s="2">
@@ -10027,13 +10019,13 @@
         <v>45</v>
       </c>
       <c r="J69" t="s" s="2">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="K69" t="s" s="2">
+        <v>495</v>
+      </c>
+      <c r="L69" t="s" s="2">
         <v>496</v>
-      </c>
-      <c r="L69" t="s" s="2">
-        <v>497</v>
       </c>
       <c r="M69" s="2"/>
       <c r="N69" s="2"/>
@@ -10084,7 +10076,7 @@
         <v>45</v>
       </c>
       <c r="AE69" t="s" s="2">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="AF69" t="s" s="2">
         <v>43</v>
@@ -10093,7 +10085,7 @@
         <v>55</v>
       </c>
       <c r="AH69" t="s" s="2">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="AI69" t="s" s="2">
         <v>67</v>
@@ -10105,10 +10097,10 @@
         <v>45</v>
       </c>
       <c r="AL69" t="s" s="2">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="AM69" t="s" s="2">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="AN69" t="s" s="2">
         <v>45</v>
@@ -10119,7 +10111,7 @@
     </row>
     <row r="70" hidden="true">
       <c r="A70" t="s" s="2">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" t="s" s="2">
@@ -10145,16 +10137,16 @@
         <v>202</v>
       </c>
       <c r="K70" t="s" s="2">
+        <v>499</v>
+      </c>
+      <c r="L70" t="s" s="2">
         <v>500</v>
       </c>
-      <c r="L70" t="s" s="2">
+      <c r="M70" t="s" s="2">
         <v>501</v>
       </c>
-      <c r="M70" t="s" s="2">
+      <c r="N70" t="s" s="2">
         <v>502</v>
-      </c>
-      <c r="N70" t="s" s="2">
-        <v>503</v>
       </c>
       <c r="O70" t="s" s="2">
         <v>45</v>
@@ -10182,11 +10174,11 @@
         <v>136</v>
       </c>
       <c r="X70" t="s" s="2">
+        <v>503</v>
+      </c>
+      <c r="Y70" t="s" s="2">
         <v>504</v>
       </c>
-      <c r="Y70" t="s" s="2">
-        <v>505</v>
-      </c>
       <c r="Z70" t="s" s="2">
         <v>45</v>
       </c>
@@ -10203,7 +10195,7 @@
         <v>45</v>
       </c>
       <c r="AE70" t="s" s="2">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="AF70" t="s" s="2">
         <v>43</v>
@@ -10221,13 +10213,13 @@
         <v>45</v>
       </c>
       <c r="AK70" t="s" s="2">
+        <v>505</v>
+      </c>
+      <c r="AL70" t="s" s="2">
         <v>506</v>
       </c>
-      <c r="AL70" t="s" s="2">
-        <v>507</v>
-      </c>
       <c r="AM70" t="s" s="2">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="AN70" t="s" s="2">
         <v>45</v>
@@ -10238,7 +10230,7 @@
     </row>
     <row r="71" hidden="true">
       <c r="A71" t="s" s="2">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B71" s="2"/>
       <c r="C71" t="s" s="2">
@@ -10264,16 +10256,16 @@
         <v>202</v>
       </c>
       <c r="K71" t="s" s="2">
+        <v>508</v>
+      </c>
+      <c r="L71" t="s" s="2">
         <v>509</v>
       </c>
-      <c r="L71" t="s" s="2">
+      <c r="M71" t="s" s="2">
         <v>510</v>
       </c>
-      <c r="M71" t="s" s="2">
+      <c r="N71" t="s" s="2">
         <v>511</v>
-      </c>
-      <c r="N71" t="s" s="2">
-        <v>512</v>
       </c>
       <c r="O71" t="s" s="2">
         <v>45</v>
@@ -10301,11 +10293,11 @@
         <v>122</v>
       </c>
       <c r="X71" t="s" s="2">
+        <v>512</v>
+      </c>
+      <c r="Y71" t="s" s="2">
         <v>513</v>
       </c>
-      <c r="Y71" t="s" s="2">
-        <v>514</v>
-      </c>
       <c r="Z71" t="s" s="2">
         <v>45</v>
       </c>
@@ -10322,7 +10314,7 @@
         <v>45</v>
       </c>
       <c r="AE71" t="s" s="2">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="AF71" t="s" s="2">
         <v>43</v>
@@ -10340,13 +10332,13 @@
         <v>45</v>
       </c>
       <c r="AK71" t="s" s="2">
+        <v>505</v>
+      </c>
+      <c r="AL71" t="s" s="2">
         <v>506</v>
       </c>
-      <c r="AL71" t="s" s="2">
-        <v>507</v>
-      </c>
       <c r="AM71" t="s" s="2">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="AN71" t="s" s="2">
         <v>45</v>
@@ -10357,7 +10349,7 @@
     </row>
     <row r="72" hidden="true">
       <c r="A72" t="s" s="2">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" t="s" s="2">
@@ -10380,17 +10372,17 @@
         <v>45</v>
       </c>
       <c r="J72" t="s" s="2">
+        <v>515</v>
+      </c>
+      <c r="K72" t="s" s="2">
         <v>516</v>
       </c>
-      <c r="K72" t="s" s="2">
+      <c r="L72" t="s" s="2">
         <v>517</v>
-      </c>
-      <c r="L72" t="s" s="2">
-        <v>518</v>
       </c>
       <c r="M72" s="2"/>
       <c r="N72" t="s" s="2">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="O72" t="s" s="2">
         <v>45</v>
@@ -10439,7 +10431,7 @@
         <v>45</v>
       </c>
       <c r="AE72" t="s" s="2">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="AF72" t="s" s="2">
         <v>43</v>
@@ -10463,7 +10455,7 @@
         <v>45</v>
       </c>
       <c r="AM72" t="s" s="2">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="AN72" t="s" s="2">
         <v>45</v>
@@ -10474,7 +10466,7 @@
     </row>
     <row r="73" hidden="true">
       <c r="A73" t="s" s="2">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" t="s" s="2">
@@ -10500,10 +10492,10 @@
         <v>57</v>
       </c>
       <c r="K73" t="s" s="2">
+        <v>521</v>
+      </c>
+      <c r="L73" t="s" s="2">
         <v>522</v>
-      </c>
-      <c r="L73" t="s" s="2">
-        <v>523</v>
       </c>
       <c r="M73" s="2"/>
       <c r="N73" s="2"/>
@@ -10554,7 +10546,7 @@
         <v>45</v>
       </c>
       <c r="AE73" t="s" s="2">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="AF73" t="s" s="2">
         <v>43</v>
@@ -10575,10 +10567,10 @@
         <v>45</v>
       </c>
       <c r="AL73" t="s" s="2">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="AM73" t="s" s="2">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="AN73" t="s" s="2">
         <v>45</v>
@@ -10589,7 +10581,7 @@
     </row>
     <row r="74" hidden="true">
       <c r="A74" t="s" s="2">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B74" s="2"/>
       <c r="C74" t="s" s="2">
@@ -10612,16 +10604,16 @@
         <v>56</v>
       </c>
       <c r="J74" t="s" s="2">
+        <v>525</v>
+      </c>
+      <c r="K74" t="s" s="2">
         <v>526</v>
       </c>
-      <c r="K74" t="s" s="2">
+      <c r="L74" t="s" s="2">
         <v>527</v>
       </c>
-      <c r="L74" t="s" s="2">
+      <c r="M74" t="s" s="2">
         <v>528</v>
-      </c>
-      <c r="M74" t="s" s="2">
-        <v>529</v>
       </c>
       <c r="N74" s="2"/>
       <c r="O74" t="s" s="2">
@@ -10671,7 +10663,7 @@
         <v>45</v>
       </c>
       <c r="AE74" t="s" s="2">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="AF74" t="s" s="2">
         <v>43</v>
@@ -10692,10 +10684,10 @@
         <v>45</v>
       </c>
       <c r="AL74" t="s" s="2">
+        <v>529</v>
+      </c>
+      <c r="AM74" t="s" s="2">
         <v>530</v>
-      </c>
-      <c r="AM74" t="s" s="2">
-        <v>531</v>
       </c>
       <c r="AN74" t="s" s="2">
         <v>45</v>
@@ -10706,7 +10698,7 @@
     </row>
     <row r="75" hidden="true">
       <c r="A75" t="s" s="2">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B75" s="2"/>
       <c r="C75" t="s" s="2">
@@ -10729,16 +10721,16 @@
         <v>56</v>
       </c>
       <c r="J75" t="s" s="2">
+        <v>532</v>
+      </c>
+      <c r="K75" t="s" s="2">
         <v>533</v>
       </c>
-      <c r="K75" t="s" s="2">
+      <c r="L75" t="s" s="2">
         <v>534</v>
       </c>
-      <c r="L75" t="s" s="2">
+      <c r="M75" t="s" s="2">
         <v>535</v>
-      </c>
-      <c r="M75" t="s" s="2">
-        <v>536</v>
       </c>
       <c r="N75" s="2"/>
       <c r="O75" t="s" s="2">
@@ -10788,7 +10780,7 @@
         <v>45</v>
       </c>
       <c r="AE75" t="s" s="2">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="AF75" t="s" s="2">
         <v>43</v>
@@ -10809,10 +10801,10 @@
         <v>45</v>
       </c>
       <c r="AL75" t="s" s="2">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="AM75" t="s" s="2">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="AN75" t="s" s="2">
         <v>45</v>
@@ -10823,7 +10815,7 @@
     </row>
     <row r="76">
       <c r="A76" t="s" s="2">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B76" s="2"/>
       <c r="C76" t="s" s="2">
@@ -10846,19 +10838,19 @@
         <v>56</v>
       </c>
       <c r="J76" t="s" s="2">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="K76" t="s" s="2">
+        <v>538</v>
+      </c>
+      <c r="L76" t="s" s="2">
+        <v>538</v>
+      </c>
+      <c r="M76" t="s" s="2">
         <v>539</v>
       </c>
-      <c r="L76" t="s" s="2">
-        <v>539</v>
-      </c>
-      <c r="M76" t="s" s="2">
+      <c r="N76" t="s" s="2">
         <v>540</v>
-      </c>
-      <c r="N76" t="s" s="2">
-        <v>541</v>
       </c>
       <c r="O76" t="s" s="2">
         <v>45</v>
@@ -10907,7 +10899,7 @@
         <v>45</v>
       </c>
       <c r="AE76" t="s" s="2">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="AF76" t="s" s="2">
         <v>43</v>
@@ -10919,19 +10911,19 @@
         <v>45</v>
       </c>
       <c r="AI76" t="s" s="2">
+        <v>541</v>
+      </c>
+      <c r="AJ76" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK76" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL76" t="s" s="2">
         <v>542</v>
       </c>
-      <c r="AJ76" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK76" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL76" t="s" s="2">
+      <c r="AM76" t="s" s="2">
         <v>543</v>
-      </c>
-      <c r="AM76" t="s" s="2">
-        <v>544</v>
       </c>
       <c r="AN76" t="s" s="2">
         <v>45</v>
@@ -10942,7 +10934,7 @@
     </row>
     <row r="77" hidden="true">
       <c r="A77" t="s" s="2">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B77" s="2"/>
       <c r="C77" t="s" s="2">
@@ -11057,7 +11049,7 @@
     </row>
     <row r="78" hidden="true">
       <c r="A78" t="s" s="2">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B78" s="2"/>
       <c r="C78" t="s" s="2">
@@ -11174,11 +11166,11 @@
     </row>
     <row r="79" hidden="true">
       <c r="A79" t="s" s="2">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B79" s="2"/>
       <c r="C79" t="s" s="2">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="D79" s="2"/>
       <c r="E79" t="s" s="2">
@@ -11200,16 +11192,16 @@
         <v>75</v>
       </c>
       <c r="K79" t="s" s="2">
+        <v>483</v>
+      </c>
+      <c r="L79" t="s" s="2">
         <v>484</v>
-      </c>
-      <c r="L79" t="s" s="2">
-        <v>485</v>
       </c>
       <c r="M79" t="s" s="2">
         <v>78</v>
       </c>
       <c r="N79" t="s" s="2">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="O79" t="s" s="2">
         <v>45</v>
@@ -11258,7 +11250,7 @@
         <v>45</v>
       </c>
       <c r="AE79" t="s" s="2">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="AF79" t="s" s="2">
         <v>43</v>
@@ -11293,7 +11285,7 @@
     </row>
     <row r="80">
       <c r="A80" t="s" s="2">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" t="s" s="2">
@@ -11319,16 +11311,16 @@
         <v>202</v>
       </c>
       <c r="K80" t="s" s="2">
+        <v>548</v>
+      </c>
+      <c r="L80" t="s" s="2">
         <v>549</v>
       </c>
-      <c r="L80" t="s" s="2">
+      <c r="M80" t="s" s="2">
         <v>550</v>
       </c>
-      <c r="M80" t="s" s="2">
+      <c r="N80" t="s" s="2">
         <v>551</v>
-      </c>
-      <c r="N80" t="s" s="2">
-        <v>552</v>
       </c>
       <c r="O80" t="s" s="2">
         <v>45</v>
@@ -11356,11 +11348,11 @@
         <v>113</v>
       </c>
       <c r="X80" t="s" s="2">
+        <v>279</v>
+      </c>
+      <c r="Y80" t="s" s="2">
         <v>280</v>
       </c>
-      <c r="Y80" t="s" s="2">
-        <v>281</v>
-      </c>
       <c r="Z80" t="s" s="2">
         <v>45</v>
       </c>
@@ -11377,7 +11369,7 @@
         <v>45</v>
       </c>
       <c r="AE80" t="s" s="2">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="AF80" t="s" s="2">
         <v>55</v>
@@ -11395,16 +11387,16 @@
         <v>45</v>
       </c>
       <c r="AK80" t="s" s="2">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="AL80" t="s" s="2">
+        <v>283</v>
+      </c>
+      <c r="AM80" t="s" s="2">
         <v>284</v>
       </c>
-      <c r="AM80" t="s" s="2">
+      <c r="AN80" t="s" s="2">
         <v>285</v>
-      </c>
-      <c r="AN80" t="s" s="2">
-        <v>286</v>
       </c>
       <c r="AO80" t="s" s="2">
         <v>45</v>
@@ -11412,7 +11404,7 @@
     </row>
     <row r="81">
       <c r="A81" t="s" s="2">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B81" s="2"/>
       <c r="C81" t="s" s="2">
@@ -11435,19 +11427,19 @@
         <v>56</v>
       </c>
       <c r="J81" t="s" s="2">
+        <v>554</v>
+      </c>
+      <c r="K81" t="s" s="2">
         <v>555</v>
       </c>
-      <c r="K81" t="s" s="2">
+      <c r="L81" t="s" s="2">
         <v>556</v>
       </c>
-      <c r="L81" t="s" s="2">
+      <c r="M81" t="s" s="2">
         <v>557</v>
       </c>
-      <c r="M81" t="s" s="2">
-        <v>558</v>
-      </c>
       <c r="N81" t="s" s="2">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="O81" t="s" s="2">
         <v>45</v>
@@ -11475,11 +11467,11 @@
         <v>194</v>
       </c>
       <c r="X81" t="s" s="2">
+        <v>558</v>
+      </c>
+      <c r="Y81" t="s" s="2">
         <v>559</v>
       </c>
-      <c r="Y81" t="s" s="2">
-        <v>560</v>
-      </c>
       <c r="Z81" t="s" s="2">
         <v>45</v>
       </c>
@@ -11496,7 +11488,7 @@
         <v>45</v>
       </c>
       <c r="AE81" t="s" s="2">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="AF81" t="s" s="2">
         <v>43</v>
@@ -11505,7 +11497,7 @@
         <v>55</v>
       </c>
       <c r="AH81" t="s" s="2">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="AI81" t="s" s="2">
         <v>67</v>
@@ -11514,24 +11506,24 @@
         <v>45</v>
       </c>
       <c r="AK81" t="s" s="2">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="AL81" t="s" s="2">
+        <v>357</v>
+      </c>
+      <c r="AM81" t="s" s="2">
         <v>358</v>
       </c>
-      <c r="AM81" t="s" s="2">
+      <c r="AN81" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO81" t="s" s="2">
         <v>359</v>
-      </c>
-      <c r="AN81" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO81" t="s" s="2">
-        <v>360</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s" s="2">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B82" s="2"/>
       <c r="C82" t="s" s="2">
@@ -11557,16 +11549,16 @@
         <v>202</v>
       </c>
       <c r="K82" t="s" s="2">
+        <v>563</v>
+      </c>
+      <c r="L82" t="s" s="2">
         <v>564</v>
       </c>
-      <c r="L82" t="s" s="2">
+      <c r="M82" t="s" s="2">
         <v>565</v>
       </c>
-      <c r="M82" t="s" s="2">
-        <v>566</v>
-      </c>
       <c r="N82" t="s" s="2">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="O82" t="s" s="2">
         <v>45</v>
@@ -11594,11 +11586,11 @@
         <v>113</v>
       </c>
       <c r="X82" t="s" s="2">
+        <v>409</v>
+      </c>
+      <c r="Y82" t="s" s="2">
         <v>410</v>
       </c>
-      <c r="Y82" t="s" s="2">
-        <v>411</v>
-      </c>
       <c r="Z82" t="s" s="2">
         <v>45</v>
       </c>
@@ -11615,7 +11607,7 @@
         <v>45</v>
       </c>
       <c r="AE82" t="s" s="2">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="AF82" t="s" s="2">
         <v>43</v>
@@ -11624,7 +11616,7 @@
         <v>55</v>
       </c>
       <c r="AH82" t="s" s="2">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="AI82" t="s" s="2">
         <v>67</v>
@@ -11639,7 +11631,7 @@
         <v>155</v>
       </c>
       <c r="AM82" t="s" s="2">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="AN82" t="s" s="2">
         <v>45</v>
@@ -11650,11 +11642,11 @@
     </row>
     <row r="83" hidden="true">
       <c r="A83" t="s" s="2">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B83" s="2"/>
       <c r="C83" t="s" s="2">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D83" s="2"/>
       <c r="E83" t="s" s="2">
@@ -11676,16 +11668,16 @@
         <v>202</v>
       </c>
       <c r="K83" t="s" s="2">
+        <v>415</v>
+      </c>
+      <c r="L83" t="s" s="2">
         <v>416</v>
       </c>
-      <c r="L83" t="s" s="2">
+      <c r="M83" t="s" s="2">
         <v>417</v>
       </c>
-      <c r="M83" t="s" s="2">
+      <c r="N83" t="s" s="2">
         <v>418</v>
-      </c>
-      <c r="N83" t="s" s="2">
-        <v>419</v>
       </c>
       <c r="O83" t="s" s="2">
         <v>45</v>
@@ -11713,11 +11705,11 @@
         <v>113</v>
       </c>
       <c r="X83" t="s" s="2">
+        <v>419</v>
+      </c>
+      <c r="Y83" t="s" s="2">
         <v>420</v>
       </c>
-      <c r="Y83" t="s" s="2">
-        <v>421</v>
-      </c>
       <c r="Z83" t="s" s="2">
         <v>45</v>
       </c>
@@ -11734,7 +11726,7 @@
         <v>45</v>
       </c>
       <c r="AE83" t="s" s="2">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="AF83" t="s" s="2">
         <v>43</v>
@@ -11752,24 +11744,24 @@
         <v>45</v>
       </c>
       <c r="AK83" t="s" s="2">
+        <v>421</v>
+      </c>
+      <c r="AL83" t="s" s="2">
         <v>422</v>
       </c>
-      <c r="AL83" t="s" s="2">
+      <c r="AM83" t="s" s="2">
         <v>423</v>
       </c>
-      <c r="AM83" t="s" s="2">
+      <c r="AN83" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO83" t="s" s="2">
         <v>424</v>
-      </c>
-      <c r="AN83" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO83" t="s" s="2">
-        <v>425</v>
       </c>
     </row>
     <row r="84" hidden="true">
       <c r="A84" t="s" s="2">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B84" s="2"/>
       <c r="C84" t="s" s="2">
@@ -11795,16 +11787,16 @@
         <v>45</v>
       </c>
       <c r="K84" t="s" s="2">
+        <v>569</v>
+      </c>
+      <c r="L84" t="s" s="2">
         <v>570</v>
       </c>
-      <c r="L84" t="s" s="2">
-        <v>571</v>
-      </c>
       <c r="M84" t="s" s="2">
+        <v>474</v>
+      </c>
+      <c r="N84" t="s" s="2">
         <v>475</v>
-      </c>
-      <c r="N84" t="s" s="2">
-        <v>476</v>
       </c>
       <c r="O84" t="s" s="2">
         <v>45</v>
@@ -11853,7 +11845,7 @@
         <v>45</v>
       </c>
       <c r="AE84" t="s" s="2">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="AF84" t="s" s="2">
         <v>43</v>
@@ -11874,10 +11866,10 @@
         <v>45</v>
       </c>
       <c r="AL84" t="s" s="2">
+        <v>477</v>
+      </c>
+      <c r="AM84" t="s" s="2">
         <v>478</v>
-      </c>
-      <c r="AM84" t="s" s="2">
-        <v>479</v>
       </c>
       <c r="AN84" t="s" s="2">
         <v>45</v>

</xml_diff>

<commit_message>
added heart-rate and respiration-rate to pulseOx. adjusted bloodpressure to current
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-VA.MHV.bloodOxygenSat.xlsx
+++ b/docs/StructureDefinition-VA.MHV.bloodOxygenSat.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AO$84</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AO$86</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3132" uniqueCount="571">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3208" uniqueCount="577">
   <si>
     <t>Path</t>
   </si>
@@ -1671,10 +1671,31 @@
     <t>When using this element, an observation will typically have either a value or a set of related resources, although both may be present in some cases.  For a discussion on the ways Observations can assembled in groups together, see [Notes](http://hl7.org/fhir/observation.html#obsgrouping) below.  Note that a system may calculate results from [QuestionnaireResponse](http://hl7.org/fhir/questionnaireresponse.html)  into a final score and represent the score as an Observation.</t>
   </si>
   <si>
+    <t xml:space="preserve">profile:resource}
+</t>
+  </si>
+  <si>
+    <t>allow a heart-rate observation and/or respiration rate that is related to this</t>
+  </si>
+  <si>
     <t>Relationships established by OBX-4 usage</t>
   </si>
   <si>
     <t>outBoundRelationship</t>
+  </si>
+  <si>
+    <t>heartRate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference(https://johnmoehrke.github.io/MHV-PGHD/StructureDefinition/VA.MHV.heartRate)
+</t>
+  </si>
+  <si>
+    <t>respirationRate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference(https://johnmoehrke.github.io/MHV-PGHD/StructureDefinition/VA.MHV.respirationRate)
+</t>
   </si>
   <si>
     <t>Observation.derivedFrom</t>
@@ -1950,7 +1971,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AO84"/>
+  <dimension ref="A1:AO86"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1986,7 +2007,7 @@
     <col min="25" max="25" width="51.34375" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="19.921875" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="40.03515625" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="68.30078125" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="14.984375" customWidth="true" bestFit="true"/>
     <col min="30" max="30" width="12.30078125" customWidth="true" bestFit="true"/>
     <col min="31" max="31" width="40.19140625" customWidth="true" bestFit="true" hidden="true"/>
@@ -10592,10 +10613,10 @@
         <v>43</v>
       </c>
       <c r="F74" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G74" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="H74" t="s" s="2">
         <v>45</v>
@@ -10651,16 +10672,16 @@
         <v>45</v>
       </c>
       <c r="AA74" t="s" s="2">
-        <v>45</v>
+        <v>529</v>
       </c>
       <c r="AB74" t="s" s="2">
-        <v>45</v>
+        <v>530</v>
       </c>
       <c r="AC74" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AD74" t="s" s="2">
-        <v>45</v>
+        <v>326</v>
       </c>
       <c r="AE74" t="s" s="2">
         <v>524</v>
@@ -10684,10 +10705,10 @@
         <v>45</v>
       </c>
       <c r="AL74" t="s" s="2">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="AM74" t="s" s="2">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="AN74" t="s" s="2">
         <v>45</v>
@@ -10698,9 +10719,11 @@
     </row>
     <row r="75" hidden="true">
       <c r="A75" t="s" s="2">
-        <v>531</v>
-      </c>
-      <c r="B75" s="2"/>
+        <v>524</v>
+      </c>
+      <c r="B75" t="s" s="2">
+        <v>533</v>
+      </c>
       <c r="C75" t="s" s="2">
         <v>45</v>
       </c>
@@ -10709,7 +10732,7 @@
         <v>43</v>
       </c>
       <c r="F75" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="G75" t="s" s="2">
         <v>45</v>
@@ -10721,16 +10744,16 @@
         <v>56</v>
       </c>
       <c r="J75" t="s" s="2">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="K75" t="s" s="2">
-        <v>533</v>
+        <v>526</v>
       </c>
       <c r="L75" t="s" s="2">
-        <v>534</v>
+        <v>527</v>
       </c>
       <c r="M75" t="s" s="2">
-        <v>535</v>
+        <v>528</v>
       </c>
       <c r="N75" s="2"/>
       <c r="O75" t="s" s="2">
@@ -10780,7 +10803,7 @@
         <v>45</v>
       </c>
       <c r="AE75" t="s" s="2">
-        <v>531</v>
+        <v>524</v>
       </c>
       <c r="AF75" t="s" s="2">
         <v>43</v>
@@ -10801,10 +10824,10 @@
         <v>45</v>
       </c>
       <c r="AL75" t="s" s="2">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="AM75" t="s" s="2">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="AN75" t="s" s="2">
         <v>45</v>
@@ -10813,11 +10836,13 @@
         <v>45</v>
       </c>
     </row>
-    <row r="76">
+    <row r="76" hidden="true">
       <c r="A76" t="s" s="2">
-        <v>537</v>
-      </c>
-      <c r="B76" s="2"/>
+        <v>524</v>
+      </c>
+      <c r="B76" t="s" s="2">
+        <v>535</v>
+      </c>
       <c r="C76" t="s" s="2">
         <v>45</v>
       </c>
@@ -10826,10 +10851,10 @@
         <v>43</v>
       </c>
       <c r="F76" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="G76" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="H76" t="s" s="2">
         <v>45</v>
@@ -10838,20 +10863,18 @@
         <v>56</v>
       </c>
       <c r="J76" t="s" s="2">
-        <v>471</v>
+        <v>536</v>
       </c>
       <c r="K76" t="s" s="2">
-        <v>538</v>
+        <v>526</v>
       </c>
       <c r="L76" t="s" s="2">
-        <v>538</v>
+        <v>527</v>
       </c>
       <c r="M76" t="s" s="2">
-        <v>539</v>
-      </c>
-      <c r="N76" t="s" s="2">
-        <v>540</v>
-      </c>
+        <v>528</v>
+      </c>
+      <c r="N76" s="2"/>
       <c r="O76" t="s" s="2">
         <v>45</v>
       </c>
@@ -10899,7 +10922,7 @@
         <v>45</v>
       </c>
       <c r="AE76" t="s" s="2">
-        <v>537</v>
+        <v>524</v>
       </c>
       <c r="AF76" t="s" s="2">
         <v>43</v>
@@ -10911,7 +10934,7 @@
         <v>45</v>
       </c>
       <c r="AI76" t="s" s="2">
-        <v>541</v>
+        <v>67</v>
       </c>
       <c r="AJ76" t="s" s="2">
         <v>45</v>
@@ -10920,10 +10943,10 @@
         <v>45</v>
       </c>
       <c r="AL76" t="s" s="2">
-        <v>542</v>
+        <v>531</v>
       </c>
       <c r="AM76" t="s" s="2">
-        <v>543</v>
+        <v>532</v>
       </c>
       <c r="AN76" t="s" s="2">
         <v>45</v>
@@ -10934,7 +10957,7 @@
     </row>
     <row r="77" hidden="true">
       <c r="A77" t="s" s="2">
-        <v>544</v>
+        <v>537</v>
       </c>
       <c r="B77" s="2"/>
       <c r="C77" t="s" s="2">
@@ -10945,7 +10968,7 @@
         <v>43</v>
       </c>
       <c r="F77" t="s" s="2">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="G77" t="s" s="2">
         <v>45</v>
@@ -10954,18 +10977,20 @@
         <v>45</v>
       </c>
       <c r="I77" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J77" t="s" s="2">
-        <v>57</v>
+        <v>538</v>
       </c>
       <c r="K77" t="s" s="2">
-        <v>69</v>
+        <v>539</v>
       </c>
       <c r="L77" t="s" s="2">
-        <v>70</v>
-      </c>
-      <c r="M77" s="2"/>
+        <v>540</v>
+      </c>
+      <c r="M77" t="s" s="2">
+        <v>541</v>
+      </c>
       <c r="N77" s="2"/>
       <c r="O77" t="s" s="2">
         <v>45</v>
@@ -11014,19 +11039,19 @@
         <v>45</v>
       </c>
       <c r="AE77" t="s" s="2">
-        <v>71</v>
+        <v>537</v>
       </c>
       <c r="AF77" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG77" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH77" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI77" t="s" s="2">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="AJ77" t="s" s="2">
         <v>45</v>
@@ -11035,10 +11060,10 @@
         <v>45</v>
       </c>
       <c r="AL77" t="s" s="2">
-        <v>45</v>
+        <v>531</v>
       </c>
       <c r="AM77" t="s" s="2">
-        <v>72</v>
+        <v>542</v>
       </c>
       <c r="AN77" t="s" s="2">
         <v>45</v>
@@ -11047,43 +11072,45 @@
         <v>45</v>
       </c>
     </row>
-    <row r="78" hidden="true">
+    <row r="78">
       <c r="A78" t="s" s="2">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="B78" s="2"/>
       <c r="C78" t="s" s="2">
-        <v>74</v>
+        <v>45</v>
       </c>
       <c r="D78" s="2"/>
       <c r="E78" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F78" t="s" s="2">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G78" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="H78" t="s" s="2">
         <v>45</v>
       </c>
       <c r="I78" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J78" t="s" s="2">
-        <v>75</v>
+        <v>471</v>
       </c>
       <c r="K78" t="s" s="2">
-        <v>76</v>
+        <v>544</v>
       </c>
       <c r="L78" t="s" s="2">
-        <v>77</v>
+        <v>544</v>
       </c>
       <c r="M78" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="N78" s="2"/>
+        <v>545</v>
+      </c>
+      <c r="N78" t="s" s="2">
+        <v>546</v>
+      </c>
       <c r="O78" t="s" s="2">
         <v>45</v>
       </c>
@@ -11131,7 +11158,7 @@
         <v>45</v>
       </c>
       <c r="AE78" t="s" s="2">
-        <v>82</v>
+        <v>543</v>
       </c>
       <c r="AF78" t="s" s="2">
         <v>43</v>
@@ -11143,7 +11170,7 @@
         <v>45</v>
       </c>
       <c r="AI78" t="s" s="2">
-        <v>83</v>
+        <v>547</v>
       </c>
       <c r="AJ78" t="s" s="2">
         <v>45</v>
@@ -11152,10 +11179,10 @@
         <v>45</v>
       </c>
       <c r="AL78" t="s" s="2">
-        <v>45</v>
+        <v>548</v>
       </c>
       <c r="AM78" t="s" s="2">
-        <v>72</v>
+        <v>549</v>
       </c>
       <c r="AN78" t="s" s="2">
         <v>45</v>
@@ -11166,43 +11193,39 @@
     </row>
     <row r="79" hidden="true">
       <c r="A79" t="s" s="2">
-        <v>546</v>
+        <v>550</v>
       </c>
       <c r="B79" s="2"/>
       <c r="C79" t="s" s="2">
-        <v>482</v>
+        <v>45</v>
       </c>
       <c r="D79" s="2"/>
       <c r="E79" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F79" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G79" t="s" s="2">
         <v>45</v>
       </c>
       <c r="H79" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="I79" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J79" t="s" s="2">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="K79" t="s" s="2">
-        <v>483</v>
+        <v>69</v>
       </c>
       <c r="L79" t="s" s="2">
-        <v>484</v>
-      </c>
-      <c r="M79" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="N79" t="s" s="2">
-        <v>485</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="M79" s="2"/>
+      <c r="N79" s="2"/>
       <c r="O79" t="s" s="2">
         <v>45</v>
       </c>
@@ -11250,19 +11273,19 @@
         <v>45</v>
       </c>
       <c r="AE79" t="s" s="2">
-        <v>486</v>
+        <v>71</v>
       </c>
       <c r="AF79" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG79" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH79" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI79" t="s" s="2">
-        <v>83</v>
+        <v>45</v>
       </c>
       <c r="AJ79" t="s" s="2">
         <v>45</v>
@@ -11274,7 +11297,7 @@
         <v>45</v>
       </c>
       <c r="AM79" t="s" s="2">
-        <v>155</v>
+        <v>72</v>
       </c>
       <c r="AN79" t="s" s="2">
         <v>45</v>
@@ -11283,45 +11306,43 @@
         <v>45</v>
       </c>
     </row>
-    <row r="80">
+    <row r="80" hidden="true">
       <c r="A80" t="s" s="2">
-        <v>547</v>
+        <v>551</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" t="s" s="2">
-        <v>45</v>
+        <v>74</v>
       </c>
       <c r="D80" s="2"/>
       <c r="E80" t="s" s="2">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="F80" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G80" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="H80" t="s" s="2">
         <v>45</v>
       </c>
       <c r="I80" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J80" t="s" s="2">
-        <v>202</v>
+        <v>75</v>
       </c>
       <c r="K80" t="s" s="2">
-        <v>548</v>
+        <v>76</v>
       </c>
       <c r="L80" t="s" s="2">
-        <v>549</v>
+        <v>77</v>
       </c>
       <c r="M80" t="s" s="2">
-        <v>550</v>
-      </c>
-      <c r="N80" t="s" s="2">
-        <v>551</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="N80" s="2"/>
       <c r="O80" t="s" s="2">
         <v>45</v>
       </c>
@@ -11345,13 +11366,13 @@
         <v>45</v>
       </c>
       <c r="W80" t="s" s="2">
-        <v>113</v>
+        <v>45</v>
       </c>
       <c r="X80" t="s" s="2">
-        <v>279</v>
+        <v>45</v>
       </c>
       <c r="Y80" t="s" s="2">
-        <v>280</v>
+        <v>45</v>
       </c>
       <c r="Z80" t="s" s="2">
         <v>45</v>
@@ -11369,77 +11390,77 @@
         <v>45</v>
       </c>
       <c r="AE80" t="s" s="2">
-        <v>547</v>
+        <v>82</v>
       </c>
       <c r="AF80" t="s" s="2">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="AG80" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH80" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI80" t="s" s="2">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="AJ80" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AK80" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL80" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AM80" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="AN80" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO80" t="s" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="81" hidden="true">
+      <c r="A81" t="s" s="2">
         <v>552</v>
-      </c>
-      <c r="AL80" t="s" s="2">
-        <v>283</v>
-      </c>
-      <c r="AM80" t="s" s="2">
-        <v>284</v>
-      </c>
-      <c r="AN80" t="s" s="2">
-        <v>285</v>
-      </c>
-      <c r="AO80" t="s" s="2">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="s" s="2">
-        <v>553</v>
       </c>
       <c r="B81" s="2"/>
       <c r="C81" t="s" s="2">
-        <v>45</v>
+        <v>482</v>
       </c>
       <c r="D81" s="2"/>
       <c r="E81" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F81" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G81" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="H81" t="s" s="2">
         <v>56</v>
-      </c>
-      <c r="H81" t="s" s="2">
-        <v>45</v>
       </c>
       <c r="I81" t="s" s="2">
         <v>56</v>
       </c>
       <c r="J81" t="s" s="2">
-        <v>554</v>
+        <v>75</v>
       </c>
       <c r="K81" t="s" s="2">
-        <v>555</v>
+        <v>483</v>
       </c>
       <c r="L81" t="s" s="2">
-        <v>556</v>
+        <v>484</v>
       </c>
       <c r="M81" t="s" s="2">
-        <v>557</v>
+        <v>78</v>
       </c>
       <c r="N81" t="s" s="2">
-        <v>354</v>
+        <v>485</v>
       </c>
       <c r="O81" t="s" s="2">
         <v>45</v>
@@ -11464,13 +11485,13 @@
         <v>45</v>
       </c>
       <c r="W81" t="s" s="2">
-        <v>194</v>
+        <v>45</v>
       </c>
       <c r="X81" t="s" s="2">
-        <v>558</v>
+        <v>45</v>
       </c>
       <c r="Y81" t="s" s="2">
-        <v>559</v>
+        <v>45</v>
       </c>
       <c r="Z81" t="s" s="2">
         <v>45</v>
@@ -11488,42 +11509,42 @@
         <v>45</v>
       </c>
       <c r="AE81" t="s" s="2">
-        <v>553</v>
+        <v>486</v>
       </c>
       <c r="AF81" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG81" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH81" t="s" s="2">
-        <v>560</v>
+        <v>45</v>
       </c>
       <c r="AI81" t="s" s="2">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="AJ81" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AK81" t="s" s="2">
-        <v>561</v>
+        <v>45</v>
       </c>
       <c r="AL81" t="s" s="2">
-        <v>357</v>
+        <v>45</v>
       </c>
       <c r="AM81" t="s" s="2">
-        <v>358</v>
+        <v>155</v>
       </c>
       <c r="AN81" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO81" t="s" s="2">
-        <v>359</v>
+        <v>45</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s" s="2">
-        <v>562</v>
+        <v>553</v>
       </c>
       <c r="B82" s="2"/>
       <c r="C82" t="s" s="2">
@@ -11531,7 +11552,7 @@
       </c>
       <c r="D82" s="2"/>
       <c r="E82" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="F82" t="s" s="2">
         <v>55</v>
@@ -11543,22 +11564,22 @@
         <v>45</v>
       </c>
       <c r="I82" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J82" t="s" s="2">
         <v>202</v>
       </c>
       <c r="K82" t="s" s="2">
-        <v>563</v>
+        <v>554</v>
       </c>
       <c r="L82" t="s" s="2">
-        <v>564</v>
+        <v>555</v>
       </c>
       <c r="M82" t="s" s="2">
-        <v>565</v>
+        <v>556</v>
       </c>
       <c r="N82" t="s" s="2">
-        <v>408</v>
+        <v>557</v>
       </c>
       <c r="O82" t="s" s="2">
         <v>45</v>
@@ -11586,10 +11607,10 @@
         <v>113</v>
       </c>
       <c r="X82" t="s" s="2">
-        <v>409</v>
+        <v>279</v>
       </c>
       <c r="Y82" t="s" s="2">
-        <v>410</v>
+        <v>280</v>
       </c>
       <c r="Z82" t="s" s="2">
         <v>45</v>
@@ -11607,16 +11628,16 @@
         <v>45</v>
       </c>
       <c r="AE82" t="s" s="2">
-        <v>562</v>
+        <v>553</v>
       </c>
       <c r="AF82" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="AG82" t="s" s="2">
         <v>55</v>
       </c>
       <c r="AH82" t="s" s="2">
-        <v>566</v>
+        <v>45</v>
       </c>
       <c r="AI82" t="s" s="2">
         <v>67</v>
@@ -11625,59 +11646,59 @@
         <v>45</v>
       </c>
       <c r="AK82" t="s" s="2">
-        <v>45</v>
+        <v>558</v>
       </c>
       <c r="AL82" t="s" s="2">
-        <v>155</v>
+        <v>283</v>
       </c>
       <c r="AM82" t="s" s="2">
-        <v>412</v>
+        <v>284</v>
       </c>
       <c r="AN82" t="s" s="2">
-        <v>45</v>
+        <v>285</v>
       </c>
       <c r="AO82" t="s" s="2">
         <v>45</v>
       </c>
     </row>
-    <row r="83" hidden="true">
+    <row r="83">
       <c r="A83" t="s" s="2">
-        <v>567</v>
+        <v>559</v>
       </c>
       <c r="B83" s="2"/>
       <c r="C83" t="s" s="2">
-        <v>414</v>
+        <v>45</v>
       </c>
       <c r="D83" s="2"/>
       <c r="E83" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F83" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G83" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="H83" t="s" s="2">
         <v>45</v>
       </c>
       <c r="I83" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J83" t="s" s="2">
-        <v>202</v>
+        <v>560</v>
       </c>
       <c r="K83" t="s" s="2">
-        <v>415</v>
+        <v>561</v>
       </c>
       <c r="L83" t="s" s="2">
-        <v>416</v>
+        <v>562</v>
       </c>
       <c r="M83" t="s" s="2">
-        <v>417</v>
+        <v>563</v>
       </c>
       <c r="N83" t="s" s="2">
-        <v>418</v>
+        <v>354</v>
       </c>
       <c r="O83" t="s" s="2">
         <v>45</v>
@@ -11702,13 +11723,13 @@
         <v>45</v>
       </c>
       <c r="W83" t="s" s="2">
-        <v>113</v>
+        <v>194</v>
       </c>
       <c r="X83" t="s" s="2">
-        <v>419</v>
+        <v>564</v>
       </c>
       <c r="Y83" t="s" s="2">
-        <v>420</v>
+        <v>565</v>
       </c>
       <c r="Z83" t="s" s="2">
         <v>45</v>
@@ -11726,16 +11747,16 @@
         <v>45</v>
       </c>
       <c r="AE83" t="s" s="2">
-        <v>567</v>
+        <v>559</v>
       </c>
       <c r="AF83" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG83" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH83" t="s" s="2">
-        <v>45</v>
+        <v>566</v>
       </c>
       <c r="AI83" t="s" s="2">
         <v>67</v>
@@ -11744,22 +11765,22 @@
         <v>45</v>
       </c>
       <c r="AK83" t="s" s="2">
-        <v>421</v>
+        <v>567</v>
       </c>
       <c r="AL83" t="s" s="2">
-        <v>422</v>
+        <v>357</v>
       </c>
       <c r="AM83" t="s" s="2">
-        <v>423</v>
+        <v>358</v>
       </c>
       <c r="AN83" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO83" t="s" s="2">
-        <v>424</v>
+        <v>359</v>
       </c>
     </row>
-    <row r="84" hidden="true">
+    <row r="84">
       <c r="A84" t="s" s="2">
         <v>568</v>
       </c>
@@ -11772,10 +11793,10 @@
         <v>43</v>
       </c>
       <c r="F84" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G84" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="H84" t="s" s="2">
         <v>45</v>
@@ -11784,7 +11805,7 @@
         <v>45</v>
       </c>
       <c r="J84" t="s" s="2">
-        <v>45</v>
+        <v>202</v>
       </c>
       <c r="K84" t="s" s="2">
         <v>569</v>
@@ -11793,10 +11814,10 @@
         <v>570</v>
       </c>
       <c r="M84" t="s" s="2">
-        <v>474</v>
+        <v>571</v>
       </c>
       <c r="N84" t="s" s="2">
-        <v>475</v>
+        <v>408</v>
       </c>
       <c r="O84" t="s" s="2">
         <v>45</v>
@@ -11821,13 +11842,13 @@
         <v>45</v>
       </c>
       <c r="W84" t="s" s="2">
-        <v>45</v>
+        <v>113</v>
       </c>
       <c r="X84" t="s" s="2">
-        <v>45</v>
+        <v>409</v>
       </c>
       <c r="Y84" t="s" s="2">
-        <v>45</v>
+        <v>410</v>
       </c>
       <c r="Z84" t="s" s="2">
         <v>45</v>
@@ -11851,10 +11872,10 @@
         <v>43</v>
       </c>
       <c r="AG84" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH84" t="s" s="2">
-        <v>45</v>
+        <v>572</v>
       </c>
       <c r="AI84" t="s" s="2">
         <v>67</v>
@@ -11866,20 +11887,258 @@
         <v>45</v>
       </c>
       <c r="AL84" t="s" s="2">
+        <v>155</v>
+      </c>
+      <c r="AM84" t="s" s="2">
+        <v>412</v>
+      </c>
+      <c r="AN84" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO84" t="s" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="85" hidden="true">
+      <c r="A85" t="s" s="2">
+        <v>573</v>
+      </c>
+      <c r="B85" s="2"/>
+      <c r="C85" t="s" s="2">
+        <v>414</v>
+      </c>
+      <c r="D85" s="2"/>
+      <c r="E85" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="F85" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="G85" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="H85" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="I85" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="J85" t="s" s="2">
+        <v>202</v>
+      </c>
+      <c r="K85" t="s" s="2">
+        <v>415</v>
+      </c>
+      <c r="L85" t="s" s="2">
+        <v>416</v>
+      </c>
+      <c r="M85" t="s" s="2">
+        <v>417</v>
+      </c>
+      <c r="N85" t="s" s="2">
+        <v>418</v>
+      </c>
+      <c r="O85" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="P85" s="2"/>
+      <c r="Q85" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="R85" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="S85" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="T85" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="U85" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="V85" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="W85" t="s" s="2">
+        <v>113</v>
+      </c>
+      <c r="X85" t="s" s="2">
+        <v>419</v>
+      </c>
+      <c r="Y85" t="s" s="2">
+        <v>420</v>
+      </c>
+      <c r="Z85" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA85" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB85" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC85" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD85" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE85" t="s" s="2">
+        <v>573</v>
+      </c>
+      <c r="AF85" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG85" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AH85" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI85" t="s" s="2">
+        <v>67</v>
+      </c>
+      <c r="AJ85" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK85" t="s" s="2">
+        <v>421</v>
+      </c>
+      <c r="AL85" t="s" s="2">
+        <v>422</v>
+      </c>
+      <c r="AM85" t="s" s="2">
+        <v>423</v>
+      </c>
+      <c r="AN85" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO85" t="s" s="2">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="86" hidden="true">
+      <c r="A86" t="s" s="2">
+        <v>574</v>
+      </c>
+      <c r="B86" s="2"/>
+      <c r="C86" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="D86" s="2"/>
+      <c r="E86" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="F86" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="G86" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="H86" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="I86" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="J86" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="K86" t="s" s="2">
+        <v>575</v>
+      </c>
+      <c r="L86" t="s" s="2">
+        <v>576</v>
+      </c>
+      <c r="M86" t="s" s="2">
+        <v>474</v>
+      </c>
+      <c r="N86" t="s" s="2">
+        <v>475</v>
+      </c>
+      <c r="O86" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="P86" s="2"/>
+      <c r="Q86" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="R86" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="S86" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="T86" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="U86" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="V86" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="W86" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="X86" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Y86" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Z86" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA86" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB86" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC86" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD86" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE86" t="s" s="2">
+        <v>574</v>
+      </c>
+      <c r="AF86" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG86" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AH86" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI86" t="s" s="2">
+        <v>67</v>
+      </c>
+      <c r="AJ86" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK86" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL86" t="s" s="2">
         <v>477</v>
       </c>
-      <c r="AM84" t="s" s="2">
+      <c r="AM86" t="s" s="2">
         <v>478</v>
       </c>
-      <c r="AN84" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO84" t="s" s="2">
+      <c r="AN86" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO86" t="s" s="2">
         <v>45</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AO84">
+  <autoFilter ref="A1:AO86">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -11889,7 +12148,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI83">
+  <conditionalFormatting sqref="A2:AI85">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>

<commit_message>
fix a profiling issue on hasMember
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-VA.MHV.bloodOxygenSat.xlsx
+++ b/docs/StructureDefinition-VA.MHV.bloodOxygenSat.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3208" uniqueCount="577">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3209" uniqueCount="577">
   <si>
     <t>Path</t>
   </si>
@@ -919,6 +919,36 @@
     <t>Observation.code.coding</t>
   </si>
   <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value:$this}
+</t>
+  </si>
+  <si>
+    <t>closed</t>
+  </si>
+  <si>
+    <t>ox1</t>
+  </si>
+  <si>
+    <t>&lt;valueCoding xmlns="http://hl7.org/fhir"&gt;
+  &lt;system value="http://loinc.org"/&gt;
+  &lt;code value="59408-5"/&gt;
+  &lt;display value="Oxygen saturation in Arterial blood by Pulse oximetry"/&gt;
+&lt;/valueCoding&gt;</t>
+  </si>
+  <si>
+    <t>ox2</t>
+  </si>
+  <si>
+    <t>&lt;valueCoding xmlns="http://hl7.org/fhir"&gt;
+  &lt;system value="http://loinc.org"/&gt;
+  &lt;code value="2708-6"/&gt;
+  &lt;display value="Oxygen saturation in Arterial blood"/&gt;
+&lt;/valueCoding&gt;</t>
+  </si>
+  <si>
     <t>Observation.code.text</t>
   </si>
   <si>
@@ -1032,9 +1062,6 @@
   <si>
     <t xml:space="preserve">type:$this}
 </t>
-  </si>
-  <si>
-    <t>closed</t>
   </si>
   <si>
     <t xml:space="preserve">vs-1
@@ -1658,7 +1685,7 @@
     <t>Observation.hasMember</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(QuestionnaireResponse|MolecularSequence|vitalsigns)
+    <t xml:space="preserve">Reference(https://johnmoehrke.github.io/MHV-PGHD/StructureDefinition/VA.MHV.heartRate|https://johnmoehrke.github.io/MHV-PGHD/StructureDefinition/VA.MHV.respirationRate)
 </t>
   </si>
   <si>
@@ -1671,31 +1698,10 @@
     <t>When using this element, an observation will typically have either a value or a set of related resources, although both may be present in some cases.  For a discussion on the ways Observations can assembled in groups together, see [Notes](http://hl7.org/fhir/observation.html#obsgrouping) below.  Note that a system may calculate results from [QuestionnaireResponse](http://hl7.org/fhir/questionnaireresponse.html)  into a final score and represent the score as an Observation.</t>
   </si>
   <si>
-    <t xml:space="preserve">profile:resource}
-</t>
-  </si>
-  <si>
-    <t>allow a heart-rate observation and/or respiration rate that is related to this</t>
-  </si>
-  <si>
     <t>Relationships established by OBX-4 usage</t>
   </si>
   <si>
     <t>outBoundRelationship</t>
-  </si>
-  <si>
-    <t>heartRate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reference(https://johnmoehrke.github.io/MHV-PGHD/StructureDefinition/VA.MHV.heartRate)
-</t>
-  </si>
-  <si>
-    <t>respirationRate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reference(https://johnmoehrke.github.io/MHV-PGHD/StructureDefinition/VA.MHV.respirationRate)
-</t>
   </si>
   <si>
     <t>Observation.derivedFrom</t>
@@ -2007,7 +2013,7 @@
     <col min="25" max="25" width="51.34375" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="19.921875" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="68.30078125" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="40.03515625" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="14.984375" customWidth="true" bestFit="true"/>
     <col min="30" max="30" width="12.30078125" customWidth="true" bestFit="true"/>
     <col min="31" max="31" width="40.19140625" customWidth="true" bestFit="true" hidden="true"/>
@@ -4610,7 +4616,7 @@
         <v>55</v>
       </c>
       <c r="F23" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G23" t="s" s="2">
         <v>56</v>
@@ -6487,10 +6493,10 @@
       </c>
       <c r="D39" s="2"/>
       <c r="E39" t="s" s="2">
-        <v>43</v>
+        <v>290</v>
       </c>
       <c r="F39" t="s" s="2">
-        <v>44</v>
+        <v>290</v>
       </c>
       <c r="G39" t="s" s="2">
         <v>45</v>
@@ -6551,16 +6557,14 @@
         <v>45</v>
       </c>
       <c r="AA39" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AB39" t="s" s="2">
-        <v>45</v>
-      </c>
+        <v>291</v>
+      </c>
+      <c r="AB39" s="2"/>
       <c r="AC39" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AD39" t="s" s="2">
-        <v>45</v>
+        <v>292</v>
       </c>
       <c r="AE39" t="s" s="2">
         <v>220</v>
@@ -6598,15 +6602,17 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>290</v>
-      </c>
-      <c r="B40" s="2"/>
+        <v>289</v>
+      </c>
+      <c r="B40" t="s" s="2">
+        <v>293</v>
+      </c>
       <c r="C40" t="s" s="2">
         <v>45</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="F40" t="s" s="2">
         <v>55</v>
@@ -6621,19 +6627,19 @@
         <v>56</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>57</v>
+        <v>109</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>266</v>
+        <v>216</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>267</v>
+        <v>217</v>
       </c>
       <c r="M40" t="s" s="2">
-        <v>268</v>
+        <v>218</v>
       </c>
       <c r="N40" t="s" s="2">
-        <v>269</v>
+        <v>219</v>
       </c>
       <c r="O40" t="s" s="2">
         <v>45</v>
@@ -6643,7 +6649,7 @@
         <v>45</v>
       </c>
       <c r="R40" t="s" s="2">
-        <v>45</v>
+        <v>294</v>
       </c>
       <c r="S40" t="s" s="2">
         <v>45</v>
@@ -6682,13 +6688,13 @@
         <v>45</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>270</v>
+        <v>220</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG40" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH40" t="s" s="2">
         <v>45</v>
@@ -6703,10 +6709,10 @@
         <v>45</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>271</v>
+        <v>221</v>
       </c>
       <c r="AM40" t="s" s="2">
-        <v>272</v>
+        <v>222</v>
       </c>
       <c r="AN40" t="s" s="2">
         <v>45</v>
@@ -6715,11 +6721,13 @@
         <v>45</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>291</v>
-      </c>
-      <c r="B41" s="2"/>
+        <v>289</v>
+      </c>
+      <c r="B41" t="s" s="2">
+        <v>295</v>
+      </c>
       <c r="C41" t="s" s="2">
         <v>45</v>
       </c>
@@ -6731,7 +6739,7 @@
         <v>55</v>
       </c>
       <c r="G41" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="H41" t="s" s="2">
         <v>45</v>
@@ -6740,19 +6748,19 @@
         <v>56</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>292</v>
+        <v>109</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>293</v>
+        <v>216</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>294</v>
+        <v>217</v>
       </c>
       <c r="M41" t="s" s="2">
-        <v>295</v>
+        <v>218</v>
       </c>
       <c r="N41" t="s" s="2">
-        <v>296</v>
+        <v>219</v>
       </c>
       <c r="O41" t="s" s="2">
         <v>45</v>
@@ -6762,7 +6770,7 @@
         <v>45</v>
       </c>
       <c r="R41" t="s" s="2">
-        <v>45</v>
+        <v>296</v>
       </c>
       <c r="S41" t="s" s="2">
         <v>45</v>
@@ -6801,13 +6809,13 @@
         <v>45</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>291</v>
+        <v>220</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG41" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH41" t="s" s="2">
         <v>45</v>
@@ -6816,19 +6824,19 @@
         <v>67</v>
       </c>
       <c r="AJ41" t="s" s="2">
-        <v>297</v>
+        <v>45</v>
       </c>
       <c r="AK41" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL41" t="s" s="2">
-        <v>298</v>
+        <v>221</v>
       </c>
       <c r="AM41" t="s" s="2">
-        <v>299</v>
+        <v>222</v>
       </c>
       <c r="AN41" t="s" s="2">
-        <v>300</v>
+        <v>45</v>
       </c>
       <c r="AO41" t="s" s="2">
         <v>45</v>
@@ -6836,7 +6844,7 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -6847,7 +6855,7 @@
         <v>43</v>
       </c>
       <c r="F42" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="G42" t="s" s="2">
         <v>45</v>
@@ -6859,18 +6867,20 @@
         <v>56</v>
       </c>
       <c r="J42" t="s" s="2">
-        <v>302</v>
+        <v>57</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>303</v>
+        <v>266</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>304</v>
+        <v>267</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>305</v>
-      </c>
-      <c r="N42" s="2"/>
+        <v>268</v>
+      </c>
+      <c r="N42" t="s" s="2">
+        <v>269</v>
+      </c>
       <c r="O42" t="s" s="2">
         <v>45</v>
       </c>
@@ -6918,13 +6928,13 @@
         <v>45</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>301</v>
+        <v>270</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG42" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH42" t="s" s="2">
         <v>45</v>
@@ -6939,35 +6949,35 @@
         <v>45</v>
       </c>
       <c r="AL42" t="s" s="2">
-        <v>283</v>
+        <v>271</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>306</v>
+        <v>272</v>
       </c>
       <c r="AN42" t="s" s="2">
-        <v>300</v>
+        <v>45</v>
       </c>
       <c r="AO42" t="s" s="2">
         <v>45</v>
       </c>
     </row>
-    <row r="43" hidden="true">
+    <row r="43">
       <c r="A43" t="s" s="2">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
-        <v>308</v>
+        <v>45</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="F43" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="G43" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="H43" t="s" s="2">
         <v>45</v>
@@ -6976,19 +6986,19 @@
         <v>56</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>309</v>
+        <v>299</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>311</v>
+        <v>301</v>
       </c>
       <c r="M43" t="s" s="2">
-        <v>312</v>
+        <v>302</v>
       </c>
       <c r="N43" t="s" s="2">
-        <v>313</v>
+        <v>303</v>
       </c>
       <c r="O43" t="s" s="2">
         <v>45</v>
@@ -7037,7 +7047,7 @@
         <v>45</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>43</v>
@@ -7052,19 +7062,19 @@
         <v>67</v>
       </c>
       <c r="AJ43" t="s" s="2">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="AK43" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL43" t="s" s="2">
-        <v>315</v>
+        <v>305</v>
       </c>
       <c r="AM43" t="s" s="2">
-        <v>316</v>
+        <v>306</v>
       </c>
       <c r="AN43" t="s" s="2">
-        <v>317</v>
+        <v>307</v>
       </c>
       <c r="AO43" t="s" s="2">
         <v>45</v>
@@ -7072,21 +7082,21 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>318</v>
+        <v>308</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
-        <v>319</v>
+        <v>45</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" t="s" s="2">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="F44" t="s" s="2">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="G44" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="H44" t="s" s="2">
         <v>45</v>
@@ -7095,20 +7105,18 @@
         <v>56</v>
       </c>
       <c r="J44" t="s" s="2">
-        <v>320</v>
+        <v>309</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>321</v>
+        <v>310</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>322</v>
+        <v>311</v>
       </c>
       <c r="M44" t="s" s="2">
-        <v>323</v>
-      </c>
-      <c r="N44" t="s" s="2">
-        <v>324</v>
-      </c>
+        <v>312</v>
+      </c>
+      <c r="N44" s="2"/>
       <c r="O44" t="s" s="2">
         <v>45</v>
       </c>
@@ -7144,68 +7152,68 @@
         <v>45</v>
       </c>
       <c r="AA44" t="s" s="2">
-        <v>325</v>
-      </c>
-      <c r="AB44" s="2"/>
+        <v>45</v>
+      </c>
+      <c r="AB44" t="s" s="2">
+        <v>45</v>
+      </c>
       <c r="AC44" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AD44" t="s" s="2">
-        <v>326</v>
+        <v>45</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>318</v>
+        <v>308</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG44" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH44" t="s" s="2">
-        <v>327</v>
+        <v>45</v>
       </c>
       <c r="AI44" t="s" s="2">
-        <v>328</v>
+        <v>67</v>
       </c>
       <c r="AJ44" t="s" s="2">
-        <v>329</v>
+        <v>45</v>
       </c>
       <c r="AK44" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL44" t="s" s="2">
-        <v>330</v>
+        <v>283</v>
       </c>
       <c r="AM44" t="s" s="2">
-        <v>331</v>
+        <v>313</v>
       </c>
       <c r="AN44" t="s" s="2">
-        <v>332</v>
+        <v>307</v>
       </c>
       <c r="AO44" t="s" s="2">
         <v>45</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>318</v>
-      </c>
-      <c r="B45" t="s" s="2">
-        <v>333</v>
-      </c>
+        <v>314</v>
+      </c>
+      <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" t="s" s="2">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="F45" t="s" s="2">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="G45" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="H45" t="s" s="2">
         <v>45</v>
@@ -7214,19 +7222,19 @@
         <v>56</v>
       </c>
       <c r="J45" t="s" s="2">
+        <v>316</v>
+      </c>
+      <c r="K45" t="s" s="2">
+        <v>317</v>
+      </c>
+      <c r="L45" t="s" s="2">
+        <v>318</v>
+      </c>
+      <c r="M45" t="s" s="2">
+        <v>319</v>
+      </c>
+      <c r="N45" t="s" s="2">
         <v>320</v>
-      </c>
-      <c r="K45" t="s" s="2">
-        <v>321</v>
-      </c>
-      <c r="L45" t="s" s="2">
-        <v>322</v>
-      </c>
-      <c r="M45" t="s" s="2">
-        <v>323</v>
-      </c>
-      <c r="N45" t="s" s="2">
-        <v>324</v>
       </c>
       <c r="O45" t="s" s="2">
         <v>45</v>
@@ -7275,7 +7283,7 @@
         <v>45</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>43</v>
@@ -7284,25 +7292,25 @@
         <v>55</v>
       </c>
       <c r="AH45" t="s" s="2">
-        <v>327</v>
+        <v>45</v>
       </c>
       <c r="AI45" t="s" s="2">
-        <v>328</v>
+        <v>67</v>
       </c>
       <c r="AJ45" t="s" s="2">
-        <v>329</v>
+        <v>321</v>
       </c>
       <c r="AK45" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL45" t="s" s="2">
-        <v>330</v>
+        <v>322</v>
       </c>
       <c r="AM45" t="s" s="2">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="AN45" t="s" s="2">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="AO45" t="s" s="2">
         <v>45</v>
@@ -7310,21 +7318,21 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>334</v>
+        <v>325</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
-        <v>45</v>
+        <v>326</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="F46" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="G46" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="H46" t="s" s="2">
         <v>45</v>
@@ -7333,18 +7341,20 @@
         <v>56</v>
       </c>
       <c r="J46" t="s" s="2">
-        <v>91</v>
+        <v>327</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>337</v>
-      </c>
-      <c r="N46" s="2"/>
+        <v>330</v>
+      </c>
+      <c r="N46" t="s" s="2">
+        <v>331</v>
+      </c>
       <c r="O46" t="s" s="2">
         <v>45</v>
       </c>
@@ -7380,19 +7390,17 @@
         <v>45</v>
       </c>
       <c r="AA46" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AB46" t="s" s="2">
-        <v>45</v>
-      </c>
+        <v>332</v>
+      </c>
+      <c r="AB46" s="2"/>
       <c r="AC46" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AD46" t="s" s="2">
-        <v>45</v>
+        <v>292</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>334</v>
+        <v>325</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>43</v>
@@ -7401,47 +7409,49 @@
         <v>55</v>
       </c>
       <c r="AH46" t="s" s="2">
-        <v>45</v>
+        <v>333</v>
       </c>
       <c r="AI46" t="s" s="2">
-        <v>67</v>
+        <v>334</v>
       </c>
       <c r="AJ46" t="s" s="2">
-        <v>45</v>
+        <v>335</v>
       </c>
       <c r="AK46" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL46" t="s" s="2">
+        <v>336</v>
+      </c>
+      <c r="AM46" t="s" s="2">
+        <v>337</v>
+      </c>
+      <c r="AN46" t="s" s="2">
         <v>338</v>
       </c>
-      <c r="AM46" t="s" s="2">
+      <c r="AO46" t="s" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="2">
+        <v>325</v>
+      </c>
+      <c r="B47" t="s" s="2">
         <v>339</v>
       </c>
-      <c r="AN46" t="s" s="2">
-        <v>340</v>
-      </c>
-      <c r="AO46" t="s" s="2">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="47" hidden="true">
-      <c r="A47" t="s" s="2">
-        <v>341</v>
-      </c>
-      <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
-        <v>45</v>
+        <v>326</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="F47" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="G47" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="H47" t="s" s="2">
         <v>45</v>
@@ -7450,17 +7460,19 @@
         <v>56</v>
       </c>
       <c r="J47" t="s" s="2">
-        <v>342</v>
+        <v>327</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>343</v>
+        <v>328</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>344</v>
-      </c>
-      <c r="M47" s="2"/>
+        <v>329</v>
+      </c>
+      <c r="M47" t="s" s="2">
+        <v>330</v>
+      </c>
       <c r="N47" t="s" s="2">
-        <v>345</v>
+        <v>331</v>
       </c>
       <c r="O47" t="s" s="2">
         <v>45</v>
@@ -7509,34 +7521,34 @@
         <v>45</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>341</v>
+        <v>325</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG47" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH47" t="s" s="2">
-        <v>45</v>
+        <v>333</v>
       </c>
       <c r="AI47" t="s" s="2">
-        <v>67</v>
+        <v>334</v>
       </c>
       <c r="AJ47" t="s" s="2">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="AK47" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL47" t="s" s="2">
-        <v>347</v>
+        <v>336</v>
       </c>
       <c r="AM47" t="s" s="2">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="AN47" t="s" s="2">
-        <v>349</v>
+        <v>338</v>
       </c>
       <c r="AO47" t="s" s="2">
         <v>45</v>
@@ -7544,7 +7556,7 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
@@ -7555,10 +7567,10 @@
         <v>43</v>
       </c>
       <c r="F48" t="s" s="2">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="G48" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="H48" t="s" s="2">
         <v>45</v>
@@ -7567,20 +7579,18 @@
         <v>56</v>
       </c>
       <c r="J48" t="s" s="2">
-        <v>351</v>
+        <v>91</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>352</v>
+        <v>341</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>352</v>
+        <v>342</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>353</v>
-      </c>
-      <c r="N48" t="s" s="2">
-        <v>354</v>
-      </c>
+        <v>343</v>
+      </c>
+      <c r="N48" s="2"/>
       <c r="O48" t="s" s="2">
         <v>45</v>
       </c>
@@ -7616,17 +7626,19 @@
         <v>45</v>
       </c>
       <c r="AA48" t="s" s="2">
-        <v>325</v>
-      </c>
-      <c r="AB48" s="2"/>
+        <v>45</v>
+      </c>
+      <c r="AB48" t="s" s="2">
+        <v>45</v>
+      </c>
       <c r="AC48" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AD48" t="s" s="2">
-        <v>326</v>
+        <v>45</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>43</v>
@@ -7635,7 +7647,7 @@
         <v>55</v>
       </c>
       <c r="AH48" t="s" s="2">
-        <v>355</v>
+        <v>45</v>
       </c>
       <c r="AI48" t="s" s="2">
         <v>67</v>
@@ -7644,28 +7656,26 @@
         <v>45</v>
       </c>
       <c r="AK48" t="s" s="2">
-        <v>356</v>
+        <v>45</v>
       </c>
       <c r="AL48" t="s" s="2">
-        <v>357</v>
+        <v>344</v>
       </c>
       <c r="AM48" t="s" s="2">
-        <v>358</v>
+        <v>345</v>
       </c>
       <c r="AN48" t="s" s="2">
-        <v>45</v>
+        <v>346</v>
       </c>
       <c r="AO48" t="s" s="2">
-        <v>359</v>
+        <v>45</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>350</v>
-      </c>
-      <c r="B49" t="s" s="2">
-        <v>360</v>
-      </c>
+        <v>347</v>
+      </c>
+      <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
         <v>45</v>
       </c>
@@ -7674,10 +7684,10 @@
         <v>43</v>
       </c>
       <c r="F49" t="s" s="2">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="G49" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="H49" t="s" s="2">
         <v>45</v>
@@ -7686,19 +7696,17 @@
         <v>56</v>
       </c>
       <c r="J49" t="s" s="2">
+        <v>348</v>
+      </c>
+      <c r="K49" t="s" s="2">
+        <v>349</v>
+      </c>
+      <c r="L49" t="s" s="2">
+        <v>350</v>
+      </c>
+      <c r="M49" s="2"/>
+      <c r="N49" t="s" s="2">
         <v>351</v>
-      </c>
-      <c r="K49" t="s" s="2">
-        <v>352</v>
-      </c>
-      <c r="L49" t="s" s="2">
-        <v>352</v>
-      </c>
-      <c r="M49" t="s" s="2">
-        <v>353</v>
-      </c>
-      <c r="N49" t="s" s="2">
-        <v>354</v>
       </c>
       <c r="O49" t="s" s="2">
         <v>45</v>
@@ -7747,42 +7755,42 @@
         <v>45</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG49" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH49" t="s" s="2">
-        <v>355</v>
+        <v>45</v>
       </c>
       <c r="AI49" t="s" s="2">
         <v>67</v>
       </c>
       <c r="AJ49" t="s" s="2">
-        <v>45</v>
+        <v>352</v>
       </c>
       <c r="AK49" t="s" s="2">
-        <v>356</v>
+        <v>45</v>
       </c>
       <c r="AL49" t="s" s="2">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="AM49" t="s" s="2">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="AN49" t="s" s="2">
-        <v>45</v>
+        <v>355</v>
       </c>
       <c r="AO49" t="s" s="2">
-        <v>359</v>
+        <v>45</v>
       </c>
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
@@ -7796,25 +7804,29 @@
         <v>55</v>
       </c>
       <c r="G50" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="H50" t="s" s="2">
         <v>45</v>
       </c>
       <c r="I50" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J50" t="s" s="2">
-        <v>57</v>
+        <v>357</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>69</v>
+        <v>358</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>70</v>
-      </c>
-      <c r="M50" s="2"/>
-      <c r="N50" s="2"/>
+        <v>358</v>
+      </c>
+      <c r="M50" t="s" s="2">
+        <v>359</v>
+      </c>
+      <c r="N50" t="s" s="2">
+        <v>360</v>
+      </c>
       <c r="O50" t="s" s="2">
         <v>45</v>
       </c>
@@ -7850,19 +7862,17 @@
         <v>45</v>
       </c>
       <c r="AA50" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AB50" t="s" s="2">
-        <v>45</v>
-      </c>
+        <v>332</v>
+      </c>
+      <c r="AB50" s="2"/>
       <c r="AC50" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AD50" t="s" s="2">
-        <v>45</v>
+        <v>292</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>71</v>
+        <v>356</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>43</v>
@@ -7871,67 +7881,71 @@
         <v>55</v>
       </c>
       <c r="AH50" t="s" s="2">
-        <v>45</v>
+        <v>361</v>
       </c>
       <c r="AI50" t="s" s="2">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="AJ50" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AK50" t="s" s="2">
-        <v>45</v>
+        <v>362</v>
       </c>
       <c r="AL50" t="s" s="2">
-        <v>45</v>
+        <v>363</v>
       </c>
       <c r="AM50" t="s" s="2">
-        <v>72</v>
+        <v>364</v>
       </c>
       <c r="AN50" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO50" t="s" s="2">
-        <v>45</v>
+        <v>365</v>
       </c>
     </row>
-    <row r="51" hidden="true">
+    <row r="51">
       <c r="A51" t="s" s="2">
-        <v>362</v>
-      </c>
-      <c r="B51" s="2"/>
+        <v>356</v>
+      </c>
+      <c r="B51" t="s" s="2">
+        <v>366</v>
+      </c>
       <c r="C51" t="s" s="2">
-        <v>74</v>
+        <v>45</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F51" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G51" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="H51" t="s" s="2">
         <v>45</v>
       </c>
       <c r="I51" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J51" t="s" s="2">
-        <v>75</v>
+        <v>357</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>76</v>
+        <v>358</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>77</v>
+        <v>358</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="N51" s="2"/>
+        <v>359</v>
+      </c>
+      <c r="N51" t="s" s="2">
+        <v>360</v>
+      </c>
       <c r="O51" t="s" s="2">
         <v>45</v>
       </c>
@@ -7967,54 +7981,54 @@
         <v>45</v>
       </c>
       <c r="AA51" t="s" s="2">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="AB51" t="s" s="2">
-        <v>80</v>
+        <v>45</v>
       </c>
       <c r="AC51" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AD51" t="s" s="2">
-        <v>81</v>
+        <v>45</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>82</v>
+        <v>356</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG51" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH51" t="s" s="2">
-        <v>45</v>
+        <v>361</v>
       </c>
       <c r="AI51" t="s" s="2">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="AJ51" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AK51" t="s" s="2">
-        <v>45</v>
+        <v>362</v>
       </c>
       <c r="AL51" t="s" s="2">
-        <v>45</v>
+        <v>363</v>
       </c>
       <c r="AM51" t="s" s="2">
-        <v>72</v>
+        <v>364</v>
       </c>
       <c r="AN51" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO51" t="s" s="2">
-        <v>45</v>
+        <v>365</v>
       </c>
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>363</v>
+        <v>367</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
@@ -8034,23 +8048,19 @@
         <v>45</v>
       </c>
       <c r="I52" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J52" t="s" s="2">
-        <v>364</v>
+        <v>57</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>365</v>
+        <v>69</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>366</v>
-      </c>
-      <c r="M52" t="s" s="2">
-        <v>367</v>
-      </c>
-      <c r="N52" t="s" s="2">
-        <v>368</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="M52" s="2"/>
+      <c r="N52" s="2"/>
       <c r="O52" t="s" s="2">
         <v>45</v>
       </c>
@@ -8098,7 +8108,7 @@
         <v>45</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>369</v>
+        <v>71</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>43</v>
@@ -8110,7 +8120,7 @@
         <v>45</v>
       </c>
       <c r="AI52" t="s" s="2">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="AJ52" t="s" s="2">
         <v>45</v>
@@ -8119,10 +8129,10 @@
         <v>45</v>
       </c>
       <c r="AL52" t="s" s="2">
-        <v>370</v>
+        <v>45</v>
       </c>
       <c r="AM52" t="s" s="2">
-        <v>371</v>
+        <v>72</v>
       </c>
       <c r="AN52" t="s" s="2">
         <v>45</v>
@@ -8133,47 +8143,45 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
-        <v>45</v>
+        <v>74</v>
       </c>
       <c r="D53" s="2"/>
       <c r="E53" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F53" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G53" t="s" s="2">
         <v>45</v>
       </c>
       <c r="H53" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="I53" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J53" t="s" s="2">
-        <v>132</v>
+        <v>75</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>373</v>
+        <v>76</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>374</v>
-      </c>
-      <c r="M53" s="2"/>
-      <c r="N53" t="s" s="2">
-        <v>375</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="M53" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="N53" s="2"/>
       <c r="O53" t="s" s="2">
         <v>45</v>
       </c>
-      <c r="P53" t="s" s="2">
-        <v>376</v>
-      </c>
+      <c r="P53" s="2"/>
       <c r="Q53" t="s" s="2">
         <v>45</v>
       </c>
@@ -8193,43 +8201,43 @@
         <v>45</v>
       </c>
       <c r="W53" t="s" s="2">
-        <v>194</v>
+        <v>45</v>
       </c>
       <c r="X53" t="s" s="2">
-        <v>377</v>
+        <v>45</v>
       </c>
       <c r="Y53" t="s" s="2">
-        <v>378</v>
+        <v>45</v>
       </c>
       <c r="Z53" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AA53" t="s" s="2">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="AB53" t="s" s="2">
-        <v>45</v>
+        <v>80</v>
       </c>
       <c r="AC53" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AD53" t="s" s="2">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="AE53" t="s" s="2">
-        <v>379</v>
+        <v>82</v>
       </c>
       <c r="AF53" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG53" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH53" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI53" t="s" s="2">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="AJ53" t="s" s="2">
         <v>45</v>
@@ -8238,10 +8246,10 @@
         <v>45</v>
       </c>
       <c r="AL53" t="s" s="2">
-        <v>380</v>
+        <v>45</v>
       </c>
       <c r="AM53" t="s" s="2">
-        <v>381</v>
+        <v>72</v>
       </c>
       <c r="AN53" t="s" s="2">
         <v>45</v>
@@ -8252,7 +8260,7 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>382</v>
+        <v>369</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
@@ -8275,17 +8283,19 @@
         <v>56</v>
       </c>
       <c r="J54" t="s" s="2">
-        <v>57</v>
+        <v>370</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>383</v>
+        <v>371</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>384</v>
-      </c>
-      <c r="M54" s="2"/>
+        <v>372</v>
+      </c>
+      <c r="M54" t="s" s="2">
+        <v>373</v>
+      </c>
       <c r="N54" t="s" s="2">
-        <v>385</v>
+        <v>374</v>
       </c>
       <c r="O54" t="s" s="2">
         <v>45</v>
@@ -8295,7 +8305,7 @@
         <v>45</v>
       </c>
       <c r="R54" t="s" s="2">
-        <v>386</v>
+        <v>45</v>
       </c>
       <c r="S54" t="s" s="2">
         <v>45</v>
@@ -8334,7 +8344,7 @@
         <v>45</v>
       </c>
       <c r="AE54" t="s" s="2">
-        <v>387</v>
+        <v>375</v>
       </c>
       <c r="AF54" t="s" s="2">
         <v>43</v>
@@ -8355,10 +8365,10 @@
         <v>45</v>
       </c>
       <c r="AL54" t="s" s="2">
-        <v>388</v>
+        <v>376</v>
       </c>
       <c r="AM54" t="s" s="2">
-        <v>389</v>
+        <v>377</v>
       </c>
       <c r="AN54" t="s" s="2">
         <v>45</v>
@@ -8369,7 +8379,7 @@
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>390</v>
+        <v>378</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" t="s" s="2">
@@ -8386,28 +8396,30 @@
         <v>45</v>
       </c>
       <c r="H55" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="I55" t="s" s="2">
         <v>56</v>
       </c>
       <c r="J55" t="s" s="2">
-        <v>97</v>
+        <v>132</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>391</v>
+        <v>379</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="M55" s="2"/>
       <c r="N55" t="s" s="2">
-        <v>393</v>
+        <v>381</v>
       </c>
       <c r="O55" t="s" s="2">
         <v>45</v>
       </c>
-      <c r="P55" s="2"/>
+      <c r="P55" t="s" s="2">
+        <v>382</v>
+      </c>
       <c r="Q55" t="s" s="2">
         <v>45</v>
       </c>
@@ -8427,13 +8439,13 @@
         <v>45</v>
       </c>
       <c r="W55" t="s" s="2">
-        <v>45</v>
+        <v>194</v>
       </c>
       <c r="X55" t="s" s="2">
-        <v>45</v>
+        <v>383</v>
       </c>
       <c r="Y55" t="s" s="2">
-        <v>45</v>
+        <v>384</v>
       </c>
       <c r="Z55" t="s" s="2">
         <v>45</v>
@@ -8451,7 +8463,7 @@
         <v>45</v>
       </c>
       <c r="AE55" t="s" s="2">
-        <v>394</v>
+        <v>385</v>
       </c>
       <c r="AF55" t="s" s="2">
         <v>43</v>
@@ -8460,7 +8472,7 @@
         <v>55</v>
       </c>
       <c r="AH55" t="s" s="2">
-        <v>395</v>
+        <v>45</v>
       </c>
       <c r="AI55" t="s" s="2">
         <v>67</v>
@@ -8472,10 +8484,10 @@
         <v>45</v>
       </c>
       <c r="AL55" t="s" s="2">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="AM55" t="s" s="2">
-        <v>396</v>
+        <v>387</v>
       </c>
       <c r="AN55" t="s" s="2">
         <v>45</v>
@@ -8486,7 +8498,7 @@
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>397</v>
+        <v>388</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
@@ -8509,19 +8521,17 @@
         <v>56</v>
       </c>
       <c r="J56" t="s" s="2">
-        <v>132</v>
+        <v>57</v>
       </c>
       <c r="K56" t="s" s="2">
-        <v>398</v>
+        <v>389</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>399</v>
-      </c>
-      <c r="M56" t="s" s="2">
-        <v>400</v>
-      </c>
+        <v>390</v>
+      </c>
+      <c r="M56" s="2"/>
       <c r="N56" t="s" s="2">
-        <v>401</v>
+        <v>391</v>
       </c>
       <c r="O56" t="s" s="2">
         <v>45</v>
@@ -8531,7 +8541,7 @@
         <v>45</v>
       </c>
       <c r="R56" t="s" s="2">
-        <v>45</v>
+        <v>392</v>
       </c>
       <c r="S56" t="s" s="2">
         <v>45</v>
@@ -8570,7 +8580,7 @@
         <v>45</v>
       </c>
       <c r="AE56" t="s" s="2">
-        <v>402</v>
+        <v>393</v>
       </c>
       <c r="AF56" t="s" s="2">
         <v>43</v>
@@ -8591,10 +8601,10 @@
         <v>45</v>
       </c>
       <c r="AL56" t="s" s="2">
-        <v>388</v>
+        <v>394</v>
       </c>
       <c r="AM56" t="s" s="2">
-        <v>403</v>
+        <v>395</v>
       </c>
       <c r="AN56" t="s" s="2">
         <v>45</v>
@@ -8603,9 +8613,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
@@ -8616,31 +8626,29 @@
         <v>43</v>
       </c>
       <c r="F57" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="G57" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="H57" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="I57" t="s" s="2">
         <v>56</v>
       </c>
-      <c r="H57" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="I57" t="s" s="2">
-        <v>45</v>
-      </c>
       <c r="J57" t="s" s="2">
-        <v>202</v>
+        <v>97</v>
       </c>
       <c r="K57" t="s" s="2">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="L57" t="s" s="2">
-        <v>406</v>
-      </c>
-      <c r="M57" t="s" s="2">
-        <v>407</v>
-      </c>
+        <v>398</v>
+      </c>
+      <c r="M57" s="2"/>
       <c r="N57" t="s" s="2">
-        <v>408</v>
+        <v>399</v>
       </c>
       <c r="O57" t="s" s="2">
         <v>45</v>
@@ -8665,13 +8673,13 @@
         <v>45</v>
       </c>
       <c r="W57" t="s" s="2">
-        <v>113</v>
+        <v>45</v>
       </c>
       <c r="X57" t="s" s="2">
-        <v>409</v>
+        <v>45</v>
       </c>
       <c r="Y57" t="s" s="2">
-        <v>410</v>
+        <v>45</v>
       </c>
       <c r="Z57" t="s" s="2">
         <v>45</v>
@@ -8689,7 +8697,7 @@
         <v>45</v>
       </c>
       <c r="AE57" t="s" s="2">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="AF57" t="s" s="2">
         <v>43</v>
@@ -8698,7 +8706,7 @@
         <v>55</v>
       </c>
       <c r="AH57" t="s" s="2">
-        <v>411</v>
+        <v>401</v>
       </c>
       <c r="AI57" t="s" s="2">
         <v>67</v>
@@ -8710,10 +8718,10 @@
         <v>45</v>
       </c>
       <c r="AL57" t="s" s="2">
-        <v>155</v>
+        <v>394</v>
       </c>
       <c r="AM57" t="s" s="2">
-        <v>412</v>
+        <v>402</v>
       </c>
       <c r="AN57" t="s" s="2">
         <v>45</v>
@@ -8724,18 +8732,18 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>413</v>
+        <v>403</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
-        <v>414</v>
+        <v>45</v>
       </c>
       <c r="D58" s="2"/>
       <c r="E58" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F58" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="G58" t="s" s="2">
         <v>45</v>
@@ -8744,22 +8752,22 @@
         <v>45</v>
       </c>
       <c r="I58" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J58" t="s" s="2">
-        <v>202</v>
+        <v>132</v>
       </c>
       <c r="K58" t="s" s="2">
-        <v>415</v>
+        <v>404</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>416</v>
+        <v>405</v>
       </c>
       <c r="M58" t="s" s="2">
-        <v>417</v>
+        <v>406</v>
       </c>
       <c r="N58" t="s" s="2">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="O58" t="s" s="2">
         <v>45</v>
@@ -8784,13 +8792,13 @@
         <v>45</v>
       </c>
       <c r="W58" t="s" s="2">
-        <v>113</v>
+        <v>45</v>
       </c>
       <c r="X58" t="s" s="2">
-        <v>419</v>
+        <v>45</v>
       </c>
       <c r="Y58" t="s" s="2">
-        <v>420</v>
+        <v>45</v>
       </c>
       <c r="Z58" t="s" s="2">
         <v>45</v>
@@ -8808,13 +8816,13 @@
         <v>45</v>
       </c>
       <c r="AE58" t="s" s="2">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="AF58" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG58" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH58" t="s" s="2">
         <v>45</v>
@@ -8826,24 +8834,24 @@
         <v>45</v>
       </c>
       <c r="AK58" t="s" s="2">
-        <v>421</v>
+        <v>45</v>
       </c>
       <c r="AL58" t="s" s="2">
-        <v>422</v>
+        <v>394</v>
       </c>
       <c r="AM58" t="s" s="2">
-        <v>423</v>
+        <v>409</v>
       </c>
       <c r="AN58" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO58" t="s" s="2">
-        <v>424</v>
+        <v>45</v>
       </c>
     </row>
-    <row r="59" hidden="true">
+    <row r="59">
       <c r="A59" t="s" s="2">
-        <v>425</v>
+        <v>410</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
@@ -8854,10 +8862,10 @@
         <v>43</v>
       </c>
       <c r="F59" t="s" s="2">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="G59" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="H59" t="s" s="2">
         <v>45</v>
@@ -8866,19 +8874,19 @@
         <v>45</v>
       </c>
       <c r="J59" t="s" s="2">
-        <v>426</v>
+        <v>202</v>
       </c>
       <c r="K59" t="s" s="2">
-        <v>427</v>
+        <v>411</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>428</v>
+        <v>412</v>
       </c>
       <c r="M59" t="s" s="2">
-        <v>429</v>
+        <v>413</v>
       </c>
       <c r="N59" t="s" s="2">
-        <v>430</v>
+        <v>414</v>
       </c>
       <c r="O59" t="s" s="2">
         <v>45</v>
@@ -8903,13 +8911,13 @@
         <v>45</v>
       </c>
       <c r="W59" t="s" s="2">
-        <v>45</v>
+        <v>113</v>
       </c>
       <c r="X59" t="s" s="2">
-        <v>45</v>
+        <v>415</v>
       </c>
       <c r="Y59" t="s" s="2">
-        <v>45</v>
+        <v>416</v>
       </c>
       <c r="Z59" t="s" s="2">
         <v>45</v>
@@ -8927,16 +8935,16 @@
         <v>45</v>
       </c>
       <c r="AE59" t="s" s="2">
-        <v>425</v>
+        <v>410</v>
       </c>
       <c r="AF59" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG59" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH59" t="s" s="2">
-        <v>45</v>
+        <v>417</v>
       </c>
       <c r="AI59" t="s" s="2">
         <v>67</v>
@@ -8948,10 +8956,10 @@
         <v>45</v>
       </c>
       <c r="AL59" t="s" s="2">
-        <v>431</v>
+        <v>155</v>
       </c>
       <c r="AM59" t="s" s="2">
-        <v>432</v>
+        <v>418</v>
       </c>
       <c r="AN59" t="s" s="2">
         <v>45</v>
@@ -8962,11 +8970,11 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>433</v>
+        <v>419</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
-        <v>45</v>
+        <v>420</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" t="s" s="2">
@@ -8988,15 +8996,17 @@
         <v>202</v>
       </c>
       <c r="K60" t="s" s="2">
-        <v>434</v>
+        <v>421</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>435</v>
+        <v>422</v>
       </c>
       <c r="M60" t="s" s="2">
-        <v>436</v>
-      </c>
-      <c r="N60" s="2"/>
+        <v>423</v>
+      </c>
+      <c r="N60" t="s" s="2">
+        <v>424</v>
+      </c>
       <c r="O60" t="s" s="2">
         <v>45</v>
       </c>
@@ -9020,13 +9030,13 @@
         <v>45</v>
       </c>
       <c r="W60" t="s" s="2">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="X60" t="s" s="2">
-        <v>437</v>
+        <v>425</v>
       </c>
       <c r="Y60" t="s" s="2">
-        <v>438</v>
+        <v>426</v>
       </c>
       <c r="Z60" t="s" s="2">
         <v>45</v>
@@ -9044,13 +9054,13 @@
         <v>45</v>
       </c>
       <c r="AE60" t="s" s="2">
-        <v>433</v>
+        <v>419</v>
       </c>
       <c r="AF60" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG60" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH60" t="s" s="2">
         <v>45</v>
@@ -9062,24 +9072,24 @@
         <v>45</v>
       </c>
       <c r="AK60" t="s" s="2">
-        <v>439</v>
+        <v>427</v>
       </c>
       <c r="AL60" t="s" s="2">
-        <v>440</v>
+        <v>428</v>
       </c>
       <c r="AM60" t="s" s="2">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="AN60" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO60" t="s" s="2">
-        <v>442</v>
+        <v>430</v>
       </c>
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>443</v>
+        <v>431</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
@@ -9090,7 +9100,7 @@
         <v>43</v>
       </c>
       <c r="F61" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="G61" t="s" s="2">
         <v>45</v>
@@ -9102,19 +9112,19 @@
         <v>45</v>
       </c>
       <c r="J61" t="s" s="2">
-        <v>202</v>
+        <v>432</v>
       </c>
       <c r="K61" t="s" s="2">
-        <v>444</v>
+        <v>433</v>
       </c>
       <c r="L61" t="s" s="2">
-        <v>445</v>
+        <v>434</v>
       </c>
       <c r="M61" t="s" s="2">
-        <v>446</v>
+        <v>435</v>
       </c>
       <c r="N61" t="s" s="2">
-        <v>447</v>
+        <v>436</v>
       </c>
       <c r="O61" t="s" s="2">
         <v>45</v>
@@ -9139,13 +9149,13 @@
         <v>45</v>
       </c>
       <c r="W61" t="s" s="2">
-        <v>122</v>
+        <v>45</v>
       </c>
       <c r="X61" t="s" s="2">
-        <v>448</v>
+        <v>45</v>
       </c>
       <c r="Y61" t="s" s="2">
-        <v>449</v>
+        <v>45</v>
       </c>
       <c r="Z61" t="s" s="2">
         <v>45</v>
@@ -9163,13 +9173,13 @@
         <v>45</v>
       </c>
       <c r="AE61" t="s" s="2">
-        <v>443</v>
+        <v>431</v>
       </c>
       <c r="AF61" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG61" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH61" t="s" s="2">
         <v>45</v>
@@ -9184,10 +9194,10 @@
         <v>45</v>
       </c>
       <c r="AL61" t="s" s="2">
-        <v>450</v>
+        <v>437</v>
       </c>
       <c r="AM61" t="s" s="2">
-        <v>451</v>
+        <v>438</v>
       </c>
       <c r="AN61" t="s" s="2">
         <v>45</v>
@@ -9198,7 +9208,7 @@
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>452</v>
+        <v>439</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
@@ -9221,16 +9231,16 @@
         <v>45</v>
       </c>
       <c r="J62" t="s" s="2">
-        <v>453</v>
+        <v>202</v>
       </c>
       <c r="K62" t="s" s="2">
-        <v>454</v>
+        <v>440</v>
       </c>
       <c r="L62" t="s" s="2">
-        <v>455</v>
+        <v>441</v>
       </c>
       <c r="M62" t="s" s="2">
-        <v>456</v>
+        <v>442</v>
       </c>
       <c r="N62" s="2"/>
       <c r="O62" t="s" s="2">
@@ -9256,13 +9266,13 @@
         <v>45</v>
       </c>
       <c r="W62" t="s" s="2">
-        <v>45</v>
+        <v>122</v>
       </c>
       <c r="X62" t="s" s="2">
-        <v>45</v>
+        <v>443</v>
       </c>
       <c r="Y62" t="s" s="2">
-        <v>45</v>
+        <v>444</v>
       </c>
       <c r="Z62" t="s" s="2">
         <v>45</v>
@@ -9280,7 +9290,7 @@
         <v>45</v>
       </c>
       <c r="AE62" t="s" s="2">
-        <v>452</v>
+        <v>439</v>
       </c>
       <c r="AF62" t="s" s="2">
         <v>43</v>
@@ -9298,24 +9308,24 @@
         <v>45</v>
       </c>
       <c r="AK62" t="s" s="2">
-        <v>457</v>
+        <v>445</v>
       </c>
       <c r="AL62" t="s" s="2">
-        <v>458</v>
+        <v>446</v>
       </c>
       <c r="AM62" t="s" s="2">
-        <v>459</v>
+        <v>447</v>
       </c>
       <c r="AN62" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO62" t="s" s="2">
-        <v>460</v>
+        <v>448</v>
       </c>
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>461</v>
+        <v>449</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" t="s" s="2">
@@ -9338,18 +9348,20 @@
         <v>45</v>
       </c>
       <c r="J63" t="s" s="2">
-        <v>462</v>
+        <v>202</v>
       </c>
       <c r="K63" t="s" s="2">
-        <v>463</v>
+        <v>450</v>
       </c>
       <c r="L63" t="s" s="2">
-        <v>464</v>
+        <v>451</v>
       </c>
       <c r="M63" t="s" s="2">
-        <v>465</v>
-      </c>
-      <c r="N63" s="2"/>
+        <v>452</v>
+      </c>
+      <c r="N63" t="s" s="2">
+        <v>453</v>
+      </c>
       <c r="O63" t="s" s="2">
         <v>45</v>
       </c>
@@ -9373,13 +9385,13 @@
         <v>45</v>
       </c>
       <c r="W63" t="s" s="2">
-        <v>45</v>
+        <v>122</v>
       </c>
       <c r="X63" t="s" s="2">
-        <v>45</v>
+        <v>454</v>
       </c>
       <c r="Y63" t="s" s="2">
-        <v>45</v>
+        <v>455</v>
       </c>
       <c r="Z63" t="s" s="2">
         <v>45</v>
@@ -9397,7 +9409,7 @@
         <v>45</v>
       </c>
       <c r="AE63" t="s" s="2">
-        <v>461</v>
+        <v>449</v>
       </c>
       <c r="AF63" t="s" s="2">
         <v>43</v>
@@ -9415,24 +9427,24 @@
         <v>45</v>
       </c>
       <c r="AK63" t="s" s="2">
-        <v>466</v>
+        <v>45</v>
       </c>
       <c r="AL63" t="s" s="2">
-        <v>467</v>
+        <v>456</v>
       </c>
       <c r="AM63" t="s" s="2">
-        <v>468</v>
+        <v>457</v>
       </c>
       <c r="AN63" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO63" t="s" s="2">
-        <v>469</v>
+        <v>45</v>
       </c>
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>470</v>
+        <v>458</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" t="s" s="2">
@@ -9455,20 +9467,18 @@
         <v>45</v>
       </c>
       <c r="J64" t="s" s="2">
-        <v>471</v>
+        <v>459</v>
       </c>
       <c r="K64" t="s" s="2">
-        <v>472</v>
+        <v>460</v>
       </c>
       <c r="L64" t="s" s="2">
-        <v>473</v>
+        <v>461</v>
       </c>
       <c r="M64" t="s" s="2">
-        <v>474</v>
-      </c>
-      <c r="N64" t="s" s="2">
-        <v>475</v>
-      </c>
+        <v>462</v>
+      </c>
+      <c r="N64" s="2"/>
       <c r="O64" t="s" s="2">
         <v>45</v>
       </c>
@@ -9516,42 +9526,42 @@
         <v>45</v>
       </c>
       <c r="AE64" t="s" s="2">
-        <v>470</v>
+        <v>458</v>
       </c>
       <c r="AF64" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG64" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH64" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI64" t="s" s="2">
-        <v>476</v>
+        <v>67</v>
       </c>
       <c r="AJ64" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AK64" t="s" s="2">
-        <v>45</v>
+        <v>463</v>
       </c>
       <c r="AL64" t="s" s="2">
-        <v>477</v>
+        <v>464</v>
       </c>
       <c r="AM64" t="s" s="2">
-        <v>478</v>
+        <v>465</v>
       </c>
       <c r="AN64" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO64" t="s" s="2">
-        <v>45</v>
+        <v>466</v>
       </c>
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>479</v>
+        <v>467</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" t="s" s="2">
@@ -9562,7 +9572,7 @@
         <v>43</v>
       </c>
       <c r="F65" t="s" s="2">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="G65" t="s" s="2">
         <v>45</v>
@@ -9574,15 +9584,17 @@
         <v>45</v>
       </c>
       <c r="J65" t="s" s="2">
-        <v>57</v>
+        <v>468</v>
       </c>
       <c r="K65" t="s" s="2">
-        <v>69</v>
+        <v>469</v>
       </c>
       <c r="L65" t="s" s="2">
-        <v>70</v>
-      </c>
-      <c r="M65" s="2"/>
+        <v>470</v>
+      </c>
+      <c r="M65" t="s" s="2">
+        <v>471</v>
+      </c>
       <c r="N65" s="2"/>
       <c r="O65" t="s" s="2">
         <v>45</v>
@@ -9631,7 +9643,7 @@
         <v>45</v>
       </c>
       <c r="AE65" t="s" s="2">
-        <v>71</v>
+        <v>467</v>
       </c>
       <c r="AF65" t="s" s="2">
         <v>43</v>
@@ -9643,41 +9655,41 @@
         <v>45</v>
       </c>
       <c r="AI65" t="s" s="2">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="AJ65" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AK65" t="s" s="2">
-        <v>45</v>
+        <v>472</v>
       </c>
       <c r="AL65" t="s" s="2">
-        <v>45</v>
+        <v>473</v>
       </c>
       <c r="AM65" t="s" s="2">
-        <v>72</v>
+        <v>474</v>
       </c>
       <c r="AN65" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO65" t="s" s="2">
-        <v>45</v>
+        <v>475</v>
       </c>
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" t="s" s="2">
-        <v>74</v>
+        <v>45</v>
       </c>
       <c r="D66" s="2"/>
       <c r="E66" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F66" t="s" s="2">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G66" t="s" s="2">
         <v>45</v>
@@ -9689,18 +9701,20 @@
         <v>45</v>
       </c>
       <c r="J66" t="s" s="2">
-        <v>75</v>
+        <v>477</v>
       </c>
       <c r="K66" t="s" s="2">
-        <v>76</v>
+        <v>478</v>
       </c>
       <c r="L66" t="s" s="2">
-        <v>77</v>
+        <v>479</v>
       </c>
       <c r="M66" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="N66" s="2"/>
+        <v>480</v>
+      </c>
+      <c r="N66" t="s" s="2">
+        <v>481</v>
+      </c>
       <c r="O66" t="s" s="2">
         <v>45</v>
       </c>
@@ -9748,7 +9762,7 @@
         <v>45</v>
       </c>
       <c r="AE66" t="s" s="2">
-        <v>82</v>
+        <v>476</v>
       </c>
       <c r="AF66" t="s" s="2">
         <v>43</v>
@@ -9760,7 +9774,7 @@
         <v>45</v>
       </c>
       <c r="AI66" t="s" s="2">
-        <v>83</v>
+        <v>482</v>
       </c>
       <c r="AJ66" t="s" s="2">
         <v>45</v>
@@ -9769,10 +9783,10 @@
         <v>45</v>
       </c>
       <c r="AL66" t="s" s="2">
-        <v>45</v>
+        <v>483</v>
       </c>
       <c r="AM66" t="s" s="2">
-        <v>72</v>
+        <v>484</v>
       </c>
       <c r="AN66" t="s" s="2">
         <v>45</v>
@@ -9783,43 +9797,39 @@
     </row>
     <row r="67" hidden="true">
       <c r="A67" t="s" s="2">
-        <v>481</v>
+        <v>485</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" t="s" s="2">
-        <v>482</v>
+        <v>45</v>
       </c>
       <c r="D67" s="2"/>
       <c r="E67" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F67" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G67" t="s" s="2">
         <v>45</v>
       </c>
       <c r="H67" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="I67" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J67" t="s" s="2">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="K67" t="s" s="2">
-        <v>483</v>
+        <v>69</v>
       </c>
       <c r="L67" t="s" s="2">
-        <v>484</v>
-      </c>
-      <c r="M67" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="N67" t="s" s="2">
-        <v>485</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="M67" s="2"/>
+      <c r="N67" s="2"/>
       <c r="O67" t="s" s="2">
         <v>45</v>
       </c>
@@ -9867,19 +9877,19 @@
         <v>45</v>
       </c>
       <c r="AE67" t="s" s="2">
-        <v>486</v>
+        <v>71</v>
       </c>
       <c r="AF67" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG67" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH67" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI67" t="s" s="2">
-        <v>83</v>
+        <v>45</v>
       </c>
       <c r="AJ67" t="s" s="2">
         <v>45</v>
@@ -9891,7 +9901,7 @@
         <v>45</v>
       </c>
       <c r="AM67" t="s" s="2">
-        <v>155</v>
+        <v>72</v>
       </c>
       <c r="AN67" t="s" s="2">
         <v>45</v>
@@ -9902,18 +9912,18 @@
     </row>
     <row r="68" hidden="true">
       <c r="A68" t="s" s="2">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B68" s="2"/>
       <c r="C68" t="s" s="2">
-        <v>45</v>
+        <v>74</v>
       </c>
       <c r="D68" s="2"/>
       <c r="E68" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F68" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G68" t="s" s="2">
         <v>45</v>
@@ -9925,15 +9935,17 @@
         <v>45</v>
       </c>
       <c r="J68" t="s" s="2">
-        <v>488</v>
+        <v>75</v>
       </c>
       <c r="K68" t="s" s="2">
-        <v>489</v>
+        <v>76</v>
       </c>
       <c r="L68" t="s" s="2">
-        <v>490</v>
-      </c>
-      <c r="M68" s="2"/>
+        <v>77</v>
+      </c>
+      <c r="M68" t="s" s="2">
+        <v>78</v>
+      </c>
       <c r="N68" s="2"/>
       <c r="O68" t="s" s="2">
         <v>45</v>
@@ -9982,19 +9994,19 @@
         <v>45</v>
       </c>
       <c r="AE68" t="s" s="2">
-        <v>487</v>
+        <v>82</v>
       </c>
       <c r="AF68" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG68" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH68" t="s" s="2">
-        <v>491</v>
+        <v>45</v>
       </c>
       <c r="AI68" t="s" s="2">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="AJ68" t="s" s="2">
         <v>45</v>
@@ -10003,10 +10015,10 @@
         <v>45</v>
       </c>
       <c r="AL68" t="s" s="2">
-        <v>492</v>
+        <v>45</v>
       </c>
       <c r="AM68" t="s" s="2">
-        <v>493</v>
+        <v>72</v>
       </c>
       <c r="AN68" t="s" s="2">
         <v>45</v>
@@ -10017,39 +10029,43 @@
     </row>
     <row r="69" hidden="true">
       <c r="A69" t="s" s="2">
-        <v>494</v>
+        <v>487</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" t="s" s="2">
-        <v>45</v>
+        <v>488</v>
       </c>
       <c r="D69" s="2"/>
       <c r="E69" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F69" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G69" t="s" s="2">
         <v>45</v>
       </c>
       <c r="H69" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="I69" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J69" t="s" s="2">
-        <v>488</v>
+        <v>75</v>
       </c>
       <c r="K69" t="s" s="2">
-        <v>495</v>
+        <v>489</v>
       </c>
       <c r="L69" t="s" s="2">
-        <v>496</v>
-      </c>
-      <c r="M69" s="2"/>
-      <c r="N69" s="2"/>
+        <v>490</v>
+      </c>
+      <c r="M69" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="N69" t="s" s="2">
+        <v>491</v>
+      </c>
       <c r="O69" t="s" s="2">
         <v>45</v>
       </c>
@@ -10097,19 +10113,19 @@
         <v>45</v>
       </c>
       <c r="AE69" t="s" s="2">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="AF69" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG69" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH69" t="s" s="2">
-        <v>491</v>
+        <v>45</v>
       </c>
       <c r="AI69" t="s" s="2">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="AJ69" t="s" s="2">
         <v>45</v>
@@ -10118,10 +10134,10 @@
         <v>45</v>
       </c>
       <c r="AL69" t="s" s="2">
-        <v>492</v>
+        <v>45</v>
       </c>
       <c r="AM69" t="s" s="2">
-        <v>497</v>
+        <v>155</v>
       </c>
       <c r="AN69" t="s" s="2">
         <v>45</v>
@@ -10132,7 +10148,7 @@
     </row>
     <row r="70" hidden="true">
       <c r="A70" t="s" s="2">
-        <v>498</v>
+        <v>493</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" t="s" s="2">
@@ -10155,20 +10171,16 @@
         <v>45</v>
       </c>
       <c r="J70" t="s" s="2">
-        <v>202</v>
+        <v>494</v>
       </c>
       <c r="K70" t="s" s="2">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="L70" t="s" s="2">
-        <v>500</v>
-      </c>
-      <c r="M70" t="s" s="2">
-        <v>501</v>
-      </c>
-      <c r="N70" t="s" s="2">
-        <v>502</v>
-      </c>
+        <v>496</v>
+      </c>
+      <c r="M70" s="2"/>
+      <c r="N70" s="2"/>
       <c r="O70" t="s" s="2">
         <v>45</v>
       </c>
@@ -10192,13 +10204,13 @@
         <v>45</v>
       </c>
       <c r="W70" t="s" s="2">
-        <v>136</v>
+        <v>45</v>
       </c>
       <c r="X70" t="s" s="2">
-        <v>503</v>
+        <v>45</v>
       </c>
       <c r="Y70" t="s" s="2">
-        <v>504</v>
+        <v>45</v>
       </c>
       <c r="Z70" t="s" s="2">
         <v>45</v>
@@ -10216,7 +10228,7 @@
         <v>45</v>
       </c>
       <c r="AE70" t="s" s="2">
-        <v>498</v>
+        <v>493</v>
       </c>
       <c r="AF70" t="s" s="2">
         <v>43</v>
@@ -10225,7 +10237,7 @@
         <v>55</v>
       </c>
       <c r="AH70" t="s" s="2">
-        <v>45</v>
+        <v>497</v>
       </c>
       <c r="AI70" t="s" s="2">
         <v>67</v>
@@ -10234,13 +10246,13 @@
         <v>45</v>
       </c>
       <c r="AK70" t="s" s="2">
-        <v>505</v>
+        <v>45</v>
       </c>
       <c r="AL70" t="s" s="2">
-        <v>506</v>
+        <v>498</v>
       </c>
       <c r="AM70" t="s" s="2">
-        <v>423</v>
+        <v>499</v>
       </c>
       <c r="AN70" t="s" s="2">
         <v>45</v>
@@ -10251,7 +10263,7 @@
     </row>
     <row r="71" hidden="true">
       <c r="A71" t="s" s="2">
-        <v>507</v>
+        <v>500</v>
       </c>
       <c r="B71" s="2"/>
       <c r="C71" t="s" s="2">
@@ -10262,7 +10274,7 @@
         <v>43</v>
       </c>
       <c r="F71" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G71" t="s" s="2">
         <v>45</v>
@@ -10274,20 +10286,16 @@
         <v>45</v>
       </c>
       <c r="J71" t="s" s="2">
-        <v>202</v>
+        <v>494</v>
       </c>
       <c r="K71" t="s" s="2">
-        <v>508</v>
+        <v>501</v>
       </c>
       <c r="L71" t="s" s="2">
-        <v>509</v>
-      </c>
-      <c r="M71" t="s" s="2">
-        <v>510</v>
-      </c>
-      <c r="N71" t="s" s="2">
-        <v>511</v>
-      </c>
+        <v>502</v>
+      </c>
+      <c r="M71" s="2"/>
+      <c r="N71" s="2"/>
       <c r="O71" t="s" s="2">
         <v>45</v>
       </c>
@@ -10311,13 +10319,13 @@
         <v>45</v>
       </c>
       <c r="W71" t="s" s="2">
-        <v>122</v>
+        <v>45</v>
       </c>
       <c r="X71" t="s" s="2">
-        <v>512</v>
+        <v>45</v>
       </c>
       <c r="Y71" t="s" s="2">
-        <v>513</v>
+        <v>45</v>
       </c>
       <c r="Z71" t="s" s="2">
         <v>45</v>
@@ -10335,16 +10343,16 @@
         <v>45</v>
       </c>
       <c r="AE71" t="s" s="2">
-        <v>507</v>
+        <v>500</v>
       </c>
       <c r="AF71" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG71" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH71" t="s" s="2">
-        <v>45</v>
+        <v>497</v>
       </c>
       <c r="AI71" t="s" s="2">
         <v>67</v>
@@ -10353,13 +10361,13 @@
         <v>45</v>
       </c>
       <c r="AK71" t="s" s="2">
-        <v>505</v>
+        <v>45</v>
       </c>
       <c r="AL71" t="s" s="2">
-        <v>506</v>
+        <v>498</v>
       </c>
       <c r="AM71" t="s" s="2">
-        <v>423</v>
+        <v>503</v>
       </c>
       <c r="AN71" t="s" s="2">
         <v>45</v>
@@ -10370,7 +10378,7 @@
     </row>
     <row r="72" hidden="true">
       <c r="A72" t="s" s="2">
-        <v>514</v>
+        <v>504</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" t="s" s="2">
@@ -10393,17 +10401,19 @@
         <v>45</v>
       </c>
       <c r="J72" t="s" s="2">
-        <v>515</v>
+        <v>202</v>
       </c>
       <c r="K72" t="s" s="2">
-        <v>516</v>
+        <v>505</v>
       </c>
       <c r="L72" t="s" s="2">
-        <v>517</v>
-      </c>
-      <c r="M72" s="2"/>
+        <v>506</v>
+      </c>
+      <c r="M72" t="s" s="2">
+        <v>507</v>
+      </c>
       <c r="N72" t="s" s="2">
-        <v>518</v>
+        <v>508</v>
       </c>
       <c r="O72" t="s" s="2">
         <v>45</v>
@@ -10428,13 +10438,13 @@
         <v>45</v>
       </c>
       <c r="W72" t="s" s="2">
-        <v>45</v>
+        <v>136</v>
       </c>
       <c r="X72" t="s" s="2">
-        <v>45</v>
+        <v>509</v>
       </c>
       <c r="Y72" t="s" s="2">
-        <v>45</v>
+        <v>510</v>
       </c>
       <c r="Z72" t="s" s="2">
         <v>45</v>
@@ -10452,7 +10462,7 @@
         <v>45</v>
       </c>
       <c r="AE72" t="s" s="2">
-        <v>514</v>
+        <v>504</v>
       </c>
       <c r="AF72" t="s" s="2">
         <v>43</v>
@@ -10470,13 +10480,13 @@
         <v>45</v>
       </c>
       <c r="AK72" t="s" s="2">
-        <v>45</v>
+        <v>511</v>
       </c>
       <c r="AL72" t="s" s="2">
-        <v>45</v>
+        <v>512</v>
       </c>
       <c r="AM72" t="s" s="2">
-        <v>519</v>
+        <v>429</v>
       </c>
       <c r="AN72" t="s" s="2">
         <v>45</v>
@@ -10487,7 +10497,7 @@
     </row>
     <row r="73" hidden="true">
       <c r="A73" t="s" s="2">
-        <v>520</v>
+        <v>513</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" t="s" s="2">
@@ -10498,7 +10508,7 @@
         <v>43</v>
       </c>
       <c r="F73" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G73" t="s" s="2">
         <v>45</v>
@@ -10510,16 +10520,20 @@
         <v>45</v>
       </c>
       <c r="J73" t="s" s="2">
-        <v>57</v>
+        <v>202</v>
       </c>
       <c r="K73" t="s" s="2">
-        <v>521</v>
+        <v>514</v>
       </c>
       <c r="L73" t="s" s="2">
-        <v>522</v>
-      </c>
-      <c r="M73" s="2"/>
-      <c r="N73" s="2"/>
+        <v>515</v>
+      </c>
+      <c r="M73" t="s" s="2">
+        <v>516</v>
+      </c>
+      <c r="N73" t="s" s="2">
+        <v>517</v>
+      </c>
       <c r="O73" t="s" s="2">
         <v>45</v>
       </c>
@@ -10543,13 +10557,13 @@
         <v>45</v>
       </c>
       <c r="W73" t="s" s="2">
-        <v>45</v>
+        <v>122</v>
       </c>
       <c r="X73" t="s" s="2">
-        <v>45</v>
+        <v>518</v>
       </c>
       <c r="Y73" t="s" s="2">
-        <v>45</v>
+        <v>519</v>
       </c>
       <c r="Z73" t="s" s="2">
         <v>45</v>
@@ -10567,13 +10581,13 @@
         <v>45</v>
       </c>
       <c r="AE73" t="s" s="2">
-        <v>520</v>
+        <v>513</v>
       </c>
       <c r="AF73" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG73" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH73" t="s" s="2">
         <v>45</v>
@@ -10585,13 +10599,13 @@
         <v>45</v>
       </c>
       <c r="AK73" t="s" s="2">
-        <v>45</v>
+        <v>511</v>
       </c>
       <c r="AL73" t="s" s="2">
-        <v>492</v>
+        <v>512</v>
       </c>
       <c r="AM73" t="s" s="2">
-        <v>523</v>
+        <v>429</v>
       </c>
       <c r="AN73" t="s" s="2">
         <v>45</v>
@@ -10602,7 +10616,7 @@
     </row>
     <row r="74" hidden="true">
       <c r="A74" t="s" s="2">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="B74" s="2"/>
       <c r="C74" t="s" s="2">
@@ -10613,30 +10627,30 @@
         <v>43</v>
       </c>
       <c r="F74" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G74" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="H74" t="s" s="2">
         <v>45</v>
       </c>
       <c r="I74" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J74" t="s" s="2">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="K74" t="s" s="2">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="L74" t="s" s="2">
-        <v>527</v>
-      </c>
-      <c r="M74" t="s" s="2">
-        <v>528</v>
-      </c>
-      <c r="N74" s="2"/>
+        <v>523</v>
+      </c>
+      <c r="M74" s="2"/>
+      <c r="N74" t="s" s="2">
+        <v>524</v>
+      </c>
       <c r="O74" t="s" s="2">
         <v>45</v>
       </c>
@@ -10672,25 +10686,25 @@
         <v>45</v>
       </c>
       <c r="AA74" t="s" s="2">
-        <v>529</v>
+        <v>45</v>
       </c>
       <c r="AB74" t="s" s="2">
-        <v>530</v>
+        <v>45</v>
       </c>
       <c r="AC74" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AD74" t="s" s="2">
-        <v>326</v>
+        <v>45</v>
       </c>
       <c r="AE74" t="s" s="2">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="AF74" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG74" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH74" t="s" s="2">
         <v>45</v>
@@ -10705,10 +10719,10 @@
         <v>45</v>
       </c>
       <c r="AL74" t="s" s="2">
-        <v>531</v>
+        <v>45</v>
       </c>
       <c r="AM74" t="s" s="2">
-        <v>532</v>
+        <v>525</v>
       </c>
       <c r="AN74" t="s" s="2">
         <v>45</v>
@@ -10719,11 +10733,9 @@
     </row>
     <row r="75" hidden="true">
       <c r="A75" t="s" s="2">
-        <v>524</v>
-      </c>
-      <c r="B75" t="s" s="2">
-        <v>533</v>
-      </c>
+        <v>526</v>
+      </c>
+      <c r="B75" s="2"/>
       <c r="C75" t="s" s="2">
         <v>45</v>
       </c>
@@ -10741,20 +10753,18 @@
         <v>45</v>
       </c>
       <c r="I75" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J75" t="s" s="2">
-        <v>534</v>
+        <v>57</v>
       </c>
       <c r="K75" t="s" s="2">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="L75" t="s" s="2">
-        <v>527</v>
-      </c>
-      <c r="M75" t="s" s="2">
         <v>528</v>
       </c>
+      <c r="M75" s="2"/>
       <c r="N75" s="2"/>
       <c r="O75" t="s" s="2">
         <v>45</v>
@@ -10803,13 +10813,13 @@
         <v>45</v>
       </c>
       <c r="AE75" t="s" s="2">
-        <v>524</v>
+        <v>526</v>
       </c>
       <c r="AF75" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG75" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH75" t="s" s="2">
         <v>45</v>
@@ -10824,10 +10834,10 @@
         <v>45</v>
       </c>
       <c r="AL75" t="s" s="2">
-        <v>531</v>
+        <v>498</v>
       </c>
       <c r="AM75" t="s" s="2">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="AN75" t="s" s="2">
         <v>45</v>
@@ -10836,13 +10846,11 @@
         <v>45</v>
       </c>
     </row>
-    <row r="76" hidden="true">
+    <row r="76">
       <c r="A76" t="s" s="2">
-        <v>524</v>
-      </c>
-      <c r="B76" t="s" s="2">
-        <v>535</v>
-      </c>
+        <v>530</v>
+      </c>
+      <c r="B76" s="2"/>
       <c r="C76" t="s" s="2">
         <v>45</v>
       </c>
@@ -10851,10 +10859,10 @@
         <v>43</v>
       </c>
       <c r="F76" t="s" s="2">
-        <v>55</v>
+        <v>290</v>
       </c>
       <c r="G76" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="H76" t="s" s="2">
         <v>45</v>
@@ -10863,16 +10871,16 @@
         <v>56</v>
       </c>
       <c r="J76" t="s" s="2">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="K76" t="s" s="2">
-        <v>526</v>
+        <v>532</v>
       </c>
       <c r="L76" t="s" s="2">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="M76" t="s" s="2">
-        <v>528</v>
+        <v>534</v>
       </c>
       <c r="N76" s="2"/>
       <c r="O76" t="s" s="2">
@@ -10922,7 +10930,7 @@
         <v>45</v>
       </c>
       <c r="AE76" t="s" s="2">
-        <v>524</v>
+        <v>530</v>
       </c>
       <c r="AF76" t="s" s="2">
         <v>43</v>
@@ -10943,10 +10951,10 @@
         <v>45</v>
       </c>
       <c r="AL76" t="s" s="2">
-        <v>531</v>
+        <v>535</v>
       </c>
       <c r="AM76" t="s" s="2">
-        <v>532</v>
+        <v>536</v>
       </c>
       <c r="AN76" t="s" s="2">
         <v>45</v>
@@ -11060,7 +11068,7 @@
         <v>45</v>
       </c>
       <c r="AL77" t="s" s="2">
-        <v>531</v>
+        <v>535</v>
       </c>
       <c r="AM77" t="s" s="2">
         <v>542</v>
@@ -11097,7 +11105,7 @@
         <v>56</v>
       </c>
       <c r="J78" t="s" s="2">
-        <v>471</v>
+        <v>477</v>
       </c>
       <c r="K78" t="s" s="2">
         <v>544</v>
@@ -11429,7 +11437,7 @@
       </c>
       <c r="B81" s="2"/>
       <c r="C81" t="s" s="2">
-        <v>482</v>
+        <v>488</v>
       </c>
       <c r="D81" s="2"/>
       <c r="E81" t="s" s="2">
@@ -11451,16 +11459,16 @@
         <v>75</v>
       </c>
       <c r="K81" t="s" s="2">
-        <v>483</v>
+        <v>489</v>
       </c>
       <c r="L81" t="s" s="2">
-        <v>484</v>
+        <v>490</v>
       </c>
       <c r="M81" t="s" s="2">
         <v>78</v>
       </c>
       <c r="N81" t="s" s="2">
-        <v>485</v>
+        <v>491</v>
       </c>
       <c r="O81" t="s" s="2">
         <v>45</v>
@@ -11509,7 +11517,7 @@
         <v>45</v>
       </c>
       <c r="AE81" t="s" s="2">
-        <v>486</v>
+        <v>492</v>
       </c>
       <c r="AF81" t="s" s="2">
         <v>43</v>
@@ -11698,7 +11706,7 @@
         <v>563</v>
       </c>
       <c r="N83" t="s" s="2">
-        <v>354</v>
+        <v>360</v>
       </c>
       <c r="O83" t="s" s="2">
         <v>45</v>
@@ -11768,16 +11776,16 @@
         <v>567</v>
       </c>
       <c r="AL83" t="s" s="2">
-        <v>357</v>
+        <v>363</v>
       </c>
       <c r="AM83" t="s" s="2">
-        <v>358</v>
+        <v>364</v>
       </c>
       <c r="AN83" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO83" t="s" s="2">
-        <v>359</v>
+        <v>365</v>
       </c>
     </row>
     <row r="84">
@@ -11817,7 +11825,7 @@
         <v>571</v>
       </c>
       <c r="N84" t="s" s="2">
-        <v>408</v>
+        <v>414</v>
       </c>
       <c r="O84" t="s" s="2">
         <v>45</v>
@@ -11845,10 +11853,10 @@
         <v>113</v>
       </c>
       <c r="X84" t="s" s="2">
-        <v>409</v>
+        <v>415</v>
       </c>
       <c r="Y84" t="s" s="2">
-        <v>410</v>
+        <v>416</v>
       </c>
       <c r="Z84" t="s" s="2">
         <v>45</v>
@@ -11890,7 +11898,7 @@
         <v>155</v>
       </c>
       <c r="AM84" t="s" s="2">
-        <v>412</v>
+        <v>418</v>
       </c>
       <c r="AN84" t="s" s="2">
         <v>45</v>
@@ -11905,7 +11913,7 @@
       </c>
       <c r="B85" s="2"/>
       <c r="C85" t="s" s="2">
-        <v>414</v>
+        <v>420</v>
       </c>
       <c r="D85" s="2"/>
       <c r="E85" t="s" s="2">
@@ -11927,16 +11935,16 @@
         <v>202</v>
       </c>
       <c r="K85" t="s" s="2">
-        <v>415</v>
+        <v>421</v>
       </c>
       <c r="L85" t="s" s="2">
-        <v>416</v>
+        <v>422</v>
       </c>
       <c r="M85" t="s" s="2">
-        <v>417</v>
+        <v>423</v>
       </c>
       <c r="N85" t="s" s="2">
-        <v>418</v>
+        <v>424</v>
       </c>
       <c r="O85" t="s" s="2">
         <v>45</v>
@@ -11964,10 +11972,10 @@
         <v>113</v>
       </c>
       <c r="X85" t="s" s="2">
-        <v>419</v>
+        <v>425</v>
       </c>
       <c r="Y85" t="s" s="2">
-        <v>420</v>
+        <v>426</v>
       </c>
       <c r="Z85" t="s" s="2">
         <v>45</v>
@@ -12003,19 +12011,19 @@
         <v>45</v>
       </c>
       <c r="AK85" t="s" s="2">
-        <v>421</v>
+        <v>427</v>
       </c>
       <c r="AL85" t="s" s="2">
-        <v>422</v>
+        <v>428</v>
       </c>
       <c r="AM85" t="s" s="2">
-        <v>423</v>
+        <v>429</v>
       </c>
       <c r="AN85" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO85" t="s" s="2">
-        <v>424</v>
+        <v>430</v>
       </c>
     </row>
     <row r="86" hidden="true">
@@ -12052,10 +12060,10 @@
         <v>576</v>
       </c>
       <c r="M86" t="s" s="2">
-        <v>474</v>
+        <v>480</v>
       </c>
       <c r="N86" t="s" s="2">
-        <v>475</v>
+        <v>481</v>
       </c>
       <c r="O86" t="s" s="2">
         <v>45</v>
@@ -12125,10 +12133,10 @@
         <v>45</v>
       </c>
       <c r="AL86" t="s" s="2">
-        <v>477</v>
+        <v>483</v>
       </c>
       <c r="AM86" t="s" s="2">
-        <v>478</v>
+        <v>484</v>
       </c>
       <c r="AN86" t="s" s="2">
         <v>45</v>

</xml_diff>